<commit_message>
Retrieved pps lightcurves and spectra for alert sources where available.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="14">
   <si>
     <t xml:space="preserve">Source number</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPS</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
@@ -184,14 +187,14 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D86" activeCellId="0" sqref="D86"/>
+      <selection pane="bottomLeft" activeCell="H85" activeCellId="0" sqref="H85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.27"/>
@@ -246,6 +249,12 @@
       <c r="D2" s="0" t="n">
         <v>2.58</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -257,6 +266,12 @@
       <c r="D3" s="0" t="n">
         <v>2.46</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -268,13 +283,19 @@
       <c r="D4" s="0" t="n">
         <v>0.899</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1.6</v>
@@ -290,13 +311,19 @@
       <c r="D6" s="0" t="n">
         <v>4.57</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2.08</v>
@@ -304,10 +331,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2.35</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,7 +348,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.275</v>
@@ -331,6 +364,12 @@
       <c r="D10" s="0" t="n">
         <v>4.12</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -342,6 +381,12 @@
       <c r="D11" s="0" t="n">
         <v>1.85</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -352,6 +397,12 @@
       </c>
       <c r="D12" s="0" t="n">
         <v>1.54</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,10 +437,16 @@
         <v>12</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2.2</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,10 +454,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.431</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,10 +471,16 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>2.59</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,10 +488,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1.18</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,10 +505,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1.3</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,10 +522,16 @@
         <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1.45</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,10 +539,16 @@
         <v>18</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.833</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +556,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.714</v>
@@ -479,13 +572,19 @@
       <c r="D24" s="3" t="n">
         <v>1.43</v>
       </c>
+      <c r="F24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>21</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1.3</v>
@@ -493,10 +592,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0.395</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,7 +609,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>1.37</v>
@@ -515,10 +620,16 @@
         <v>23</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0.913</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,10 +637,16 @@
         <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>3.63</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +654,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0.0511</v>
@@ -548,23 +665,35 @@
         <v>26</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>3.31</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="0" t="n">
         <v>3.14</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>27</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>6.6</v>
@@ -575,10 +704,16 @@
         <v>28</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1.95</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +721,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>1.45</v>
@@ -597,10 +732,16 @@
         <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>0.98</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,10 +749,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0.182</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,7 +766,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>3.35</v>
@@ -630,10 +777,16 @@
         <v>33</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0.588</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +794,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0.193</v>
@@ -652,7 +805,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2.86</v>
@@ -663,7 +816,7 @@
         <v>36</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0.935</v>
@@ -707,10 +860,16 @@
         <v>40</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D46" s="3" t="n">
         <v>97</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,6 +882,12 @@
       <c r="D47" s="0" t="n">
         <v>2.82</v>
       </c>
+      <c r="F47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -745,6 +910,12 @@
       <c r="D49" s="0" t="n">
         <v>2.95</v>
       </c>
+      <c r="F49" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -762,10 +933,16 @@
         <v>45</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>7.22</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,10 +961,16 @@
         <v>47</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>0.294</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,10 +989,16 @@
         <v>49</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>37.2</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="56" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,6 +1011,12 @@
       <c r="D56" s="3" t="n">
         <v>2.93</v>
       </c>
+      <c r="F56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -839,10 +1034,16 @@
         <v>52</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0.504</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,10 +1051,16 @@
         <v>53</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>23.8</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,7 +1079,7 @@
         <v>55</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>0.649</v>
@@ -888,6 +1095,12 @@
       <c r="D62" s="0" t="n">
         <v>2.95</v>
       </c>
+      <c r="F62" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -905,31 +1118,55 @@
         <v>58</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>16.8</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D65" s="0" t="n">
         <v>17.3</v>
       </c>
+      <c r="F65" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D66" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="F66" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>59</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>9.76</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="68" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,7 +1174,7 @@
         <v>60</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D68" s="3" t="n">
         <v>2.43</v>
@@ -948,10 +1185,16 @@
         <v>61</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>28.4</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,10 +1202,16 @@
         <v>62</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>3.09</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,26 +1219,44 @@
         <v>63</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>1.42</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D72" s="0" t="n">
         <v>1.43</v>
       </c>
+      <c r="F72" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>64</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>55.4</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,10 +1264,16 @@
         <v>65</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>4.13</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,6 +1286,12 @@
       <c r="D75" s="0" t="n">
         <v>3.44</v>
       </c>
+      <c r="F75" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -1030,10 +1309,16 @@
         <v>68</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>3.08</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,10 +1337,16 @@
         <v>70</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D79" s="3" t="n">
         <v>1.32</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,6 +1359,12 @@
       <c r="D80" s="0" t="n">
         <v>3.76</v>
       </c>
+      <c r="F80" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
@@ -1079,13 +1376,19 @@
       <c r="D81" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="F81" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>73</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>4.17</v>
@@ -1101,13 +1404,19 @@
       <c r="D83" s="0" t="n">
         <v>8.22</v>
       </c>
+      <c r="F83" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>75</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>2.07</v>
@@ -1118,10 +1427,16 @@
         <v>76</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>2.55</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for completion og lightcurve processing for all real alerts.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$L$85</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="24">
   <si>
     <t xml:space="preserve">Source number</t>
   </si>
@@ -55,13 +58,43 @@
     <t xml:space="preserve">PPS</t>
   </si>
   <si>
+    <t xml:space="preserve">PPS?</t>
+  </si>
+  <si>
     <t xml:space="preserve">H</t>
   </si>
   <si>
+    <t xml:space="preserve">Reproc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pending group</t>
+  </si>
+  <si>
     <t xml:space="preserve">L</t>
   </si>
   <si>
+    <t xml:space="preserve">See comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source location in PN image is affected by chip gap. Source too faint to appear on MOS images.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE ALERT – REMOVE</t>
+  </si>
+  <si>
     <t xml:space="preserve">PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentially part of reflection ring. Hard to conclude with certainty.</t>
   </si>
 </sst>
 </file>
@@ -179,6 +212,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -187,12 +224,12 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H85" activeCellId="0" sqref="H85"/>
+      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.1"/>
@@ -253,7 +290,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +307,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,7 +324,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -295,10 +332,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1.6</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,7 +358,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,15 +366,24 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2.08</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6.1</v>
+      </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2.35</v>
@@ -340,7 +392,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,10 +400,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.275</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -368,7 +426,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -385,7 +443,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,24 +460,42 @@
         <v>10</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>10.1</v>
+      </c>
       <c r="C13" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>5.02</v>
       </c>
+      <c r="F13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>10.2</v>
+      </c>
       <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>3.03</v>
       </c>
+      <c r="F14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -431,13 +507,16 @@
       <c r="D15" s="0" t="n">
         <v>1.5</v>
       </c>
+      <c r="F15" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2.2</v>
@@ -446,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,7 +533,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.431</v>
@@ -463,7 +542,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,7 +550,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>2.59</v>
@@ -480,7 +559,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +567,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1.18</v>
@@ -497,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +584,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1.3</v>
@@ -514,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,7 +601,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1.45</v>
@@ -531,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,7 +618,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.833</v>
@@ -548,7 +627,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,10 +635,19 @@
         <v>19</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.714</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,8 +663,8 @@
       <c r="F24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
+      <c r="G24" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,15 +672,24 @@
         <v>21</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>1.3</v>
       </c>
+      <c r="F25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>21.1</v>
+      </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>0.395</v>
@@ -601,7 +698,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,10 +706,19 @@
         <v>22</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>1.37</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,7 +726,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>0.913</v>
@@ -629,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,7 +743,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>3.63</v>
@@ -646,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,10 +760,19 @@
         <v>25</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>0.0511</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,7 +780,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>3.31</v>
@@ -674,10 +789,16 @@
         <v>10</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>12</v>
+      </c>
       <c r="D32" s="0" t="n">
         <v>3.14</v>
       </c>
@@ -685,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,10 +814,16 @@
         <v>27</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>6.6</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,7 +831,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1.95</v>
@@ -713,7 +840,7 @@
         <v>10</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,10 +848,19 @@
         <v>29</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>1.45</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +868,7 @@
         <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>0.98</v>
@@ -740,8 +876,8 @@
       <c r="F36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>10</v>
+      <c r="G36" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,7 +885,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>0.182</v>
@@ -758,7 +894,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,10 +902,16 @@
         <v>32</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>3.35</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,7 +919,7 @@
         <v>33</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0.588</v>
@@ -786,7 +928,7 @@
         <v>10</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,10 +936,16 @@
         <v>34</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>0.193</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,10 +953,16 @@
         <v>35</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2.86</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,10 +970,16 @@
         <v>36</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>0.935</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,6 +992,9 @@
       <c r="D43" s="0" t="n">
         <v>4.12</v>
       </c>
+      <c r="F43" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -843,6 +1006,9 @@
       <c r="D44" s="0" t="n">
         <v>1.15</v>
       </c>
+      <c r="F44" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -854,13 +1020,19 @@
       <c r="D45" s="0" t="n">
         <v>1.69</v>
       </c>
+      <c r="F45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="n">
         <v>40</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" s="3" t="n">
         <v>97</v>
@@ -868,8 +1040,8 @@
       <c r="F46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>10</v>
+      <c r="G46" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,6 +1071,9 @@
       <c r="D48" s="0" t="n">
         <v>6.11</v>
       </c>
+      <c r="F48" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -914,7 +1089,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,13 +1102,22 @@
       <c r="D50" s="0" t="n">
         <v>4.99</v>
       </c>
+      <c r="F50" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>45</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>7.22</v>
@@ -942,7 +1126,7 @@
         <v>10</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,13 +1139,19 @@
       <c r="D52" s="0" t="n">
         <v>2.48</v>
       </c>
+      <c r="F52" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>47</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>0.294</v>
@@ -970,7 +1160,7 @@
         <v>10</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,13 +1173,19 @@
       <c r="D54" s="0" t="n">
         <v>0.102</v>
       </c>
+      <c r="F54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>49</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>37.2</v>
@@ -998,7 +1194,7 @@
         <v>10</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,8 +1210,8 @@
       <c r="F56" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>10</v>
+      <c r="G56" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,13 +1224,16 @@
       <c r="D57" s="0" t="n">
         <v>0.95</v>
       </c>
+      <c r="F57" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>52</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>0.504</v>
@@ -1043,7 +1242,7 @@
         <v>10</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,7 +1250,7 @@
         <v>53</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>23.8</v>
@@ -1060,7 +1259,7 @@
         <v>10</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,16 +1272,28 @@
       <c r="D60" s="0" t="n">
         <v>16.1</v>
       </c>
+      <c r="F60" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>55</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>0.649</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,13 +1323,16 @@
       <c r="D63" s="0" t="n">
         <v>1.54</v>
       </c>
+      <c r="F63" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>58</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>16.8</v>
@@ -1127,10 +1341,16 @@
         <v>10</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="D65" s="0" t="n">
         <v>17.3</v>
       </c>
@@ -1138,10 +1358,16 @@
         <v>10</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="D66" s="0" t="n">
         <v>24</v>
       </c>
@@ -1149,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1157,7 +1383,7 @@
         <v>59</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>9.76</v>
@@ -1166,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,10 +1400,16 @@
         <v>60</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D68" s="3" t="n">
         <v>2.43</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,7 +1417,7 @@
         <v>61</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>28.4</v>
@@ -1194,7 +1426,7 @@
         <v>10</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1434,7 @@
         <v>62</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>3.09</v>
@@ -1211,7 +1443,7 @@
         <v>10</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,7 +1451,7 @@
         <v>63</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>1.42</v>
@@ -1228,10 +1460,16 @@
         <v>10</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="D72" s="0" t="n">
         <v>1.43</v>
       </c>
@@ -1239,7 +1477,7 @@
         <v>10</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1485,7 @@
         <v>64</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>55.4</v>
@@ -1256,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,7 +1502,7 @@
         <v>65</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>4.13</v>
@@ -1273,7 +1511,7 @@
         <v>10</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,7 +1528,7 @@
         <v>10</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,13 +1541,19 @@
       <c r="D76" s="0" t="n">
         <v>2.76</v>
       </c>
+      <c r="F76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>68</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>3.08</v>
@@ -1318,7 +1562,7 @@
         <v>10</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,13 +1575,19 @@
       <c r="D78" s="0" t="n">
         <v>2.45</v>
       </c>
+      <c r="F78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="79" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="n">
         <v>70</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D79" s="3" t="n">
         <v>1.32</v>
@@ -1345,8 +1595,8 @@
       <c r="F79" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>10</v>
+      <c r="G79" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,7 +1613,7 @@
         <v>10</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1630,7 @@
         <v>10</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,10 +1638,16 @@
         <v>73</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>4.17</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,7 +1664,7 @@
         <v>10</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,10 +1672,19 @@
         <v>75</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>2.07</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L84" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1692,7 @@
         <v>76</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>2.55</v>
@@ -1436,10 +1701,23 @@
         <v>10</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L85"/>
+  <conditionalFormatting sqref="D2:D85">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1447,5 +1725,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sources for five additional false alerts.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$L$85</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$L$80</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="23">
   <si>
     <t xml:space="preserve">Source number</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Source location in PN image is affected by chip gap. Source too faint to appear on MOS images.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE ALERT – REMOVE</t>
   </si>
   <si>
     <t xml:space="preserve">PV</t>
@@ -183,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -197,6 +194,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,15 +222,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.1"/>
@@ -502,13 +503,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1.5</v>
+        <v>2.2</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,10 +520,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>2.2</v>
+        <v>0.431</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>10</v>
@@ -533,10 +537,10 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.431</v>
+        <v>2.59</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>10</v>
@@ -550,10 +554,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>2.59</v>
+        <v>1.18</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>10</v>
@@ -567,10 +571,10 @@
         <v>15</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>1.18</v>
+        <v>1.3</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>10</v>
@@ -587,7 +591,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>1.3</v>
+        <v>1.45</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>10</v>
@@ -601,10 +605,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1.45</v>
+        <v>0.833</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>10</v>
@@ -618,87 +622,90 @@
         <v>18</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.714</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>0.833</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+    </row>
+    <row r="23" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>0.714</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>13</v>
+      <c r="C23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>10</v>
+      <c r="C24" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>14</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0.395</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>21.1</v>
+        <v>21</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.395</v>
+        <v>1.37</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,16 +716,13 @@
         <v>12</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1.37</v>
+        <v>0.913</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,7 +733,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>0.913</v>
+        <v>3.63</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>10</v>
@@ -743,16 +747,19 @@
         <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>3.63</v>
+        <v>0.0511</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,30 +767,27 @@
         <v>25</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.0511</v>
+        <v>3.31</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>26</v>
+        <v>25.1</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>3.31</v>
+        <v>3.14</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>10</v>
@@ -794,19 +798,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>26.1</v>
+        <v>26</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>3.14</v>
+        <v>6.6</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,13 +821,13 @@
         <v>12</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>6.6</v>
+        <v>1.95</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,33 +838,33 @@
         <v>12</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>1.95</v>
+        <v>1.45</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>1.45</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>13</v>
+      <c r="C35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="4" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,12 +875,12 @@
         <v>15</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>0.98</v>
+        <v>0.182</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="G36" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -885,16 +889,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.182</v>
+        <v>3.35</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,16 +906,16 @@
         <v>32</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>3.35</v>
+        <v>0.588</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,16 +923,16 @@
         <v>33</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>0.588</v>
+        <v>0.193</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,10 +940,10 @@
         <v>34</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>0.193</v>
+        <v>2.86</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>13</v>
@@ -956,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>2.86</v>
+        <v>0.935</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>13</v>
@@ -970,16 +974,13 @@
         <v>36</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>0.935</v>
+        <v>1.15</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,24 +991,30 @@
         <v>9</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>4.12</v>
+        <v>1.69</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>13</v>
+      <c r="C44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="4" t="n">
+        <v>97</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,13 +1025,13 @@
         <v>9</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>1.69</v>
+        <v>2.82</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,15 +1039,15 @@
         <v>40</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>97</v>
+        <v>2.95</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="G46" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1052,13 +1059,16 @@
         <v>9</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>2.82</v>
+        <v>4.99</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="L47" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,13 +1076,16 @@
         <v>42</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>6.11</v>
+        <v>7.22</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,13 +1096,13 @@
         <v>9</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>2.95</v>
+        <v>2.48</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,19 +1110,16 @@
         <v>44</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>4.99</v>
+        <v>0.294</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L50" s="0" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,16 +1127,16 @@
         <v>45</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>7.22</v>
+        <v>0.102</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,29 +1144,29 @@
         <v>46</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>2.48</v>
+        <v>37.2</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="n">
         <v>47</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>0.294</v>
-      </c>
-      <c r="F53" s="0" t="s">
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="4" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G53" s="0" t="s">
@@ -1168,16 +1178,16 @@
         <v>48</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>0.102</v>
+        <v>0.504</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,10 +1195,10 @@
         <v>49</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>37.2</v>
+        <v>23.8</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>10</v>
@@ -1205,13 +1215,13 @@
         <v>9</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>2.93</v>
+        <v>16.1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,13 +1229,16 @@
         <v>51</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>0.95</v>
+        <v>0.649</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,10 +1246,10 @@
         <v>52</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>0.504</v>
+        <v>2.95</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>10</v>
@@ -1250,10 +1263,10 @@
         <v>53</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>23.8</v>
+        <v>16.8</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>10</v>
@@ -1264,47 +1277,47 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>54</v>
+        <v>53.1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>16.1</v>
+        <v>17.3</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>55</v>
+        <v>53.2</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>0.649</v>
+        <v>24</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>2.95</v>
+        <v>9.76</v>
       </c>
       <c r="F62" s="0" t="s">
         <v>10</v>
@@ -1313,29 +1326,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="0" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>18</v>
+    <row r="63" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="n">
+        <v>55</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="4" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>16.8</v>
+        <v>28.4</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>10</v>
@@ -1346,13 +1362,13 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>58.1</v>
+        <v>57</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>17.3</v>
+        <v>3.09</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>10</v>
@@ -1363,13 +1379,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>58.2</v>
+        <v>58</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>24</v>
+        <v>1.42</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>10</v>
@@ -1380,64 +1396,64 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="0" t="n">
-        <v>9.76</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="n">
+      <c r="C68" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>55.4</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="3" t="n">
-        <v>2.43</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="0" t="n">
-        <v>28.4</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G69" s="0" t="s">
+      <c r="C69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>3.09</v>
+        <v>3.44</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>10</v>
@@ -1448,30 +1464,30 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>1.42</v>
+        <v>2.76</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>63.1</v>
+        <v>63</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>1.43</v>
+        <v>3.08</v>
       </c>
       <c r="F72" s="0" t="s">
         <v>10</v>
@@ -1485,29 +1501,29 @@
         <v>64</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>55.4</v>
+        <v>2.45</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="4" t="n">
         <v>65</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D74" s="0" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="F74" s="0" t="s">
+      <c r="D74" s="4" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G74" s="0" t="s">
@@ -1522,7 +1538,7 @@
         <v>9</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>3.44</v>
+        <v>3.76</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>10</v>
@@ -1539,13 +1555,13 @@
         <v>9</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>2.76</v>
+        <v>2</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,16 +1569,16 @@
         <v>68</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>3.08</v>
+        <v>4.17</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,30 +1589,33 @@
         <v>9</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>2.45</v>
+        <v>8.22</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" s="3" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>10</v>
+      <c r="C79" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="L79" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,10 +1623,10 @@
         <v>71</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>3.76</v>
+        <v>2.55</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>10</v>
@@ -1616,97 +1635,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G81" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
-        <v>73</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" s="0" t="n">
-        <v>4.17</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
-        <v>74</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>8.22</v>
-      </c>
-      <c r="F83" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G83" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="n">
-        <v>75</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>2.07</v>
-      </c>
-      <c r="F84" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L84" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
-        <v>76</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="F85" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G85" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L85"/>
-  <conditionalFormatting sqref="D2:D85">
+  <autoFilter ref="A1:L80"/>
+  <conditionalFormatting sqref="D2:D80">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
Updated for all new reprocessed lightcurves not available through PPS.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="23">
   <si>
     <t xml:space="preserve">Source number</t>
   </si>
@@ -225,12 +225,12 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
+      <selection pane="bottomLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.1"/>
@@ -980,6 +980,9 @@
         <v>1.15</v>
       </c>
       <c r="F42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="0" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reprocessed spectra for alerts not in PPS.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="22">
   <si>
     <t xml:space="preserve">Source number</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">Reproc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pending group</t>
   </si>
   <si>
     <t xml:space="preserve">L</t>
@@ -225,12 +222,12 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.1"/>
@@ -342,7 +339,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,7 +373,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,16 +398,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.275</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +475,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +492,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,7 +517,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.431</v>
@@ -554,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1.18</v>
@@ -605,7 +602,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0.833</v>
@@ -622,7 +619,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.714</v>
@@ -631,10 +628,10 @@
         <v>13</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,7 +656,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1.3</v>
@@ -668,7 +665,7 @@
         <v>13</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +673,7 @@
         <v>20.1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>0.395</v>
@@ -702,10 +699,10 @@
         <v>13</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,7 +744,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0.0511</v>
@@ -756,10 +753,10 @@
         <v>13</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +807,7 @@
         <v>13</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,10 +841,10 @@
         <v>13</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,7 +852,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>0.98</v>
@@ -872,7 +869,7 @@
         <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>0.182</v>
@@ -889,7 +886,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>3.35</v>
@@ -898,7 +895,7 @@
         <v>13</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,7 +903,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0.588</v>
@@ -923,7 +920,7 @@
         <v>33</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0.193</v>
@@ -932,7 +929,7 @@
         <v>13</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,7 +946,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,7 +963,7 @@
         <v>13</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,10 +1065,10 @@
         <v>13</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1102,7 @@
         <v>13</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,7 +1110,7 @@
         <v>44</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>0.294</v>
@@ -1181,7 +1178,7 @@
         <v>48</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>0.504</v>
@@ -1198,7 +1195,7 @@
         <v>49</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>23.8</v>
@@ -1224,7 +1221,7 @@
         <v>13</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,7 +1263,7 @@
         <v>53</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>16.8</v>
@@ -1283,7 +1280,7 @@
         <v>53.1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>17.3</v>
@@ -1300,7 +1297,7 @@
         <v>53.2</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>24</v>
@@ -1385,7 +1382,7 @@
         <v>58</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>1.42</v>
@@ -1402,7 +1399,7 @@
         <v>58.1</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>1.43</v>
@@ -1436,7 +1433,7 @@
         <v>60</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D69" s="3" t="n">
         <v>4.13</v>
@@ -1521,7 +1518,7 @@
         <v>65</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74" s="4" t="n">
         <v>1.32</v>
@@ -1572,7 +1569,7 @@
         <v>68</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>4.17</v>
@@ -1615,10 +1612,10 @@
         <v>13</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L79" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated for final false alert in obs. Added basic spectral fitting routines.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$L$80</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$L$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="20">
   <si>
     <t xml:space="preserve">Source number</t>
   </si>
@@ -58,9 +58,6 @@
     <t xml:space="preserve">PPS</t>
   </si>
   <si>
-    <t xml:space="preserve">PPS?</t>
-  </si>
-  <si>
     <t xml:space="preserve">H</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potentially part of reflection ring. Hard to conclude with certainty.</t>
   </si>
 </sst>
 </file>
@@ -177,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,6 +189,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,15 +217,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
+      <selection pane="bottomLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.1"/>
@@ -288,7 +286,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,7 +303,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,7 +320,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,16 +328,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1.6</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +354,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,16 +362,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>2.08</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,7 +379,7 @@
         <v>6.1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2.35</v>
@@ -390,7 +388,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,16 +396,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.275</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +422,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,7 +439,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,7 +456,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,10 +470,10 @@
         <v>5.02</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,10 +487,10 @@
         <v>3.03</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,7 +498,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2.2</v>
@@ -509,7 +507,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +515,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.431</v>
@@ -526,7 +524,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,7 +532,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>2.59</v>
@@ -543,7 +541,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1.18</v>
@@ -560,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +566,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1.3</v>
@@ -577,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -585,7 +583,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1.45</v>
@@ -594,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -602,7 +600,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0.833</v>
@@ -611,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,19 +617,19 @@
         <v>18</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.714</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,16 +654,16 @@
         <v>20</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>1.3</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,7 +671,7 @@
         <v>20.1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>0.395</v>
@@ -681,8 +679,8 @@
       <c r="F25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>11</v>
+      <c r="G25" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,19 +688,19 @@
         <v>21</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>1.37</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,7 +708,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>0.913</v>
@@ -719,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,7 +725,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>3.63</v>
@@ -736,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,19 +742,19 @@
         <v>24</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0.0511</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -764,7 +762,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>3.31</v>
@@ -773,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,7 +779,7 @@
         <v>25.1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>3.14</v>
@@ -790,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,16 +796,16 @@
         <v>26</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>6.6</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +813,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>1.95</v>
@@ -824,7 +822,7 @@
         <v>10</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,19 +830,19 @@
         <v>28</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>1.45</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,7 +850,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>0.98</v>
@@ -861,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,7 +867,7 @@
         <v>30</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" s="3" t="n">
         <v>0.182</v>
@@ -877,8 +875,8 @@
       <c r="F36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>11</v>
+      <c r="G36" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,16 +884,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>3.35</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +901,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>0.588</v>
@@ -912,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,16 +918,16 @@
         <v>33</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>0.193</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,16 +935,16 @@
         <v>34</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>2.86</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,16 +952,16 @@
         <v>35</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>0.935</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,10 +975,10 @@
         <v>1.15</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,10 +992,10 @@
         <v>1.69</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +1003,7 @@
         <v>38</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44" s="4" t="n">
         <v>97</v>
@@ -1014,7 +1012,7 @@
         <v>10</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,7 +1029,7 @@
         <v>10</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,8 +1045,8 @@
       <c r="F46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>11</v>
+      <c r="G46" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,19 +1054,16 @@
         <v>41</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>4.99</v>
+        <v>7.22</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="L47" s="0" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,16 +1071,16 @@
         <v>42</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>7.22</v>
+        <v>2.48</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,16 +1088,16 @@
         <v>43</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D49" s="0" t="n">
-        <v>2.48</v>
+        <v>0.294</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,16 +1105,16 @@
         <v>44</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>0.294</v>
+        <v>0.102</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,50 +1122,50 @@
         <v>45</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>0.102</v>
+        <v>37.2</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="n">
         <v>46</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>37.2</v>
-      </c>
-      <c r="F52" s="0" t="s">
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="4" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="4" t="n">
-        <v>2.93</v>
-      </c>
-      <c r="F53" s="4" t="s">
+      <c r="C53" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="F53" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,33 +1173,33 @@
         <v>48</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>0.504</v>
+        <v>23.8</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="0" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="0" t="s">
-        <v>11</v>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="4" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="56" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,16 +1207,16 @@
         <v>50</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>16.1</v>
+        <v>0.649</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,16 +1224,16 @@
         <v>51</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>0.649</v>
+        <v>2.95</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,101 +1241,101 @@
         <v>52</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>2.95</v>
+        <v>16.8</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>53</v>
+        <v>52.1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>16.8</v>
+        <v>17.3</v>
       </c>
       <c r="F59" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>53.1</v>
+        <v>52.2</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>17.3</v>
+        <v>24</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>53.2</v>
+        <v>53</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>24</v>
+        <v>9.76</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="n">
         <v>54</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <v>9.76</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="n">
+      <c r="C62" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="4" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D63" s="4" t="n">
-        <v>2.43</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>13</v>
+      <c r="C63" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,16 +1343,16 @@
         <v>56</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>28.4</v>
+        <v>3.09</v>
       </c>
       <c r="F64" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,67 +1360,67 @@
         <v>57</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>3.09</v>
+        <v>1.42</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>58</v>
+        <v>57.1</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="F66" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>58.1</v>
+        <v>58</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>1.43</v>
+        <v>55.4</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="4" t="n">
         <v>59</v>
       </c>
-      <c r="C68" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="0" t="n">
-        <v>55.4</v>
-      </c>
-      <c r="F68" s="0" t="s">
+      <c r="C68" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="4" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,16 +1428,16 @@
         <v>60</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>4.13</v>
+        <v>3.44</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>11</v>
+      <c r="G69" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,13 +1448,13 @@
         <v>9</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>3.44</v>
+        <v>2.76</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,16 +1462,16 @@
         <v>62</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>2.76</v>
+        <v>3.08</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,50 +1479,50 @@
         <v>63</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>3.08</v>
+        <v>2.45</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="4" t="n">
         <v>64</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="F73" s="0" t="s">
+      <c r="C73" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D73" s="4" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G73" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="4" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="F74" s="4" t="s">
+      <c r="C74" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="F74" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,13 +1533,13 @@
         <v>9</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>3.76</v>
+        <v>2</v>
       </c>
       <c r="F75" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,16 +1547,16 @@
         <v>67</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>2</v>
+        <v>4.17</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,16 +1564,16 @@
         <v>68</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>4.17</v>
+        <v>8.22</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,16 +1581,19 @@
         <v>69</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>8.22</v>
+        <v>2.07</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="L78" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,41 +1601,21 @@
         <v>70</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>2.07</v>
+        <v>2.55</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="L79" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
-        <v>71</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D80" s="0" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L80"/>
-  <conditionalFormatting sqref="D2:D80">
+  <autoFilter ref="A1:L79"/>
+  <conditionalFormatting sqref="D2:D79">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
Update for first pass through at identifying GP alert sources.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="103">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -65,7 +65,25 @@
     <t xml:space="preserve">PPS</t>
   </si>
   <si>
-    <t xml:space="preserve">No Opt/IR conterpart wihtin 10+ sigma. SIMBAD association with star?</t>
+    <t xml:space="preserve">SIMBAD association to 2MASS source for variable star. Nearer GAIA association to unknown object. Best fit spectrum is for bremsstrahlung kT = 2.8keV although poor quality. No distance estimate, Lx at 8kpc is 1.1e33 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check periodicity in lightcurve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Opt/IR conterpart wihtin 10+ sigma. SIMBAD association with star at approx 12sig. Best fit spectrum is bbody with kT = 1.2keV, Lx at 8kpc 9.4e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for periodicity in lightcurve.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia/2MASS association within 4”. Best fit spectrum is apec with kT = 43keV. At distance of GAIA source would have Lx 6.5e30 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ariadne fit to confirm GAIA/2M is star.</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
@@ -74,7 +92,16 @@
     <t xml:space="preserve">Reproc</t>
   </si>
   <si>
-    <t xml:space="preserve">No Opt/IR conterpart wihtin 5+ sigma</t>
+    <t xml:space="preserve">SIMBAD association to X-ray source at 6”. No good GAIA/2MASS within 3”. Best fit spectrum is powerlaw with index 1.4. Lx at 8kpc would be 8.9e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for periodicity at higher energies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No good GAIA/2MASS sources within 4sig+. Significant variability in hard band. Best fit spectrum is for bbody with kT=0.29keV and high nH with an additional emission line at 6.7keV. Lx at 8kpc is 4.3e33 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Opt/IR conterpart wihtin 5+ sigma. No distinguishing features in lcs. Spectra for both obs best fit by powerlaw although poor quality of spectra. Photon indices are 0.8 and -0.4. Lx at 9kpc would be 1.1e33 and 2.7e33 erg/s.</t>
   </si>
   <si>
     <t xml:space="preserve">L</t>
@@ -89,28 +116,46 @@
     <t xml:space="preserve">Source location in PN image is affected by chip gap. Source too faint to appear on MOS images.</t>
   </si>
   <si>
+    <t xml:space="preserve">No further actions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by powerlaw index 1.1 with Lx at 8kpc 2.1e33 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARIADNE fit to confirm if star. Check for pulsation in lc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia source within 2sig. No distinguishing features in lightcurves. Spectra best fit by apec (x2 for 10, and x1 for 10.2) and bbody for alert 10.1. kT are 0.04 and 5.4keV, 1.21keV and 1.4keV respectively. Lx at GAIA source dist 1.3, 3.3 and 2.1e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARIADNE fit for GAIA source to confirm it is star.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Star</t>
   </si>
   <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ariadne fit to confirm GAIA/2M is star.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Star?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s.</t>
   </si>
   <si>
     <t xml:space="preserve">PV</t>
   </si>
   <si>
-    <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source?</t>
+    <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source? No clear features in lightcurve. Best fit spectrum is powerlaw index 1.0. Lx at 8kpc is 9.8e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is for power law, or powerlaw with emission line at 6.4keV. Both power laws have index 1.34. Lack of good distance estimate means no luminosity, but flux estimate is 2e-12 erg/s/cm2</t>
   </si>
   <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s.</t>
@@ -128,23 +173,7 @@
     <t xml:space="preserve">Search for periodicity?</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Far softer in second observation. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s.</t>
-    </r>
+    <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s.</t>
   </si>
   <si>
     <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead.</t>
@@ -223,6 +252,87 @@
   </si>
   <si>
     <t xml:space="preserve">Power law with iron line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWIFT XRB association.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ariadne fit to confirm GAIA/2M is star. Check for periodicity in low energy lc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strong 2MASS association but no GAIA, and no visible optical source. SIMBAD association IRAS 1747-2648 at 4”. Best fit spec (albeit poor quality) is for power law and bbody with index -1.5, kT 0.78keV and emission line at 6.7keV. Lx at 8kpc is 3.6e33 erg/s. Very variable hard energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAIA/2MASS/AllWISE source within 1sig. SIMBAD association to SWIFt source at 6”. Poor spectra (MOS only) and best fit is for power law with index 3.6. Lx at distance to optical source is 1.8e31 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No GAIA/2MASS/AllWISE source within 12sig. Best fit spectrum is for bbody kT = 1.1keV. No distance estimate, but Lx 3.6e33 erg/s at 8kpc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Little information in lightcurve. Spectrum is low quality and best fits are apec and power law with kT = 5.9keV, or index of 1.5. No distance estimate, but at galactic centre Lx 1.4e33 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash fit to spectrum?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 10sig. Lightcurve shows potentially three peaks with periods of quiescence in between. Spectrum is best fit by blackbody with kT 0.9keV. No distance estimate, but at 8kpc Lx 1.2e33 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential for proposal to follow-up on order 25ks. Combine PN and M2 data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2mass sources within 5sig. Lightcurve shows little variability. Spectrum best fit by powerlaw with index 0.9. No distance estimate, but Lx at 8kpc is 3.0e33 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try and combine MOS2 data with PN particularly for spectrum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Gaia/2mass association with nearby star. Best fit spectrum is for either double or single apec model, with kT1 = 1keV and kT2 =4.0keV. Lx at location of star is 1.2e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARIADNE fit to confirm star.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association within 2sig to Gaia/sMASS source. Lightcurve shows not outstanding features. Best fit spectrum is for apec with kT 3.3keV. Lx at opt/IR source distance is 4.3e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for periodicitty in lc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMBAD association with 2MASS for YSO. LC shows one strong flare towards end of obs, but many bad time ints before. Best fit spec is for powerlaw with index 1.4. No distance estimate, but Lx at 8kpc is 2.9e33 erg/s. Not detected in two recent XMM obs. Check flare size/duration against YSOs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check flare against YSO/star.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Gaia/2MASS source association. Best fit spectrum is bbody with kT 1.3keV and Lx at Gaia source of 2.6e32 erg/s. No distinguishing features in lc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No GAIA/2MASS source within 6sig. Small, but fast variability in lc at higher energy. Best fit spectrum is bbody kT = 0.38keV with an iron line at 6.4keV. Lx at 8kpc would be 1.4e33 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for periodcity in lc. How else to confirm CV?</t>
   </si>
 </sst>
 </file>
@@ -232,7 +342,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -253,11 +363,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -345,11 +450,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,10 +476,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -477,25 +582,25 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L61" activeCellId="0" sqref="L61"/>
+      <selection pane="bottomLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="98.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="11.72"/>
@@ -539,7 +644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -555,10 +660,14 @@
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -575,11 +684,13 @@
         <v>12</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -595,29 +706,40 @@
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1.6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -633,27 +755,29 @@
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2.08</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -662,7 +786,7 @@
         <v>6.1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2.35</v>
@@ -681,23 +805,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.275</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -713,11 +839,13 @@
       <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -732,11 +860,18 @@
       <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="L11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -751,11 +886,18 @@
       <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="L12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="5" t="n">
         <v>10.1</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -765,39 +907,45 @@
         <v>5.02</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>10.2</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="6" t="n">
+      <c r="C14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7" t="n">
         <v>3.03</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>2.2</v>
@@ -809,13 +957,13 @@
         <v>12</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +971,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0.431</v>
@@ -835,13 +983,13 @@
         <v>12</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>2.59</v>
@@ -861,21 +1009,21 @@
         <v>12</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1.18</v>
@@ -886,15 +1034,22 @@
       <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1.3</v>
@@ -906,16 +1061,16 @@
         <v>12</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1.45</v>
@@ -926,7 +1081,9 @@
       <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0.833</v>
@@ -946,13 +1103,13 @@
         <v>12</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,112 +1117,112 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0.714</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="n">
+    <row r="23" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="8" t="n">
+      <c r="C23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="9" t="n">
         <v>1.43</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1.3</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
         <v>20.1</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="6" t="n">
+      <c r="C25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="7" t="n">
         <v>0.395</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>12</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1.37</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="N26" s="4"/>
     </row>
@@ -1074,7 +1231,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0.913</v>
@@ -1093,7 +1250,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>3.63</v>
@@ -1112,19 +1269,19 @@
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>0.0511</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N29" s="4"/>
     </row>
@@ -1133,7 +1290,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>3.31</v>
@@ -1145,10 +1302,10 @@
         <v>12</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="N30" s="4"/>
     </row>
@@ -1157,7 +1314,7 @@
         <v>25.1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>3.14</v>
@@ -1169,10 +1326,10 @@
         <v>12</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -1181,16 +1338,16 @@
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>6.6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -1200,7 +1357,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>1.95</v>
@@ -1219,72 +1376,72 @@
         <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>1.45</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="N34" s="4"/>
     </row>
-    <row r="35" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="9" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="7" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="8" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L35" s="8" t="s">
+      <c r="M36" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N36" s="13" t="s">
         <v>19</v>
-      </c>
-      <c r="M35" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="n">
-        <v>30</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="6" t="n">
-        <v>0.182</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N36" s="13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,16 +1449,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>3.35</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -1311,7 +1468,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0.588</v>
@@ -1323,13 +1480,13 @@
         <v>12</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,16 +1494,16 @@
         <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>0.193</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -1356,16 +1513,16 @@
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>2.86</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -1375,19 +1532,19 @@
         <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>0.935</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="N41" s="4"/>
     </row>
@@ -1402,10 +1559,10 @@
         <v>1.15</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -1421,43 +1578,43 @@
         <v>1.69</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="8" t="n">
+      <c r="C44" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="9" t="n">
         <v>97</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L44" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="N44" s="9" t="s">
-        <v>47</v>
+      <c r="L44" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M44" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N44" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,31 +1636,31 @@
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
     </row>
-    <row r="46" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="n">
+    <row r="46" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="6" t="n">
+      <c r="C46" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="7" t="n">
         <v>2.95</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G46" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>41</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>7.22</v>
@@ -1528,10 +1685,10 @@
         <v>2.48</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
@@ -1541,7 +1698,7 @@
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>0.294</v>
@@ -1553,7 +1710,7 @@
         <v>12</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -1568,13 +1725,13 @@
         <v>0.102</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="N50" s="4"/>
     </row>
@@ -1583,7 +1740,7 @@
         <v>45</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>37.2</v>
@@ -1595,31 +1752,31 @@
         <v>12</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="N51" s="4"/>
     </row>
-    <row r="52" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8" t="n">
+    <row r="52" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9" t="n">
         <v>46</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="8" t="n">
+      <c r="C52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="9" t="n">
         <v>2.93</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M52" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N52" s="9" t="s">
-        <v>52</v>
+      <c r="M52" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N52" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,7 +1784,7 @@
         <v>47</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>0.504</v>
@@ -1639,21 +1796,21 @@
         <v>12</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="5" t="n">
         <v>48</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>23.8</v>
@@ -1665,50 +1822,50 @@
         <v>12</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="N54" s="4"/>
     </row>
-    <row r="55" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8" t="n">
+    <row r="55" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="8" t="n">
+      <c r="C55" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="9" t="n">
         <v>16.1</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M55" s="9"/>
-      <c r="N55" s="9"/>
-    </row>
-    <row r="56" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="n">
+      <c r="F55" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+    </row>
+    <row r="56" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="6" t="n">
+      <c r="C56" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="7" t="n">
         <v>0.649</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="n">
@@ -1727,10 +1884,10 @@
         <v>12</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,7 +1895,7 @@
         <v>52</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>16.8</v>
@@ -1750,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
@@ -1760,7 +1917,7 @@
         <v>52.1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>17.3</v>
@@ -1779,7 +1936,7 @@
         <v>52.2</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>24</v>
@@ -1798,7 +1955,7 @@
         <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>9.76</v>
@@ -1810,37 +1967,42 @@
         <v>12</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="8" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="9" t="n">
         <v>54</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" s="8" t="n">
+      <c r="C62" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="9" t="n">
         <v>2.43</v>
       </c>
-      <c r="F62" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M62" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="N62" s="10"/>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>55</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>28.4</v>
@@ -1851,15 +2013,22 @@
       <c r="G63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>56</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>3.09</v>
@@ -1870,15 +2039,17 @@
       <c r="G64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M64" s="4"/>
+      <c r="M64" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="N64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+    <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="n">
         <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>1.42</v>
@@ -1889,15 +2060,22 @@
       <c r="G65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
+      <c r="L65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M65" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="5" t="n">
         <v>57.1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>1.43</v>
@@ -1911,12 +2089,12 @@
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>58</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>55.4</v>
@@ -1927,48 +2105,61 @@
       <c r="G67" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-    </row>
-    <row r="68" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="n">
+      <c r="M67" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9" t="n">
         <v>59</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="9" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L68" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D68" s="8" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-    </row>
-    <row r="69" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="n">
+      <c r="M68" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N68" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="6" t="n">
+      <c r="C69" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="7" t="n">
         <v>3.44</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F69" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M69" s="7"/>
-      <c r="N69" s="7"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M69" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N69" s="8"/>
+    </row>
+    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <v>61</v>
       </c>
@@ -1979,22 +2170,24 @@
         <v>2.76</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N70" s="4"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="n">
         <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>3.08</v>
@@ -2005,12 +2198,17 @@
       <c r="G71" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="L71" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="M71" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N71" s="4"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <v>63</v>
       </c>
@@ -2021,35 +2219,46 @@
         <v>2.45</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
-    </row>
-    <row r="73" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="9" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L73" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D73" s="8" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M73" s="9"/>
-      <c r="N73" s="9"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
+      <c r="M73" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N73" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="n">
         <v>65</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -2064,10 +2273,17 @@
       <c r="G74" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M74" s="4"/>
-      <c r="N74" s="4"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N74" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <v>66</v>
       </c>
@@ -2083,29 +2299,43 @@
       <c r="G75" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
         <v>67</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>4.17</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="N76" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <v>68</v>
       </c>
@@ -2121,36 +2351,43 @@
       <c r="G77" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L77" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M77" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N77" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
         <v>69</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>2.07</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="N78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
         <v>70</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>2.55</v>
@@ -2161,11 +2398,18 @@
       <c r="G79" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
+      <c r="L79" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N79"/>
+  <autoFilter ref="A1:M79"/>
   <conditionalFormatting sqref="D2:D79">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>

<commit_message>
Incremental update for source classification.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="123">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -164,6 +164,9 @@
     <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead.</t>
   </si>
   <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by power law with index 4.3. Lx at 8kpc 2.5e32 erg/s.</t>
+  </si>
+  <si>
     <t xml:space="preserve">CV Binary?</t>
   </si>
   <si>
@@ -176,19 +179,40 @@
     <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead.</t>
-  </si>
-  <si>
     <t xml:space="preserve">YSO?</t>
   </si>
   <si>
+    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Lx for YSO ranges.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No clear features in lcs. Spectrum best fit is for bbody with temperature 1.7keV. Lx at 8kpc would be 5.1e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good SIMBAD associatoin to radio source. No clear GAIA/2MASS association. Best fit spectrum for bbody with kT 3.6keV and Lx 2.4e33 erg/s at 8kpc distance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARIADNE fit on GAIA source to confirm star.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 0.9keV and nH at reasonable value for source location. At distance source would have Lx 2e31 erg/s.</t>
   </si>
   <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 1.4keV and nH at low value for source location. At distance source would have Lx 3e31 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source.</t>
+    <t xml:space="preserve">Good association to 2MASS source but no optical counterpart. Some variability in lc, but no periodicity. Best fit spectrum is apec with kT = 18.2keV with Lx 4.4e32 at 8kpc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close match to 2MASS source. In area populated by many YSO. No clear features in lc. Best spectrum is apec with kT 5.4keV and Lx at 8kpc is 1.2e33 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Close match to 2MASS source. In area populated by many YSO.  Best spectrum is apec with kT 11.0keV and Lx at 8kpc is 1.2e33 erg/s</t>
   </si>
   <si>
     <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s</t>
@@ -197,10 +221,22 @@
     <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s.</t>
   </si>
   <si>
+    <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and kT2 1.3keV and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s</t>
+    <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No GAIA/2MASS counterparts within 5” or 4+sig. No significant features in lightcurve. Best fit spectrum is for bbody with kT = 0.45 but very high nH. Lx at 8kpc would be 8.0e32 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No good GAIA/2MASS sources within 5” and 3sig+. No significant features in lcs. Spectra poorly fit, but best is for apec+apec with kT1 0.02 and kT2 19.9keV. Lx at 8kpc would be 1.2e33 erg/s.</t>
   </si>
   <si>
     <t xml:space="preserve">SIMBAD association with YSO at 3.2”. 2MASS source at 2.56”, nearest Gaia source at 6.2”.</t>
@@ -215,15 +251,33 @@
     <t xml:space="preserve">Read G-Cas stars. Pulsations etc.</t>
   </si>
   <si>
+    <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 2sig+. No features in lightcurve. Best fit spectrum is for bbody with kT = 1.3keV. At 8kpc Lx would be 1.0e33 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 4sig+. No significant features in lightcurve. Best fit spectrum is for power law with index 1.9. Lx at 8kpc would be 1.7e33 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum (although low quality) is power law with index -0.14. Lx at 8kpc would be 3.1e33 erg/s.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Problems fitting spectrum. Look further into fitting issues. Potential periodicity in lightcurve?</t>
   </si>
   <si>
-    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig.</t>
+    <t xml:space="preserve">Dwarf star?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Potential small flare in lc. Best fit spectrum is for apec with kT 0.8keV. Lx at 8kpc would be 6.1e31 erg/s.</t>
   </si>
   <si>
     <t xml:space="preserve">Magnetar?</t>
   </si>
   <si>
+    <t xml:space="preserve">Paper edits for NW.</t>
+  </si>
+  <si>
     <t xml:space="preserve">GAIA/2MASS association within 2.5”. Best fit spectrum is for bbody with kT=2.1keV. Lx at distance of 1.6kpc would be 1.4e32 erg/s</t>
   </si>
   <si>
@@ -237,6 +291,12 @@
   </si>
   <si>
     <t xml:space="preserve">SIMBAD/GAIA/2MASS association. High mass XRB. Best fit spectrum is for bbody with kT=1.7keV and nH close to expected value. Lx during obs 1.5e35 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flaring lightcurve. Difficulties comparing spectra. All spectra very hard with high Lx estimates at 8kpc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reprocess data for all insts.</t>
   </si>
   <si>
     <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. Several other obs with non-dets.</t>
@@ -474,7 +534,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -582,9 +642,9 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+      <selection pane="bottomLeft" activeCell="M67" activeCellId="0" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -594,7 +654,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.27"/>
@@ -1136,7 +1196,7 @@
       </c>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
         <v>19</v>
       </c>
@@ -1152,7 +1212,9 @@
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="10"/>
+      <c r="M23" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="N23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,13 +1234,13 @@
         <v>21</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,15 +1260,15 @@
         <v>12</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+    <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1221,12 +1283,17 @@
       <c r="G26" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="L26" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="M26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N26" s="4"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>22</v>
       </c>
@@ -1242,10 +1309,12 @@
       <c r="G27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="N27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>23</v>
       </c>
@@ -1261,11 +1330,13 @@
       <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1280,10 +1351,15 @@
       <c r="G29" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="L29" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="M29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N29" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
@@ -1305,7 +1381,7 @@
         <v>51</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N30" s="4"/>
     </row>
@@ -1329,11 +1405,11 @@
         <v>51</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>26</v>
       </c>
@@ -1349,10 +1425,12 @@
       <c r="G32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="N32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>27</v>
       </c>
@@ -1368,10 +1446,15 @@
       <c r="G33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M33" s="4"/>
+      <c r="L33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="N33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>28</v>
       </c>
@@ -1387,8 +1470,11 @@
       <c r="G34" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="L34" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="M34" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="N34" s="4"/>
     </row>
@@ -1412,7 +1498,7 @@
         <v>28</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>19</v>
@@ -1438,14 +1524,14 @@
         <v>17</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="N36" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
         <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1460,8 +1546,15 @@
       <c r="G37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
+      <c r="L37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
@@ -1483,14 +1576,14 @@
         <v>17</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
         <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1505,10 +1598,17 @@
       <c r="G39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>34</v>
       </c>
@@ -1524,11 +1624,13 @@
       <c r="G40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="N40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="5" t="n">
         <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1543,12 +1645,17 @@
       <c r="G41" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="L41" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="M41" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>36</v>
       </c>
@@ -1564,7 +1671,9 @@
       <c r="G42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M42" s="4"/>
+      <c r="M42" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="N42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,7 +1696,7 @@
         <v>51</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="N43" s="4"/>
     </row>
@@ -1608,16 +1717,16 @@
         <v>12</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>39</v>
       </c>
@@ -1633,10 +1742,12 @@
       <c r="G45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M45" s="4"/>
+      <c r="M45" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="N45" s="4"/>
     </row>
-    <row r="46" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="n">
         <v>40</v>
       </c>
@@ -1652,11 +1763,13 @@
       <c r="G46" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M46" s="8"/>
+      <c r="M46" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="N46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="n">
         <v>41</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1671,10 +1784,17 @@
       <c r="G47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>42</v>
       </c>
@@ -1690,7 +1810,9 @@
       <c r="G48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="N48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,11 +1832,11 @@
         <v>12</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="N49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>44</v>
       </c>
@@ -1730,8 +1852,11 @@
       <c r="G50" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="L50" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="M50" s="4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="N50" s="4"/>
     </row>
@@ -1752,9 +1877,11 @@
         <v>12</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N51" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="52" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="n">
@@ -1773,10 +1900,10 @@
         <v>12</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="N52" s="10" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,7 +1926,7 @@
         <v>17</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>19</v>
@@ -1822,10 +1949,10 @@
         <v>12</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="N54" s="4"/>
     </row>
@@ -1845,8 +1972,12 @@
       <c r="G55" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
+      <c r="M55" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="N55" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="56" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="n">
@@ -1884,10 +2015,10 @@
         <v>12</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,7 +2038,7 @@
         <v>12</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
@@ -1967,10 +2098,10 @@
         <v>12</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,7 +2124,7 @@
         <v>17</v>
       </c>
       <c r="M62" s="10" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="N62" s="10"/>
     </row>
@@ -2014,13 +2145,13 @@
         <v>12</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>43</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2040,7 +2171,7 @@
         <v>12</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -2064,10 +2195,10 @@
         <v>17</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2237,7 @@
         <v>12</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>23</v>
@@ -2132,7 +2263,7 @@
         <v>17</v>
       </c>
       <c r="M68" s="10" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="N68" s="10" t="s">
         <v>19</v>
@@ -2155,7 +2286,7 @@
         <v>12</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="N69" s="8"/>
     </row>
@@ -2176,10 +2307,10 @@
         <v>21</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,13 +2330,13 @@
         <v>12</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,10 +2356,10 @@
         <v>21</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,10 +2382,10 @@
         <v>17</v>
       </c>
       <c r="M73" s="10" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,10 +2408,10 @@
         <v>17</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2303,10 +2434,10 @@
         <v>17</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,10 +2460,10 @@
         <v>17</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,10 +2486,10 @@
         <v>51</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,7 +2509,7 @@
         <v>21</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -2399,13 +2530,13 @@
         <v>12</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incremental check for new EuClust alert docs.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="124">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -161,7 +161,10 @@
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead.</t>
+    <t xml:space="preserve">YSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Surrounded by several YSOs.</t>
   </si>
   <si>
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by power law with index 4.3. Lx at 8kpc 2.5e32 erg/s.</t>
@@ -179,10 +182,7 @@
     <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">YSO?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s.</t>
+    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s. Source in region high density YSOs.</t>
   </si>
   <si>
     <t xml:space="preserve">Check Lx for YSO ranges.</t>
@@ -293,12 +293,15 @@
     <t xml:space="preserve">SIMBAD/GAIA/2MASS association. High mass XRB. Best fit spectrum is for bbody with kT=1.7keV and nH close to expected value. Lx during obs 1.5e35 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">Flaring lightcurve. Difficulties comparing spectra. All spectra very hard with high Lx estimates at 8kpc.</t>
+    <t xml:space="preserve">Flaring lightcurve. Difficulties comparing spectra. All spectra very hard with high Lx estimates at 8kpc. In region sparsely populated by variable stars.</t>
   </si>
   <si>
     <t xml:space="preserve">Reprocess data for all insts.</t>
   </si>
   <si>
+    <t xml:space="preserve">Potential close GAIA/2MASS sources. Lightcurve shows significant variability. Spectrum best fit by apec model with kT = 0.5keV. At distance of GAIA source Lx 2.3e30 erg/s.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. Several other obs with non-dets.</t>
   </si>
   <si>
@@ -371,10 +374,10 @@
     <t xml:space="preserve">Association within 2sig to Gaia/sMASS source. Lightcurve shows not outstanding features. Best fit spectrum is for apec with kT 3.3keV. Lx at opt/IR source distance is 4.3e31 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s.</t>
+    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s. In region populated with several long period variable stars.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars.</t>
   </si>
   <si>
     <t xml:space="preserve">Check for periodicitty in lc.</t>
@@ -642,9 +645,9 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M67" activeCellId="0" sqref="M67"/>
+      <selection pane="bottomLeft" activeCell="I76" activeCellId="0" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1189,10 +1192,10 @@
         <v>21</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N22" s="4"/>
     </row>
@@ -1213,7 +1216,7 @@
         <v>12</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N23" s="10"/>
     </row>
@@ -1234,13 +1237,13 @@
         <v>21</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,10 +1263,10 @@
         <v>12</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N25" s="8"/>
     </row>
@@ -1284,7 +1287,7 @@
         <v>21</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>52</v>
@@ -1378,7 +1381,7 @@
         <v>12</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>58</v>
@@ -1402,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>59</v>
@@ -1447,7 +1450,7 @@
         <v>12</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>61</v>
@@ -1471,7 +1474,7 @@
         <v>21</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>62</v>
@@ -1693,7 +1696,7 @@
         <v>21</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>71</v>
@@ -1956,7 +1959,7 @@
       </c>
       <c r="N54" s="4"/>
     </row>
-    <row r="55" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="n">
         <v>49</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="n">
         <v>50</v>
       </c>
@@ -1995,8 +1998,15 @@
       <c r="G56" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
+      <c r="L56" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M56" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="N56" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="n">
@@ -2015,10 +2025,10 @@
         <v>12</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,7 +2048,7 @@
         <v>12</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
@@ -2098,10 +2108,10 @@
         <v>12</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2134,7 @@
         <v>17</v>
       </c>
       <c r="M62" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N62" s="10"/>
     </row>
@@ -2145,13 +2155,13 @@
         <v>12</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>43</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2181,7 @@
         <v>12</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -2195,10 +2205,10 @@
         <v>17</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2237,7 +2247,7 @@
         <v>12</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N67" s="4" t="s">
         <v>23</v>
@@ -2263,7 +2273,7 @@
         <v>17</v>
       </c>
       <c r="M68" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N68" s="10" t="s">
         <v>19</v>
@@ -2286,7 +2296,7 @@
         <v>12</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N69" s="8"/>
     </row>
@@ -2307,10 +2317,10 @@
         <v>21</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,13 +2340,13 @@
         <v>12</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,10 +2366,10 @@
         <v>21</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2382,10 +2392,10 @@
         <v>17</v>
       </c>
       <c r="M73" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,13 +2418,13 @@
         <v>17</v>
       </c>
       <c r="M74" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="N74" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="N74" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <v>66</v>
       </c>
@@ -2434,13 +2444,13 @@
         <v>17</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
         <v>67</v>
       </c>
@@ -2460,10 +2470,10 @@
         <v>17</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2483,13 +2493,13 @@
         <v>12</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2519,7 @@
         <v>21</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -2530,13 +2540,13 @@
         <v>12</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated lightcurve plots to show background contributions.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -645,9 +645,9 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I76" activeCellId="0" sqref="I76"/>
+      <selection pane="bottomLeft" activeCell="H77" activeCellId="0" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2550,7 +2550,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M79"/>
+  <autoFilter ref="A1:N79"/>
   <conditionalFormatting sqref="D2:D79">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>

<commit_message>
Added potential optical-x-ray flux ratio calcs to spectral notebooks.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -645,9 +645,9 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H77" activeCellId="0" sqref="H77"/>
+      <selection pane="bottomLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2550,7 +2550,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N79"/>
+  <autoFilter ref="A1:M79"/>
   <conditionalFormatting sqref="D2:D79">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>

<commit_message>
Stellar fitting with ARIADNE.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$N$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$M$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="122">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -80,10 +80,7 @@
     <t xml:space="preserve">Star?</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaia/2MASS association within 4”. Best fit spectrum is apec with kT = 43keV. At distance of GAIA source would have Lx 6.5e30 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ariadne fit to confirm GAIA/2M is star.</t>
+    <t xml:space="preserve">Gaia/2MASS association within 4”. Best fit spectrum is apec with kT = 43keV. At distance of GAIA source would have Lx 6.5e30 erg/s. Ariadne – Lbol 4Lsun, log(Lx/Lbol) -3.5</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
@@ -122,34 +119,85 @@
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by powerlaw index 1.1 with Lx at 8kpc 2.1e33 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARIADNE fit to confirm if star. Check for pulsation in lc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia source within 2sig. No distinguishing features in lightcurves. Spectra best fit by apec (x2 for 10, and x1 for 10.2) and bbody for alert 10.1. kT are 0.04 and 5.4keV, 1.21keV and 1.4keV respectively. Lx at GAIA source dist 1.3, 3.3 and 2.1e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARIADNE fit for GAIA source to confirm it is star.</t>
+    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc. Insufficient data for ARIADNE fit to stellar properties.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for pulsation in lc. Check Gaia enhanced cats for Lum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia source within 2sig. No distinguishing features in lightcurves. Spectra best fit by apec (x2 for 10, and x1 for 10.2) and bbody for alert 10.1. kT are 0.04 and 5.4keV, 1.21keV and 1.4keV respectively. Lx at GAIA source dist 1.3, 3.3 and 2.1e31 erg/s. Insufficient data for ARIADNE fit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaeck Gaia enhanced cats for Lum</t>
   </si>
   <si>
     <t xml:space="preserve">Star</t>
   </si>
   <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 10.2Lsun, log(Lx/Lbol) -2.8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Ariadne – Lbol 13.5Lsun, log(Lx/Lbol) -3.0</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s. No source available in ARIADNE catalogue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Gaia enhanced cats for Lum.</t>
   </si>
   <si>
     <t xml:space="preserve">PV</t>
   </si>
   <si>
-    <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 13.1Lsun, log(Lx/Lbol) -3.1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source? No clear features in lightcurve. Best fit spectrum is powerlaw index 1.0. Lx at 8kpc is 9.8e32 erg/s.</t>
@@ -158,7 +206,23 @@
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is for power law, or powerlaw with emission line at 6.4keV. Both power laws have index 1.34. Lack of good distance estimate means no luminosity, but flux estimate is 2e-12 erg/s/cm2</t>
   </si>
   <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 15.8Lsun, log(Lx/Lbol) -3.8</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">YSO?</t>
@@ -194,10 +258,23 @@
     <t xml:space="preserve">Good SIMBAD associatoin to radio source. No clear GAIA/2MASS association. Best fit spectrum for bbody with kT 3.6keV and Lx 2.4e33 erg/s at 8kpc distance.</t>
   </si>
   <si>
-    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARIADNE fit on GAIA source to confirm star.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 0.7Lsun, log(Lx/Lbol) -3.6</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 0.9keV and nH at reasonable value for source location. At distance source would have Lx 2e31 erg/s.</t>
@@ -215,25 +292,105 @@
     <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Close match to 2MASS source. In area populated by many YSO.  Best spectrum is apec with kT 11.0keV and Lx at 8kpc is 1.2e33 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 0.04Lsun, log(Lx/Lbol) -4.4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 6.4Lsun, log(Lx/Lbol) -4.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 3.0Lsun, log(Lx/Lbol) -1.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Ariadne – Lbol 24.8Lsun, log(Lx/Lbol) -4.7</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s. No association in ARIADNE dbs.</t>
   </si>
   <si>
     <t xml:space="preserve">No GAIA/2MASS counterparts within 5” or 4+sig. No significant features in lightcurve. Best fit spectrum is for bbody with kT = 0.45 but very high nH. Lx at 8kpc would be 8.0e32 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 15.7Lsun, log(Lx/Lbol) -3.0</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">No good GAIA/2MASS sources within 5” and 3sig+. No significant features in lcs. Spectra poorly fit, but best is for apec+apec with kT1 0.02 and kT2 19.9keV. Lx at 8kpc would be 1.2e33 erg/s.</t>
@@ -257,7 +414,23 @@
     <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 4sig+. No significant features in lightcurve. Best fit spectrum is for power law with index 1.9. Lx at 8kpc would be 1.7e33 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Ariadne – Lbol 5.3Lsun, log(Lx/Lbol) -2.3</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum (although low quality) is power law with index -0.14. Lx at 8kpc would be 3.1e33 erg/s.</t>
@@ -284,7 +457,23 @@
     <t xml:space="preserve">Periodicity in lightcurve?</t>
   </si>
   <si>
-    <t xml:space="preserve">GAIA and 2MASS source within 2.5”. Best fit spectrum is for apec with kT=0.19keV. NH gives reasonable values. Lx at distance of GAIA source gives 6.1e29 erg/s</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GAIA and 2MASS source within 2.5”. Best fit spectrum is for apec with kT=0.19keV. NH gives reasonable values. Lx at distance of GAIA source gives 6.1e29 erg/s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Ariadne – Lbol 3.2Lsun, log(Lx/Lbol) -4.3</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">HM XRB</t>
@@ -299,7 +488,7 @@
     <t xml:space="preserve">Reprocess data for all insts.</t>
   </si>
   <si>
-    <t xml:space="preserve">Potential close GAIA/2MASS sources. Lightcurve shows significant variability. Spectrum best fit by apec model with kT = 0.5keV. At distance of GAIA source Lx 2.3e30 erg/s.</t>
+    <t xml:space="preserve">Potential close GAIA/2MASS sources. Lightcurve shows significant variability. Spectrum best fit by apec model with kT = 0.5keV. At distance of GAIA source Lx 2.3e30 erg/s. No association in ARIADNE cats.</t>
   </si>
   <si>
     <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. Several other obs with non-dets.</t>
@@ -317,7 +506,23 @@
     <t xml:space="preserve">Power law with iron line</t>
   </si>
   <si>
-    <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 0.95Lsun, log(Lx/Lbol) -2.2</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">XRB</t>
@@ -329,16 +534,32 @@
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ariadne fit to confirm GAIA/2M is star. Check for periodicity in low energy lc.</t>
+    <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc. No ARIADNE association in cat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for periodicity in low energy lc. Check for lum in GAIA enahnced cats.</t>
   </si>
   <si>
     <t xml:space="preserve">Strong 2MASS association but no GAIA, and no visible optical source. SIMBAD association IRAS 1747-2648 at 4”. Best fit spec (albeit poor quality) is for power law and bbody with index -1.5, kT 0.78keV and emission line at 6.7keV. Lx at 8kpc is 3.6e33 erg/s. Very variable hard energy</t>
   </si>
   <si>
-    <t xml:space="preserve">GAIA/2MASS/AllWISE source within 1sig. SIMBAD association to SWIFt source at 6”. Poor spectra (MOS only) and best fit is for power law with index 3.6. Lx at distance to optical source is 1.8e31 erg/s</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GAIA/2MASS/AllWISE source within 1sig. SIMBAD association to SWIFt source at 6”. Poor spectra (MOS only) and best fit is for power law with index 3.6. Lx at distance to optical source is 1.8e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 11.2Lsun, log(Lx/Lbol) -3.4</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">No GAIA/2MASS/AllWISE source within 12sig. Best fit spectrum is for bbody kT = 1.1keV. No distance estimate, but Lx 3.6e33 erg/s at 8kpc.</t>
@@ -365,19 +586,80 @@
     <t xml:space="preserve">Try and combine MOS2 data with PN particularly for spectrum.</t>
   </si>
   <si>
-    <t xml:space="preserve">Good Gaia/2mass association with nearby star. Best fit spectrum is for either double or single apec model, with kT1 = 1keV and kT2 =4.0keV. Lx at location of star is 1.2e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARIADNE fit to confirm star.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association within 2sig to Gaia/sMASS source. Lightcurve shows not outstanding features. Best fit spectrum is for apec with kT 3.3keV. Lx at opt/IR source distance is 4.3e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s. In region populated with several long period variable stars.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Good Gaia/2mass association with nearby star. Best fit spectrum is for either double or single apec model, with kT1 = 1keV and kT2 =4.0keV. Lx at location of star is 1.2e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 39.2Lsun, log(Lx/Lbol) -4.1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Association within 2sig to Gaia/sMASS source. Lightcurve shows not outstanding features. Best fit spectrum is for apec with kT 3.3keV. Lx at opt/IR source distance is 4.3e31 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 5.5Lsun, log(Lx/Lbol) -2.7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s. In region populated with several long period variable stars. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 572Lsun, log(Lx/Lbol) -3.6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 1466Lsun, log(Lx/Lbol) -4.5</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Check for periodicitty in lc.</t>
@@ -405,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -426,6 +708,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -496,7 +783,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -557,8 +844,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -647,7 +946,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -775,31 +1074,29 @@
       <c r="M4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1.6</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,7 +1116,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -828,19 +1125,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2.08</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -849,7 +1146,7 @@
         <v>6.1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2.35</v>
@@ -868,22 +1165,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.275</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,11 +1200,11 @@
         <v>12</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>9</v>
       </c>
@@ -927,10 +1224,10 @@
         <v>17</v>
       </c>
       <c r="M11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,10 +1250,10 @@
         <v>17</v>
       </c>
       <c r="M12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,10 +1267,10 @@
         <v>5.02</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>17</v>
@@ -992,10 +1289,10 @@
         <v>3.03</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>17</v>
@@ -1003,12 +1300,12 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>2.2</v>
@@ -1020,21 +1317,19 @@
         <v>12</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0.431</v>
@@ -1046,21 +1341,19 @@
         <v>12</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>2.59</v>
@@ -1075,10 +1368,10 @@
         <v>17</v>
       </c>
       <c r="M17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,16 +1396,14 @@
       <c r="M18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N18" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1.3</v>
@@ -1133,7 +1424,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1.45</v>
@@ -1149,7 +1440,7 @@
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
         <v>17</v>
       </c>
@@ -1171,9 +1462,7 @@
       <c r="M21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="N21" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="N21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
@@ -1186,10 +1475,10 @@
         <v>0.714</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>45</v>
@@ -1231,10 +1520,10 @@
         <v>1.3</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>48</v>
@@ -1251,7 +1540,7 @@
         <v>20.1</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="7" t="n">
         <v>0.395</v>
@@ -1275,16 +1564,16 @@
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1.37</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>45</v>
@@ -1301,7 +1590,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0.913</v>
@@ -1322,7 +1611,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>3.63</v>
@@ -1338,21 +1627,21 @@
       </c>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>0.0511</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>17</v>
@@ -1360,16 +1649,14 @@
       <c r="M29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N29" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="N29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>3.31</v>
@@ -1384,7 +1671,7 @@
         <v>45</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N30" s="4"/>
     </row>
@@ -1393,7 +1680,7 @@
         <v>25.1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>3.14</v>
@@ -1408,7 +1695,7 @@
         <v>45</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -1417,19 +1704,19 @@
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>6.6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -1438,7 +1725,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>1.95</v>
@@ -1453,7 +1740,7 @@
         <v>45</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N33" s="4"/>
     </row>
@@ -1462,22 +1749,22 @@
         <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>1.45</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N34" s="4"/>
     </row>
@@ -1486,7 +1773,7 @@
         <v>29</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>0.98</v>
@@ -1498,21 +1785,19 @@
         <v>12</v>
       </c>
       <c r="L35" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="N35" s="4"/>
     </row>
     <row r="36" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="7" t="n">
         <v>0.182</v>
@@ -1527,11 +1812,9 @@
         <v>17</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="N36" s="13" t="s">
-        <v>19</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="N36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="n">
@@ -1544,27 +1827,25 @@
         <v>3.35</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="N37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
         <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0.588</v>
@@ -1579,11 +1860,9 @@
         <v>17</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="N38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="n">
@@ -1596,19 +1875,19 @@
         <v>0.193</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,19 +1895,19 @@
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>2.86</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N40" s="4"/>
     </row>
@@ -1637,26 +1916,24 @@
         <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>0.935</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="N41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1669,13 +1946,13 @@
         <v>1.15</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N42" s="4"/>
     </row>
@@ -1690,43 +1967,43 @@
         <v>1.69</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="9" t="n">
+      <c r="C44" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="14" t="n">
         <v>97</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L44" s="9" t="s">
+      <c r="F44" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L44" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M44" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="M44" s="10" t="s">
+      <c r="N44" s="16" t="s">
         <v>73</v>
-      </c>
-      <c r="N44" s="10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +2023,7 @@
         <v>12</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N45" s="4"/>
     </row>
@@ -1767,7 +2044,7 @@
         <v>12</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N46" s="8"/>
     </row>
@@ -1776,7 +2053,7 @@
         <v>41</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>7.22</v>
@@ -1791,11 +2068,9 @@
         <v>17</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="N47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -1808,13 +2083,13 @@
         <v>2.48</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N48" s="4"/>
     </row>
@@ -1823,7 +2098,7 @@
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>0.294</v>
@@ -1835,7 +2110,7 @@
         <v>12</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -1850,40 +2125,40 @@
         <v>0.102</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="N50" s="4"/>
+    </row>
+    <row r="51" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="n">
+        <v>45</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="17" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M51" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="N50" s="4"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="1" t="n">
-        <v>37.2</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M51" s="4" t="s">
+      <c r="N51" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="N51" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="52" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,10 +2178,10 @@
         <v>12</v>
       </c>
       <c r="M52" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N52" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="N52" s="10" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,35 +2204,33 @@
         <v>17</v>
       </c>
       <c r="M53" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N53" s="4"/>
+    </row>
+    <row r="54" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="15" t="n">
+        <v>48</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="17" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="N53" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
-        <v>48</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="1" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L54" s="1" t="s">
+      <c r="M54" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="M54" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="N54" s="4"/>
+      <c r="N54" s="18"/>
     </row>
     <row r="55" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="n">
@@ -1970,16 +2243,16 @@
         <v>16.1</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M55" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="N55" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="N55" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="56" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,25 +2260,25 @@
         <v>50</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D56" s="7" t="n">
         <v>0.649</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L56" s="7" t="s">
         <v>17</v>
       </c>
       <c r="M56" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="N56" s="8" t="s">
-        <v>35</v>
+        <v>90</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,78 +2298,78 @@
         <v>12</v>
       </c>
       <c r="M57" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="N57" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N57" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="58" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="n">
         <v>52</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D58" s="1" t="n">
+      <c r="C58" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="17" t="n">
         <v>16.8</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F58" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+    </row>
+    <row r="59" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="n">
         <v>52.1</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" s="1" t="n">
+      <c r="C59" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="17" t="n">
         <v>17.3</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F59" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+    </row>
+    <row r="60" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="15" t="n">
         <v>52.2</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" s="1" t="n">
+      <c r="C60" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="17" t="n">
         <v>24</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
+      <c r="F60" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="n">
         <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>9.76</v>
@@ -2108,10 +2381,10 @@
         <v>12</v>
       </c>
       <c r="M61" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N61" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="N61" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="62" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,22 +2392,22 @@
         <v>54</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D62" s="9" t="n">
         <v>2.43</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L62" s="9" t="s">
         <v>17</v>
       </c>
       <c r="M62" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N62" s="10"/>
     </row>
@@ -2143,7 +2416,7 @@
         <v>55</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>28.4</v>
@@ -2155,13 +2428,13 @@
         <v>12</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>43</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2442,7 @@
         <v>56</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>3.09</v>
@@ -2181,7 +2454,7 @@
         <v>12</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -2190,7 +2463,7 @@
         <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>1.42</v>
@@ -2205,10 +2478,10 @@
         <v>17</v>
       </c>
       <c r="M65" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N65" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="N65" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,7 +2489,7 @@
         <v>57.1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>1.43</v>
@@ -2235,7 +2508,7 @@
         <v>58</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>55.4</v>
@@ -2247,18 +2520,18 @@
         <v>12</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="n">
         <v>59</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D68" s="9" t="n">
         <v>4.13</v>
@@ -2273,11 +2546,9 @@
         <v>17</v>
       </c>
       <c r="M68" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="N68" s="10" t="s">
-        <v>19</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="N68" s="10"/>
     </row>
     <row r="69" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7" t="n">
@@ -2296,7 +2567,7 @@
         <v>12</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N69" s="8"/>
     </row>
@@ -2311,16 +2582,16 @@
         <v>2.76</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M70" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="N70" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="N70" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,7 +2599,7 @@
         <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>3.08</v>
@@ -2340,13 +2611,13 @@
         <v>12</v>
       </c>
       <c r="L71" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M71" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="M71" s="4" t="s">
+      <c r="N71" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="N71" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,16 +2631,16 @@
         <v>2.45</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M72" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N72" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="N72" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="73" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,7 +2648,7 @@
         <v>64</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D73" s="9" t="n">
         <v>1.32</v>
@@ -2392,11 +2663,9 @@
         <v>17</v>
       </c>
       <c r="M73" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N73" s="10" t="s">
-        <v>114</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="N73" s="10"/>
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="n">
@@ -2418,11 +2687,9 @@
         <v>17</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="N74" s="4" t="s">
-        <v>114</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="N74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
@@ -2444,11 +2711,9 @@
         <v>17</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N75" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="N75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -2461,19 +2726,19 @@
         <v>4.17</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,10 +2761,10 @@
         <v>45</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,19 +2772,19 @@
         <v>69</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>2.07</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -2528,7 +2793,7 @@
         <v>70</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>2.55</v>
@@ -2540,17 +2805,17 @@
         <v>12</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M79"/>
+  <autoFilter ref="A1:N79"/>
   <conditionalFormatting sqref="D2:D79">
     <cfRule type="colorScale" priority="2">
       <colorScale>

</xml_diff>

<commit_message>
Periodicity check in unided sources.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="123">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">Gaia/2MASS association within 4”. Best fit spectrum is apec with kT = 43keV. At distance of GAIA source would have Lx 6.5e30 erg/s. Ariadne – Lbol 4Lsun, log(Lx/Lbol) -3.5</t>
   </si>
   <si>
+    <t xml:space="preserve">Fx/Fopt greater than 1?</t>
+  </si>
+  <si>
     <t xml:space="preserve">H</t>
   </si>
   <si>
@@ -107,7 +110,7 @@
     <t xml:space="preserve">See comments</t>
   </si>
   <si>
-    <t xml:space="preserve">PM*</t>
+    <t xml:space="preserve">PM STAR</t>
   </si>
   <si>
     <t xml:space="preserve">Source location in PN image is affected by chip gap. Source too faint to appear on MOS images.</t>
@@ -119,10 +122,10 @@
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by powerlaw index 1.1 with Lx at 8kpc 2.1e33 erg/s.</t>
   </si>
   <si>
-    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc. Insufficient data for ARIADNE fit to stellar properties.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check for pulsation in lc. Check Gaia enhanced cats for Lum.</t>
+    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc. Insufficient data for ARIADNE fit to stellar properties. Noi GAIA cat lum estimate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for pulsation in lc. </t>
   </si>
   <si>
     <t xml:space="preserve">Gaia source within 2sig. No distinguishing features in lightcurves. Spectra best fit by apec (x2 for 10, and x1 for 10.2) and bbody for alert 10.1. kT are 0.04 and 5.4keV, 1.21keV and 1.4keV respectively. Lx at GAIA source dist 1.3, 3.3 and 2.1e31 erg/s. Insufficient data for ARIADNE fit.</t>
@@ -131,7 +134,13 @@
     <t xml:space="preserve">Chaeck Gaia enhanced cats for Lum</t>
   </si>
   <si>
-    <t xml:space="preserve">Star</t>
+    <t xml:space="preserve">STAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s. Ariadne – Lbol 10.2Lsun, log(Lx/Lbol) -2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s. Ariadne – Lbol 13.5Lsun, log(Lx/Lbol) -3.0</t>
   </si>
   <si>
     <r>
@@ -141,7 +150,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s. </t>
+      <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s. No source available in ARIADNE catalogue, but GAIA cat gives Lbol 0.62Lsun and l</t>
     </r>
     <r>
       <rPr>
@@ -149,8 +158,89 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 10.2Lsun, log(Lx/Lbol) -2.8</t>
+      <t xml:space="preserve">og(Lx/Lbol) -2.1</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s. Ariadne – Lbol 13.1Lsun, log(Lx/Lbol) -3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source? No clear features in lightcurve. Best fit spectrum is powerlaw index 1.0. Lx at 8kpc is 9.8e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is for power law, or powerlaw with emission line at 6.4keV. Both power laws have index 1.34. Lack of good distance estimate means no luminosity, but flux estimate is 2e-12 erg/s/cm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s. Ariadne – Lbol 15.8Lsun, log(Lx/Lbol) -3.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Surrounded by several YSOs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by power law with index 4.3. Lx at 8kpc 2.5e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV Binary?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS suorce (within 1sig). Best fit spectrum is for powerlaw with index ~2. nH lower than expected. At distance Lx would be 4.3e30 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search for periodicity?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s. Source in region high density YSOs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Lx for YSO ranges.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No clear features in lcs. Spectrum best fit is for bbody with temperature 1.7keV. Lx at 8kpc would be 5.1e32 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good SIMBAD associatoin to radio source. No clear GAIA/2MASS association. Best fit spectrum for bbody with kT 3.6keV and Lx 2.4e33 erg/s at 8kpc distance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s. Ariadne – Lbol 0.7Lsun, log(Lx/Lbol) -3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 0.9keV and nH at reasonable value for source location. At distance source would have Lx 2e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 1.4keV and nH at low value for source location. At distance source would have Lx 3e31 erg/s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good association to 2MASS source but no optical counterpart. Some variability in lc, but no periodicity. Best fit spectrum is apec with kT = 18.2keV with Lx 4.4e32 at 8kpc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close match to 2MASS source. In area populated by many YSO. No clear features in lc. Best spectrum is apec with kT 5.4keV and Lx at 8kpc is 1.2e33 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Close match to 2MASS source. In area populated by many YSO.  Best spectrum is apec with kT 11.0keV and Lx at 8kpc is 1.2e33 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s. Ariadne – Lbol 0.04Lsun, log(Lx/Lbol) -4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s. Ariadne – Lbol 6.4Lsun, log(Lx/Lbol) -4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s. Ariadne – Lbol 3.0Lsun, log(Lx/Lbol) -1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fx/Fopt greater than 2?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s Ariadne – Lbol 24.8Lsun, log(Lx/Lbol) -4.7</t>
   </si>
   <si>
     <r>
@@ -160,7 +250,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s.</t>
+      <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s. </t>
     </r>
     <r>
       <rPr>
@@ -168,229 +258,14 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Ariadne – Lbol 13.5Lsun, log(Lx/Lbol) -3.0</t>
+      <t xml:space="preserve">No source available in ARIADNE catalogue, but GAIA cat gives Lbol 62Lsun and log(Lx/Lbol) -3.9.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s. No source available in ARIADNE catalogue.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Gaia enhanced cats for Lum.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 13.1Lsun, log(Lx/Lbol) -3.1</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source? No clear features in lightcurve. Best fit spectrum is powerlaw index 1.0. Lx at 8kpc is 9.8e32 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is for power law, or powerlaw with emission line at 6.4keV. Both power laws have index 1.34. Lack of good distance estimate means no luminosity, but flux estimate is 2e-12 erg/s/cm2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 15.8Lsun, log(Lx/Lbol) -3.8</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">YSO?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Surrounded by several YSOs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by power law with index 4.3. Lx at 8kpc 2.5e32 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Binary?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS suorce (within 1sig). Best fit spectrum is for powerlaw with index ~2. nH lower than expected. At distance Lx would be 4.3e30 erg/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search for periodicity?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s. Source in region high density YSOs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Lx for YSO ranges.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No clear features in lcs. Spectrum best fit is for bbody with temperature 1.7keV. Lx at 8kpc would be 5.1e32 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good SIMBAD associatoin to radio source. No clear GAIA/2MASS association. Best fit spectrum for bbody with kT 3.6keV and Lx 2.4e33 erg/s at 8kpc distance.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 0.7Lsun, log(Lx/Lbol) -3.6</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 0.9keV and nH at reasonable value for source location. At distance source would have Lx 2e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 1.4keV and nH at low value for source location. At distance source would have Lx 3e31 erg/s.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good association to 2MASS source but no optical counterpart. Some variability in lc, but no periodicity. Best fit spectrum is apec with kT = 18.2keV with Lx 4.4e32 at 8kpc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close match to 2MASS source. In area populated by many YSO. No clear features in lc. Best spectrum is apec with kT 5.4keV and Lx at 8kpc is 1.2e33 erg/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Close match to 2MASS source. In area populated by many YSO.  Best spectrum is apec with kT 11.0keV and Lx at 8kpc is 1.2e33 erg/s</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 0.04Lsun, log(Lx/Lbol) -4.4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 6.4Lsun, log(Lx/Lbol) -4.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 3.0Lsun, log(Lx/Lbol) -1.2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Ariadne – Lbol 24.8Lsun, log(Lx/Lbol) -4.7</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s. No association in ARIADNE dbs.</t>
-  </si>
-  <si>
     <t xml:space="preserve">No GAIA/2MASS counterparts within 5” or 4+sig. No significant features in lightcurve. Best fit spectrum is for bbody with kT = 0.45 but very high nH. Lx at 8kpc would be 8.0e32 erg/s</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 15.7Lsun, log(Lx/Lbol) -3.0</t>
-    </r>
+    <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s. Ariadne – Lbol 15.7Lsun, log(Lx/Lbol) -3.0</t>
   </si>
   <si>
     <t xml:space="preserve">No good GAIA/2MASS sources within 5” and 3sig+. No significant features in lcs. Spectra poorly fit, but best is for apec+apec with kT1 0.02 and kT2 19.9keV. Lx at 8kpc would be 1.2e33 erg/s.</t>
@@ -414,23 +289,7 @@
     <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 4sig+. No significant features in lightcurve. Best fit spectrum is for power law with index 1.9. Lx at 8kpc would be 1.7e33 erg/s.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. Ariadne – Lbol 5.3Lsun, log(Lx/Lbol) -2.3</t>
-    </r>
+    <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s. Ariadne – Lbol 5.3Lsun, log(Lx/Lbol) -2.3</t>
   </si>
   <si>
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum (although low quality) is power law with index -0.14. Lx at 8kpc would be 3.1e33 erg/s.</t>
@@ -457,23 +316,7 @@
     <t xml:space="preserve">Periodicity in lightcurve?</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">GAIA and 2MASS source within 2.5”. Best fit spectrum is for apec with kT=0.19keV. NH gives reasonable values. Lx at distance of GAIA source gives 6.1e29 erg/s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. Ariadne – Lbol 3.2Lsun, log(Lx/Lbol) -4.3</t>
-    </r>
+    <t xml:space="preserve">GAIA and 2MASS source within 2.5”. Best fit spectrum is for apec with kT=0.19keV. NH gives reasonable values. Lx at distance of GAIA source gives 6.1e29 erg/s. Ariadne – Lbol 3.2Lsun, log(Lx/Lbol) -4.3</t>
   </si>
   <si>
     <t xml:space="preserve">HM XRB</t>
@@ -494,7 +337,7 @@
     <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. Several other obs with non-dets.</t>
   </si>
   <si>
-    <t xml:space="preserve">Check background at end of exposure. Check luminosity during final section of lc.</t>
+    <t xml:space="preserve">Check luminosity during final section of lc.</t>
   </si>
   <si>
     <t xml:space="preserve">RS Cvn Var</t>
@@ -506,23 +349,7 @@
     <t xml:space="preserve">Power law with iron line</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 0.95Lsun, log(Lx/Lbol) -2.2</t>
-    </r>
+    <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s. Ariadne – Lbol 0.95Lsun, log(Lx/Lbol) -2.2</t>
   </si>
   <si>
     <t xml:space="preserve">XRB</t>
@@ -534,32 +361,16 @@
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc. No ARIADNE association in cat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check for periodicity in low energy lc. Check for lum in GAIA enahnced cats.</t>
+    <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc. No ARIADNE association in cat. No GAIA associated luminosity estimate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for periodicity in low energy lc.</t>
   </si>
   <si>
     <t xml:space="preserve">Strong 2MASS association but no GAIA, and no visible optical source. SIMBAD association IRAS 1747-2648 at 4”. Best fit spec (albeit poor quality) is for power law and bbody with index -1.5, kT 0.78keV and emission line at 6.7keV. Lx at 8kpc is 3.6e33 erg/s. Very variable hard energy</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">GAIA/2MASS/AllWISE source within 1sig. SIMBAD association to SWIFt source at 6”. Poor spectra (MOS only) and best fit is for power law with index 3.6. Lx at distance to optical source is 1.8e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 11.2Lsun, log(Lx/Lbol) -3.4</t>
-    </r>
+    <t xml:space="preserve">GAIA/2MASS/AllWISE source within 1sig. SIMBAD association to SWIFt source at 6”. Poor spectra (MOS only) and best fit is for power law with index 3.6. Lx at distance to optical source is 1.8e31 erg/s. Ariadne – Lbol 11.2Lsun, log(Lx/Lbol) -3.4</t>
   </si>
   <si>
     <t xml:space="preserve">No GAIA/2MASS/AllWISE source within 12sig. Best fit spectrum is for bbody kT = 1.1keV. No distance estimate, but Lx 3.6e33 erg/s at 8kpc.</t>
@@ -586,80 +397,16 @@
     <t xml:space="preserve">Try and combine MOS2 data with PN particularly for spectrum.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Good Gaia/2mass association with nearby star. Best fit spectrum is for either double or single apec model, with kT1 = 1keV and kT2 =4.0keV. Lx at location of star is 1.2e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 39.2Lsun, log(Lx/Lbol) -4.1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Association within 2sig to Gaia/sMASS source. Lightcurve shows not outstanding features. Best fit spectrum is for apec with kT 3.3keV. Lx at opt/IR source distance is 4.3e31 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 5.5Lsun, log(Lx/Lbol) -2.7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s. In region populated with several long period variable stars. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 572Lsun, log(Lx/Lbol) -3.6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 1466Lsun, log(Lx/Lbol) -4.5</t>
-    </r>
+    <t xml:space="preserve">Good Gaia/2mass association with nearby star. Best fit spectrum is for either double or single apec model, with kT1 = 1keV and kT2 =4.0keV. Lx at location of star is 1.2e31 erg/s. Ariadne – Lbol 39.2Lsun, log(Lx/Lbol) -4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Association within 2sig to Gaia/sMASS source. Lightcurve shows not outstanding features. Best fit spectrum is for apec with kT 3.3keV. Lx at opt/IR source distance is 4.3e31 erg/s. Ariadne – Lbol 5.5Lsun, log(Lx/Lbol) -2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.9 or 4.2keV. Luminosity at distance of Gaia source Lx 6.2e32 erg/s. In region populated with several long period variable stars. Ariadne – Lbol 572Lsun, log(Lx/Lbol) -3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars. Ariadne – Lbol 1466Lsun, log(Lx/Lbol) -4.5</t>
   </si>
   <si>
     <t xml:space="preserve">Check for periodicitty in lc.</t>
@@ -715,12 +462,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5983B0"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -730,8 +483,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5983B0"/>
-        <bgColor rgb="FF808080"/>
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -783,7 +536,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -804,11 +557,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -818,6 +587,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -836,28 +609,32 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -915,7 +692,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF5EB91E"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF5983B0"/>
       <rgbColor rgb="FF969696"/>
@@ -944,9 +721,9 @@
   <dimension ref="A1:N79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="bottomLeft" activeCell="I73" activeCellId="0" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1052,51 +829,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="5" t="n">
         <v>0.899</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1.6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,7 +895,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1125,19 +904,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2.08</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -1146,7 +925,7 @@
         <v>6.1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2.35</v>
@@ -1160,27 +939,27 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+    <row r="9" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="1" t="n">
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="7" t="n">
         <v>0.275</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="1" t="s">
+      <c r="F9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="L9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="M9" s="8" t="s">
         <v>29</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,12 +979,12 @@
         <v>12</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="9" t="n">
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1224,14 +1003,14 @@
         <v>17</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1250,14 +1029,14 @@
         <v>17</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="9" t="n">
         <v>10.1</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1267,10 +1046,10 @@
         <v>5.02</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>17</v>
@@ -1278,132 +1057,130 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
+    <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="n">
         <v>10.2</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="11" t="n">
         <v>3.03</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="7" t="s">
+      <c r="F14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+    </row>
+    <row r="15" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="n">
+      <c r="C15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="7" t="n">
         <v>2.2</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" s="4" t="s">
+      <c r="F15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="n">
+      <c r="M15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="7" t="n">
         <v>0.431</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="F16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="1" t="n">
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="n">
         <v>2.59</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" s="4" t="s">
+      <c r="F17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="7" t="n">
         <v>1.18</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M18" s="4" t="s">
+      <c r="F18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1.3</v>
@@ -1424,7 +1201,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1.45</v>
@@ -1440,32 +1217,32 @@
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+    <row r="21" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="D21" s="7" t="n">
         <v>0.833</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" s="4" t="s">
+      <c r="F21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="N21" s="4"/>
+      <c r="N21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="n">
+      <c r="A22" s="9" t="n">
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1475,10 +1252,10 @@
         <v>0.714</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>45</v>
@@ -1488,29 +1265,29 @@
       </c>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="n">
+    <row r="23" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="14" t="n">
         <v>1.43</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="M23" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="N23" s="10"/>
+      <c r="N23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="n">
+      <c r="A24" s="9" t="n">
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1520,10 +1297,10 @@
         <v>1.3</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>48</v>
@@ -1535,45 +1312,45 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="n">
+    <row r="25" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="n">
         <v>20.1</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="7" t="n">
+      <c r="C25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="11" t="n">
         <v>0.395</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="11" t="s">
+      <c r="F25" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="N25" s="8"/>
+      <c r="N25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="n">
+      <c r="A26" s="9" t="n">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1.37</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>45</v>
@@ -1590,7 +1367,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0.913</v>
@@ -1611,7 +1388,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>3.63</v>
@@ -1627,36 +1404,36 @@
       </c>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="n">
+    <row r="29" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <v>0.0511</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="D29" s="1" t="n">
-        <v>0.0511</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N29" s="4"/>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="n">
-        <v>25</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>3.31</v>
@@ -1676,11 +1453,11 @@
       <c r="N30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="n">
+      <c r="A31" s="9" t="n">
         <v>25.1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>3.14</v>
@@ -1704,16 +1481,16 @@
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>6.6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>59</v>
@@ -1725,7 +1502,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>1.95</v>
@@ -1749,16 +1526,16 @@
         <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>1.45</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>45</v>
@@ -1768,56 +1545,56 @@
       </c>
       <c r="N34" s="4"/>
     </row>
-    <row r="35" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="n">
+    <row r="35" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="17" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="9" t="n">
+      <c r="C35" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="17" t="n">
         <v>0.98</v>
       </c>
-      <c r="F35" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M35" s="10" t="s">
+      <c r="F35" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="N35" s="4"/>
-    </row>
-    <row r="36" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="n">
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="19" t="n">
         <v>30</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="7" t="n">
+      <c r="C36" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="19" t="n">
         <v>0.182</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M36" s="8" t="s">
+      <c r="F36" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M36" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N36" s="13"/>
+      <c r="N36" s="21"/>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="n">
+      <c r="A37" s="9" t="n">
         <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1827,10 +1604,10 @@
         <v>3.35</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>17</v>
@@ -1838,102 +1615,102 @@
       <c r="M37" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N37" s="4"/>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="n">
+      <c r="N37" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
         <v>32</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="1" t="n">
+      <c r="C38" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="7" t="n">
         <v>0.588</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N38" s="4"/>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="n">
+      <c r="F38" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="N38" s="8"/>
+    </row>
+    <row r="39" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="n">
         <v>33</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="1" t="n">
+      <c r="D39" s="7" t="n">
         <v>0.193</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="F39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>2.86</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="n">
+    <row r="41" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1" t="n">
+      <c r="C41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="7" t="n">
         <v>0.935</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N41" s="4"/>
+      <c r="F41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1946,18 +1723,18 @@
         <v>1.15</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="n">
+      <c r="A43" s="9" t="n">
         <v>37</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1967,43 +1744,43 @@
         <v>1.69</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="n">
+    <row r="44" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="14" t="n">
+      <c r="C44" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="17" t="n">
         <v>97</v>
       </c>
-      <c r="F44" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L44" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="M44" s="16" t="s">
+      <c r="F44" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L44" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="N44" s="16" t="s">
+      <c r="M44" s="18" t="s">
         <v>73</v>
+      </c>
+      <c r="N44" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,54 +1800,54 @@
         <v>12</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N45" s="4"/>
     </row>
-    <row r="46" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="n">
+    <row r="46" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11" t="n">
         <v>40</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="7" t="n">
+      <c r="D46" s="11" t="n">
         <v>2.95</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="N46" s="8"/>
-    </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="n">
+      <c r="F46" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M46" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N46" s="12"/>
+    </row>
+    <row r="47" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="n">
         <v>41</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="1" t="n">
+      <c r="C47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="7" t="n">
         <v>7.22</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="N47" s="4"/>
+      <c r="F47" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -2083,22 +1860,22 @@
         <v>2.48</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="n">
+      <c r="A49" s="23" t="n">
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>0.294</v>
@@ -2110,7 +1887,7 @@
         <v>12</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -2125,164 +1902,164 @@
         <v>0.102</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N50" s="4"/>
     </row>
-    <row r="51" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15" t="n">
+    <row r="51" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="24" t="n">
         <v>45</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="17" t="n">
+      <c r="C51" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="7" t="n">
         <v>37.2</v>
       </c>
-      <c r="F51" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M51" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="N51" s="18" t="s">
+      <c r="F51" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M51" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
+      <c r="N51" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="14" t="n">
         <v>46</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="9" t="n">
+      <c r="D52" s="14" t="n">
         <v>2.93</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M52" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="N52" s="10" t="s">
+      <c r="M52" s="15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="N52" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="1" t="n">
+      <c r="D53" s="7" t="n">
         <v>0.504</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L53" s="1" t="s">
+      <c r="F53" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N53" s="8"/>
+    </row>
+    <row r="54" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="24" t="n">
+        <v>48</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="7" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="M54" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="N54" s="8"/>
+    </row>
+    <row r="55" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="14" t="n">
+        <v>49</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="14" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="N55" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="11" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L56" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M53" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N53" s="4"/>
-    </row>
-    <row r="54" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15" t="n">
-        <v>48</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="17" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L54" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="M54" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="N54" s="18"/>
-    </row>
-    <row r="55" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="n">
-        <v>49</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="9" t="n">
-        <v>16.1</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M55" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="N55" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="n">
-        <v>50</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" s="7" t="n">
-        <v>0.649</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M56" s="8" t="s">
-        <v>90</v>
+      <c r="M56" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="15" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="24" t="n">
         <v>51</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2298,78 +2075,78 @@
         <v>12</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="15" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="24" t="n">
         <v>52</v>
       </c>
-      <c r="C58" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" s="17" t="n">
+      <c r="C58" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="7" t="n">
         <v>16.8</v>
       </c>
-      <c r="F58" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L58" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-    </row>
-    <row r="59" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="15" t="n">
+      <c r="F58" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+    </row>
+    <row r="59" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="24" t="n">
         <v>52.1</v>
       </c>
-      <c r="C59" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="17" t="n">
+      <c r="C59" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="7" t="n">
         <v>17.3</v>
       </c>
-      <c r="F59" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M59" s="18"/>
-      <c r="N59" s="18"/>
-    </row>
-    <row r="60" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="n">
+      <c r="F59" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+    </row>
+    <row r="60" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="24" t="n">
         <v>52.2</v>
       </c>
-      <c r="C60" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="17" t="n">
+      <c r="C60" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="7" t="n">
         <v>24</v>
       </c>
-      <c r="F60" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M60" s="18"/>
-      <c r="N60" s="18"/>
+      <c r="F60" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="15" t="n">
+      <c r="A61" s="23" t="n">
         <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>9.76</v>
@@ -2381,42 +2158,42 @@
         <v>12</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="17" t="n">
         <v>54</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="9" t="n">
+      <c r="C62" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="17" t="n">
         <v>2.43</v>
       </c>
-      <c r="F62" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G62" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="L62" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M62" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="N62" s="10"/>
+      <c r="F62" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M62" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="N62" s="18"/>
     </row>
     <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
         <v>55</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>28.4</v>
@@ -2428,13 +2205,13 @@
         <v>12</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>43</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,7 +2219,7 @@
         <v>56</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>3.09</v>
@@ -2454,16 +2231,16 @@
         <v>12</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N64" s="4"/>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
+      <c r="A65" s="9" t="n">
         <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>1.42</v>
@@ -2478,18 +2255,18 @@
         <v>17</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
+      <c r="A66" s="9" t="n">
         <v>57.1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>1.43</v>
@@ -2508,7 +2285,7 @@
         <v>58</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>55.4</v>
@@ -2520,56 +2297,56 @@
         <v>12</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" s="17" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="17" t="n">
         <v>59</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" s="9" t="n">
+      <c r="C68" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="17" t="n">
         <v>4.13</v>
       </c>
-      <c r="F68" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L68" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M68" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="N68" s="10"/>
-    </row>
-    <row r="69" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7" t="n">
+      <c r="F68" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L68" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M68" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="N68" s="18"/>
+    </row>
+    <row r="69" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="11" t="n">
         <v>60</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="7" t="n">
+      <c r="D69" s="11" t="n">
         <v>3.44</v>
       </c>
-      <c r="F69" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M69" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="N69" s="8"/>
+      <c r="F69" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M69" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -2582,24 +2359,24 @@
         <v>2.76</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="15" t="n">
+      <c r="A71" s="23" t="n">
         <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>3.08</v>
@@ -2611,13 +2388,13 @@
         <v>12</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,89 +2408,89 @@
         <v>2.45</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="73" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="12" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="17" t="n">
         <v>64</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" s="9" t="n">
+      <c r="C73" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="17" t="n">
         <v>1.32</v>
       </c>
-      <c r="F73" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L73" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M73" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="N73" s="10"/>
-    </row>
-    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
+      <c r="F73" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L73" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M73" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="N73" s="18"/>
+    </row>
+    <row r="74" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="n">
         <v>65</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D74" s="1" t="n">
+      <c r="D74" s="7" t="n">
         <v>3.76</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M74" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="N74" s="4"/>
-    </row>
-    <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+      <c r="F74" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M74" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="N74" s="8"/>
+    </row>
+    <row r="75" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="1" t="n">
+      <c r="D75" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L75" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M75" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N75" s="4"/>
+      <c r="F75" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="N75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -2726,19 +2503,19 @@
         <v>4.17</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,10 +2538,10 @@
         <v>45</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,19 +2549,19 @@
         <v>69</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>2.07</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -2793,7 +2570,7 @@
         <v>70</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>2.55</v>
@@ -2805,13 +2582,13 @@
         <v>12</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incremental update to include multi-XMM obs sources and prior dets.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sources of Interest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$N$79</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$L$79</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="142">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -42,15 +42,15 @@
     <t xml:space="preserve">Spectrum</t>
   </si>
   <si>
-    <t xml:space="preserve">Periodogram?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prior det lcs?</t>
   </si>
   <si>
     <t xml:space="preserve">Prior det specs?</t>
   </si>
   <si>
+    <t xml:space="preserve">EQ Real Alert?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Class</t>
   </si>
   <si>
@@ -66,6 +66,9 @@
     <t xml:space="preserve">PPS</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">CV cand</t>
   </si>
   <si>
@@ -81,6 +84,9 @@
     <t xml:space="preserve">Check Chandra obs.</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Star?</t>
   </si>
   <si>
@@ -102,10 +108,13 @@
     <t xml:space="preserve">No good GAIA/2MASS sources within 4sig+. Significant variability in hard band. Best fit spectrum is for bbody with kT=0.29keV and high nH with an additional emission line at 6.7keV. Lx at 8kpc is 4.3e33 erg/s. No MUWCLASS.</t>
   </si>
   <si>
-    <t xml:space="preserve">No Opt/IR conterpart wihtin 5+ sigma. No distinguishing features in lcs. Spectra for both obs best fit by powerlaw although poor quality of spectra. Photon indices are 0.8 and -0.4. Lx at 9kpc would be 1.1e33 and 2.7e33 erg/s. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Examine MOS products from preior obs.</t>
+    <t xml:space="preserve">XRB?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Opt/IR conterpart wihtin 5+ sigma. No distinguishing features in lcs. Spectra for both obs best fit by powerlaw although poor quality of spectra. Photon indices are 0.8 and -0.4. Lx at 9kpc would be 1.1e33 and 2.7e33 erg/s. No MUWCLASS. Not visible in 0554720101 or on chip gaps/bad areas. In prev obs spectrum best fit bbody kT 14keV. Fx/Fopt &gt; 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined spectral fit to all obs?</t>
   </si>
   <si>
     <t xml:space="preserve">Not visible in one prior XMM obs and out of PN view on the second. CLAXBOI – XRB</t>
@@ -129,202 +138,236 @@
     <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by powerlaw index 1.1 with Lx at 8kpc 2.1e33 erg/s. CLAXBOI QSO. No MUWCLASS</t>
   </si>
   <si>
+    <t xml:space="preserve">Check Chandra Oobs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Star/CV?</t>
   </si>
   <si>
-    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc with period ~9ks. Insufficient data for ARIADNE fit to stellar properties. Noi GAIA cat lum estimate. Source not visible in following two XMM observations, and no flux limit map. No CLAXBOI.</t>
+    <t xml:space="preserve">Nearby GAIA source without IR counterpart. Best fit spectrum is for apec with kT 3.1keV and Lx at location of GAIA source 9.2e30 erg/s. Potential periodic variability in lc with period ~9ks. Insufficient data for ARIADNE fit to stellar properties. Noi GAIA cat lum estimate. Source not visible in following two XMM observations, and no flux limit map. No CLAXBOI. No other obs with source detected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reprocess PPS products?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y?</t>
   </si>
   <si>
     <t xml:space="preserve">Gaia source within 2sig. No distinguishing features in lightcurves. Spectra best fit by apec (x2 for 10, and x1 for 10.2) and bbody for alert 10.1. kT are 0.04 and 5.4keV, 1.21keV and 1.4keV respectively. Lx at GAIA source dist 1.3, 3.3 and 2.1e31 erg/s. Insufficient data for ARIADNE fit. No CLAXBOI</t>
   </si>
   <si>
+    <t xml:space="preserve">Chaeck Gaia enhanced cats for Lum. Combined spectral fitting?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s. Ariadne – Lbol 10.2Lsun, log(Lx/Lbol) -2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s. Ariadne – Lbol 13.5Lsun, log(Lx/Lbol) -3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s. No source available in ARIADNE catalogue, but GAIA cat gives Lbol 0.62Lsun and log(Lx/Lbol) -2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s. Ariadne – Lbol 13.1Lsun, log(Lx/Lbol) -3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source? No clear features in lightcurve. Best fit spectrum is powerlaw index 1.0. Lx at 8kpc is 9.8e32 erg/s. In region densely populated by YSOs. MYStIX class is Xgal. No CLAXBOI. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check other Chandra obs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is for power law, or powerlaw with emission line at 6.4keV. Both power laws have index 1.34. Lx would be 5.7e32 at 8kpc. Fx/Fopt is greater than 1.4. Source not detected in two other XMM obs during GP survey 6 months later. Transient source? No CLAXBOI. MUWCLASS – YSO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s. Ariadne – Lbol 15.8Lsun, log(Lx/Lbol) -3.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Surrounded by several YSOs. Classed as YSO by MYStIX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by power law with index 4.3. Lx at 8kpc 2.5e32 erg/s. No detection in XMM obs 5 days later with any instrument. No CLAXBOI.. No MUWCLASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS suorce (within 1sig). Best fit spectrum is for powerlaw with index ~2. nH lower than expected. At distance Lx would be 4.3e30 erg/s. No detected periodicity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s. No detected periodicity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s. Source in region high density YSOs. Identified as YSO by MYStIX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No clear features in lcs. Spectrum best fit is for bbody with temperature 1.7keV. Lx at 8kpc would be 5.1e32 erg/s. Previous XMM detection is questionable. CLAXBOI QSO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good SIMBAD associatoin to radio source. No clear GAIA/2MASS association. Best fit spectrum for bbody with kT 3.6keV and Lx 2.4e33 erg/s at 8kpc distance. CLAXBOI XRB. Previous obs best fit by bbody or powerlaw. Fx/Fopt consistently greater than 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s. Ariadne – Lbol 0.7Lsun, log(Lx/Lbol) -3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 0.9keV and nH at reasonable value for source location. At distance source would have Lx 2e31 erg/s. Classed as YSO by MYStIX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 1.4keV and nH at low value for source location. At distance source would have Lx 3e31 erg/s. Classed as YSO by MYStIX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good association to 2MASS source but no optical counterpart. Some variability in lc, but no periodicity. Best fit spectrum is apec with kT = 18.2keV with Lx 4.4e32 at 8kpc. No CLAXBOI. No SFRs nearby. No MUWCLASS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close match to 2MASS source. In area populated by many YSO. No clear features in lc. Best spectrum is apec with kT 5.4keV and Lx at 2kpc is 7.5e31 erg/s. Not in MYStIX. Not in XMM obs one day previous. No CLAXBOI. Within SFR as per Avedisova 02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Close match to 2MASS source. In area populated by many YSO.  Best spectrum is apec with kT 11.0keV and Lx at 8kpc is 1.2e33 erg/s. Not in MYStIX. Not detected in XMM obs one day previous. No CLAXBOI. Within SFR as per Avedisova 02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s. Ariadne – Lbol 0.04Lsun, log(Lx/Lbol) -4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s. Ariadne – Lbol 6.4Lsun, log(Lx/Lbol) -4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s. Ariadne – Lbol 3.0Lsun, log(Lx/Lbol) -1.2. Not in MYStIX. CLAXBOI XRB. No MUWCLASS. No features in previous obs lcs. Spectra from prior obs best fit by bbody. KT ~1keV. Fx/Fopt consistently above 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s Ariadne – Lbol 24.8Lsun, log(Lx/Lbol) -4.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s. No source available in ARIADNE catalogue, but GAIA cat gives Lbol 62Lsun and log(Lx/Lbol) -3.9.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No GAIA/2MASS counterparts within 5” or 4+sig. No significant features in lightcurve. Best fit spectrum is for bbody with kT = 0.45 but very high nH. Lx at 8kpc would be 8.0e32 erg/s. CLAXBOI XRB. No MUWCLASS. Fx/Fopt of the order 1. Best fits in previous observations is for bbody.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s. Ariadne – Lbol 15.7Lsun, log(Lx/Lbol) -3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star/YSO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No good GAIA/2MASS sources within 5” and 3sig+. No significant features in lcs. Spectra poorly fit, but best is for apec+apec with kT1 0.02 and kT2 19.9keV. Lx at 8kpc would be 1.2e33 erg/s. Source not in following GP obs. No CLAXBOI. No MUWCLASS. Not detected in two followig XMM obs 5/6 months later.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMBAD association with YSO at 3.2”. 2MASS source at 2.56”, nearest Gaia source at 6.2”. Not present in GP obs 6 months later. Lx is 4.5e32 erg/s at 4kpc. No CLAXBOI. Within SFR as per Avedisova 02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gam-Cas?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMBAD/Gaia/2MASS association. Be Star, possible pulsations. Identified by Mondal, Ponti et al as IP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read G-Cas stars. Pulsations etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 2sig+. No features in lightcurve. Best fit spectrum is for bbody with kT = 1.3keV. At 8kpc Lx would be 1.0e33 erg/s. No CLAXBOI. No other observations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 4sig+. No significant features in lightcurve. Best fit spectrum is for power law with index 1.9. Lx at 8kpc would be 1.7e33 erg/s. Source not detected in obs 4 days earlier. No CLAXBOI. No MUWCLASS. Not visible in XMM GP obs 4 days earlier/just off FoV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s. Ariadne – Lbol 5.3Lsun, log(Lx/Lbol) -2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum (although low quality) is power law with index -0.14. Lx at 8kpc would be 3.1e33 erg/s. No CLAXBOI. Not visible in other XMM GP obs. No MUWCLASS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Problems fitting spectrum. Look further into fitting issues. No detectable periodicity in lightcurve. No CLAXBOI. Source detected in previous XMM GP obs but not subsequent. Potentially below sensitivity limit. Interesting features in SWIFT? - EQ. Previous XMM obs spec best fit by powerlaw, index 2. Previous XMM GP obs suggests long term flux decay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fit both XMM obs simultaneously. Try fitting to long-term flux decay. Linear? Exponential?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dwarf star?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Potential small flare in lc. Best fit spectrum is for apec with kT 0.8keV. Lx at 8kpc would be 6.1e31 erg/s. No CLAXBOI. Potential det in other XMM obs as 4XMM J180226.9-232544?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check XMM det for other source?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetar?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper edits for NW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAIA/2MASS association within 2.5”. Best fit spectrum is for bbody with kT=2.1keV. Lx at distance of 1.6kpc would be 1.4e32 erg/s. No periodicity detected in lightcurve. No CLAXBOI. No MUWCLASS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAIA and 2MASS source within 2.5”. Best fit spectrum is for apec with kT=0.19keV. NH gives reasonable values. Lx at distance of GAIA source gives 6.1e29 erg/s. Ariadne – Lbol 3.2Lsun, log(Lx/Lbol) -4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HM XRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMBAD/GAIA/2MASS association. High mass XRB. Best fit spectrum is for bbody with kT=1.7keV and nH close to expected value. Lx during obs 1.5e35 erg/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flaring lightcurve. Difficulties comparing spectra. All spectra very hard with high Lx estimates at 8kpc. In region sparsely populated by variable stars. No CLAXBOI. No MUWCLASS. In suspect area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential close GAIA/2MASS sources. Lightcurve shows significant variability. Spectrum best fit by apec model with kT = 0.5keV. At distance of GAIA source Lx 2.3e30 erg/s. No association in ARIADNE cats. No CLAXBOI. Not detected in three other XMM GP obs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chaeck Gaia enhanced cats for Lum</t>
   </si>
   <si>
-    <t xml:space="preserve">STAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is apec with nH matching expected for location and distance of Gaia/2M source. Temperature ~8keV? At distance source would have Lx approx 6e31 erg/s. Ariadne – Lbol 10.2Lsun, log(Lx/Lbol) -2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 5.4e31 erg/s. Ariadne – Lbol 13.5Lsun, log(Lx/Lbol) -3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 1sig). Best fit spectrum is apec with kT 4.3keV. At distance of Gaia/2M source Lx would be 2e31 erg/s. No source available in ARIADNE catalogue, but GAIA cat gives Lbol 0.62Lsun and log(Lx/Lbol) -2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibe GAIA/2MASS counterpart at 2sig+. Lightcurve to be checked for periodicity. Best fit spectrum is for bbody with kT = 0.65keV. Lx at distance of GAIA source is 3.9e31 erg/s. Ariadne – Lbol 13.1Lsun, log(Lx/Lbol) -3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YSO?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Opt/IR conterpart wihtin 7+ sigma. SIMBAD association with milimetric radio source? No clear features in lightcurve. Best fit spectrum is powerlaw index 1.0. Lx at 8kpc is 9.8e32 erg/s. In region densely populated by YSOs. MYStIX class is Xgal. No CLAXBOI. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check other Chandra obs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XRB?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is for power law, or powerlaw with emission line at 6.4keV. Both power laws have index 1.34. Lx would be 5.7e32 at 8kpc. Fx/Fopt is greater than 1.4. Source not detected in two other XMM obs during GP survey. Transient source? No CLAXBOI. MUWCLASS – YSO.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2sig). Best fit spectrum is powlaw with index ~2, nH slightly lower expected for location and distance of Gaia/2M source. At distance source would have Lx approx 1.1e31 erg/s. Ariadne – Lbol 15.8Lsun, log(Lx/Lbol) -3.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YSO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Surrounded by several YSOs. Classed as YSO by MYStIX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No distinguishing features in lightcurve. Spectrum best fit by power law with index 4.3. Lx at 8kpc 2.5e32 erg/s. No detection in XMM obs 5 days later. No CLAXBOI.. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CV Binary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS suorce (within 1sig). Best fit spectrum is for powerlaw with index ~2. nH lower than expected. At distance Lx would be 4.3e30 erg/s. No detected periodicity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Far softer in second observation.  Best fit spectrum is for apec with kT 0.7keV, and nH around expected value. At distance Lx would be 2.2e30 erg/s. No detected periodicity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source location too close to PN lower edge. MOS2 detection used instead. Good association with GAIA/2MASS/SIMBAD source. LC shows no features. Spectrum best fit by power law index 0.22. Distance est 3.5kpc gives Lx 2.3e32 erg/s. Source in region high density YSOs. Identified as YSO by MYStIX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. No clear features in lcs. Spectrum best fit is for bbody with temperature 1.7keV. Lx at 8kpc would be 5.1e32 erg/s. Previous XMM detection is questionable. CLAXBOI QSO.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good SIMBAD associatoin to radio source. No clear GAIA/2MASS association. Best fit spectrum for bbody with kT 3.6keV and Lx 2.4e33 erg/s at 8kpc distance. CLAXBOI XRB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check for detections in past XMM,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No source apparent on PN image. MOS2 detection used instead. Potential close GAIA/2MASS source. No features in lc. Spectrum best fit by powerlaw index 1.93 and Lx at GAIA source distance gives 6.5e29 erg/s. Ariadne – Lbol 0.7Lsun, log(Lx/Lbol) -3.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 0.9keV and nH at reasonable value for source location. At distance source would have Lx 2e31 erg/s. Classed as YSO by MYStIX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby Gaia/2MASS source (within 2”). Best fit spectrum is bbody with kT 1.4keV and nH at low value for source location. At distance source would have Lx 3e31 erg/s. Classed as YSO by MYStIX.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good association to 2MASS source but no optical counterpart. Some variability in lc, but no periodicity. Best fit spectrum is apec with kT = 18.2keV with Lx 4.4e32 at 8kpc. No CLAXBOI. No SFRs nearby. No MUWCLASS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close match to 2MASS source. In area populated by many YSO. No clear features in lc. Best spectrum is apec with kT 5.4keV and Lx at 2kpc is 7.5e31 erg/s. Not in MYStIX. Not in XMM obs one day previous. No CLAXBOI. Within SFR as per Avedisova 02.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Close match to 2MASS source. In area populated by many YSO.  Best spectrum is apec with kT 11.0keV and Lx at 8kpc is 1.2e33 erg/s. Not in MYStIX. Not detected in XMM obs one day previous. No CLAXBOI. Within SFR as per Avedisova 02.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia source within 1sig. SIMBAD association to high PM star. Best spectrum is 2 apec with kT1 0.3keV and kT2 1.2keV. At location approx 30pc Lx 7.3e27 erg/s. Ariadne – Lbol 0.04Lsun, log(Lx/Lbol) -4.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia and 2MASS sources within 2sig, and SIMBAD association to star. Best fit is apec (although poor), with kT 1.1keV and appropriate nH value. At location of 1.6kpc Lx 1.9e30 erg/s. Ariadne – Lbol 6.4Lsun, log(Lx/Lbol) -4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential close GAIA source. Best fit spectrum is for bbody with kT 1.3keV. Unreliable parallax for Gaia source, but Lx at 8kpc is 8.1e32 erg/s. Ariadne – Lbol 3.0Lsun, log(Lx/Lbol) -1.2. Not in MYStIX. CLAXBOI XRB. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fx/Fopt greater than 2? Look at prior XMM obs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia/2MASS source within 2sig. Best spectrum is 2 apec with kT1 0.19keV and kT2 1.3keV and reasonable nH. At distance of Gaia source 800pc Lx 4.7e30 erg/s Ariadne – Lbol 24.8Lsun, log(Lx/Lbol) -4.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good association with GAIA/2MASS source within 1 sig. No significant features in lightcurves. Best fit spectrum is for powerlaw with index 1.1. Lx at distance to GAIA soruce is 3.3e31 erg/s. No source available in ARIADNE catalogue, but GAIA cat gives Lbol 62Lsun and log(Lx/Lbol) -3.9.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No GAIA/2MASS counterparts within 5” or 4+sig. No significant features in lightcurve. Best fit spectrum is for bbody with kT = 0.45 but very high nH. Lx at 8kpc would be 8.0e32 erg/s. CLAXBOI XRB. No MUWCLASS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check MOS FoV for previous XMM obs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gaia/2MASS source within 1sig. Best spectrum is powerlaw with index 0.9 and low nH. At distance of Gaia source 2.5kpc Lx 6.5e31 erg/s. Ariadne – Lbol 15.7Lsun, log(Lx/Lbol) -3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Star/YSO?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No good GAIA/2MASS sources within 5” and 3sig+. No significant features in lcs. Spectra poorly fit, but best is for apec+apec with kT1 0.02 and kT2 19.9keV. Lx at 8kpc would be 1.2e33 erg/s. Source not in following GP obs. No CLAXBOI. No MUWCLASS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMBAD association with YSO at 3.2”. 2MASS source at 2.56”, nearest Gaia source at 6.2”. Not present in GP obs 6 months later. Lx is 4.5e32 erg/s at 4kpc. No CLAXBOI. Within SFR as per Avedisova 02.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gam-Cas?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMBAD/Gaia/2MASS association. Be Star, possible pulsations. Identified by Mondal, Ponti et al as IP.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read G-Cas stars. Pulsations etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 2sig+. No features in lightcurve. Best fit spectrum is for bbody with kT = 1.3keV. At 8kpc Lx would be 1.0e33 erg/s. No CLAXBOI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS coutnerpart, and none within 4sig+. No significant features in lightcurve. Best fit spectrum is for power law with index 1.9. Lx at 8kpc would be 1.7e33 erg/s. Source not detected in obs 4 days earlier. No CLAXBOI. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close GAIA counterpart. No significant feature in lc. Best fit spectrum is for apec with kT 4.8keV. Lx at distance of GAIA source would be 9.9e31 erg/s. Ariadne – Lbol 5.3Lsun, log(Lx/Lbol) -2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum (although low quality) is power law with index -0.14. Lx at 8kpc would be 3.1e33 erg/s. No CLAXBOI. Not visible in other XMM GP obs. No MUWCLASS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Problems fitting spectrum. Look further into fitting issues. No detectable periodicity in lightcurve. No CLAXBOI. Source detected in previous XMM GP obs but not subsequent. Potentially below sensitivity limit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dwarf star?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Potential small flare in lc. Best fit spectrum is for apec with kT 0.8keV. Lx at 8kpc would be 6.1e31 erg/s. No CLAXBOI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reprocess MOS data for obs with source in FoV.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnetar?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paper edits for NW.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAIA/2MASS association within 2.5”. Best fit spectrum is for bbody with kT=2.1keV. Lx at distance of 1.6kpc would be 1.4e32 erg/s. No periodicity detected in lightcurve. No CLAXBOI. No MUWCLASS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAIA and 2MASS source within 2.5”. Best fit spectrum is for apec with kT=0.19keV. NH gives reasonable values. Lx at distance of GAIA source gives 6.1e29 erg/s. Ariadne – Lbol 3.2Lsun, log(Lx/Lbol) -4.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HM XRB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIMBAD/GAIA/2MASS association. High mass XRB. Best fit spectrum is for bbody with kT=1.7keV and nH close to expected value. Lx during obs 1.5e35 erg/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flaring lightcurve. Difficulties comparing spectra. All spectra very hard with high Lx estimates at 8kpc. In region sparsely populated by variable stars. No CLAXBOI. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reprocess data for all insts.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential close GAIA/2MASS sources. Lightcurve shows significant variability. Spectrum best fit by apec model with kT = 0.5keV. At distance of GAIA source Lx 2.3e30 erg/s. No association in ARIADNE cats. No CLAXBOI.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. Several other obs with non-dets. In region sparsley populated by YSOs. No CLAXBOI. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check luminosity during final section of lc.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ariadne – Lbol 0.28Lsun, log(Lx/Lbol) -2.3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Several other obs with non-dets. In region sparsley populated by YSOs. No CLAXBOI. No MUWCLASS</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Check luminosity during final section of lc. ARIADNE fit to source.</t>
   </si>
   <si>
     <t xml:space="preserve">RS Cvn Var</t>
@@ -333,7 +376,7 @@
     <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 8sig. Best fit spectrum is for apec with kT = 2.44keV. High nH above 10^23. Compare prev XMM obs. Spectral changes? CLAXBOI XRB</t>
   </si>
   <si>
-    <t xml:space="preserve">Power law with iron line</t>
+    <t xml:space="preserve">Examine products from other XMM obs. Pulsation search?</t>
   </si>
   <si>
     <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s. Ariadne – Lbol 0.95Lsun, log(Lx/Lbol) -2.2</t>
@@ -348,7 +391,10 @@
     <t xml:space="preserve">SWIFT XRB association.</t>
   </si>
   <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s. No CLAXBOI. No MUWCLASS</t>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s. No CLAXBOI. No MUWCLASS. Look at short-term Chandra var – EQ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examine products from other XMM obs.</t>
   </si>
   <si>
     <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc. No ARIADNE association in cat. No GAIA associated luminosity estimate. No periodicity in lightcurves.</t>
@@ -369,22 +415,19 @@
     <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Little information in lightcurve. Spectrum is low quality and best fits are apec and power law with kT = 5.9keV, or index of 1.5. No distance estimate, but at galactic centre Lx 1.4e33 erg/s. No CLAXBOI. No MUWCLASS</t>
   </si>
   <si>
-    <t xml:space="preserve">Cash fit to spectrum?</t>
-  </si>
-  <si>
     <t xml:space="preserve">CV?</t>
   </si>
   <si>
-    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 10sig. Lightcurve shows potentially three peaks with periods of quiescence in between. Spectrum is best fit by blackbody with kT 0.9keV. No distance estimate, but at 8kpc Lx 1.2e33 erg/s. No CLAXBOI. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potential for proposal to follow-up on order 25ks. Combine PN and M2 data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Gaia/2mass sources within 5sig. Lightcurve shows little variability. Spectrum best fit by powerlaw with index 0.9. No distance estimate, but Lx at 8kpc is 3.0e33 erg/s. No CLAXBOI. No MUWCLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Try and combine MOS2 data with PN particularly for spectrum.</t>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 10sig. Lightcurve shows potentially three peaks with periods of quiescence in between. Spectrum is best fit by blackbody with kT 0.9keV. No distance estimate, but at 8kpc Lx 1.2e33 erg/s. No CLAXBOI. No MUWCLASS. Possibility of NICER TOO? - EQ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine PN and M2 data. Check Chandra obs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2mass sources within 5sig. Lightcurve shows little variability. Spectrum best fit by powerlaw with index 0.9. No distance estimate, but Lx at 8kpc is 3.0e33 erg/s. No CLAXBOI. No MUWCLASS. Pulsations?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try and combine MOS2 data with PN particularly for spectrum. Check Chandra obs. Pulsation search?</t>
   </si>
   <si>
     <t xml:space="preserve">Good Gaia/2mass association with nearby star. Best fit spectrum is for either double or single apec model, with kT1 = 1keV and kT2 =4.0keV. Lx at location of star is 1.2e31 erg/s. Ariadne – Lbol 39.2Lsun, log(Lx/Lbol) -4.1</t>
@@ -399,13 +442,16 @@
     <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars. Ariadne – Lbol 1466Lsun, log(Lx/Lbol) -4.5. No periodicity detectable in lightcurves.</t>
   </si>
   <si>
-    <t xml:space="preserve">SIMBAD association with 2MASS for YSO. LC shows one strong flare towards end of obs, but many bad time ints before. Best fit spec is for powerlaw with index 1.4. No distance estimate, but Lx at 8kpc is 2.9e33 erg/s. Not detected in two recent XMM obs. Check flare size/duration against YSOs. Not in MYStIX. No CLAXBOI</t>
+    <t xml:space="preserve">SIMBAD association with 2MASS for YSO. LC shows one strong flare towards end of obs, but many bad time ints before. Best fit spec is for powerlaw with index 1.4. No distance estimate, but Lx at 8kpc is 2.9e33 erg/s. Not detected in two recent XMM obs. Flux limit 0886040201 – 9.4e-15. Check flare size/duration against YSOs. Not in MYStIX. No CLAXBOI</t>
   </si>
   <si>
     <t xml:space="preserve">Check flare against YSO/star.</t>
   </si>
   <si>
-    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Gaia/2MASS source association. Best fit spectrum is bbody with kT 1.3keV and Lx at Gaia source of 2.6e32 erg/s. No distinguishing features in lc. No CLAXBOI. No MUWCLASS</t>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Gaia/2MASS source association. Best fit spectrum is bbody with kT 1.3keV and Lx at Gaia source of 2.6e32 erg/s. No distinguishing features in lc. No CLAXBOI. No MUWCLASS. Not detected 0902780101, 0902780201, 0902780701.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check products from other XMM obs.</t>
   </si>
   <si>
     <t xml:space="preserve">No GAIA/2MASS source within 6sig. Small, but fast variability in lc at higher energy. Best fit spectrum is bbody kT = 0.38keV with an iron line at 6.4keV. Lx at 8kpc would be 1.4e33 erg/s. No periodicity detectable in lcs. CLAXBOI QSO. No MUWCLASS.</t>
@@ -439,7 +485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -461,8 +507,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,6 +536,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF6D"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -542,7 +599,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -583,7 +640,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -616,6 +677,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -728,12 +793,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:AMJ80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="M50" activeCellId="0" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -745,14 +810,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="98.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="98.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="14" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,16 +847,16 @@
       <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -809,15 +874,19 @@
       <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="M2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -835,11 +904,14 @@
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="M3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,14 +930,17 @@
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>18</v>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,22 +948,25 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1.6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,42 +985,51 @@
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="M6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2.08</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="9" t="n">
         <v>6.1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2.35</v>
@@ -953,33 +1040,40 @@
       <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" s="7"/>
+      <c r="J8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>0.275</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -997,10 +1091,15 @@
       <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="M10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" s="7"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="n">
@@ -1018,16 +1117,21 @@
       <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>34</v>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="7"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="n">
+      <c r="A12" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1042,18 +1146,21 @@
       <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>18</v>
+      <c r="J12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="n">
+      <c r="A13" s="10" t="n">
         <v>10.1</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1063,45 +1170,52 @@
         <v>5.02</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+    </row>
+    <row r="14" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="n">
         <v>10.2</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11" t="n">
+      <c r="D14" s="12" t="n">
         <v>3.03</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="F14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="n">
         <v>2.2</v>
@@ -1112,20 +1226,24 @@
       <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="6"/>
+      <c r="J15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>0.431</v>
@@ -1136,20 +1254,24 @@
       <c r="G16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" s="6"/>
+      <c r="J16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>2.59</v>
@@ -1160,20 +1282,24 @@
       <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N17" s="6"/>
+      <c r="J17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D18" s="5" t="n">
         <v>1.18</v>
@@ -1184,20 +1310,24 @@
       <c r="G18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N18" s="6"/>
+      <c r="J18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1.3</v>
@@ -1208,14 +1338,17 @@
       <c r="G19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>44</v>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,7 +1356,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1.45</v>
@@ -1234,14 +1367,17 @@
       <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>47</v>
+      <c r="J20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N20" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1385,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5" t="n">
         <v>0.833</v>
@@ -1260,139 +1396,163 @@
       <c r="G21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="N21" s="6"/>
+      <c r="J21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M21" s="6"/>
+      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
         <v>18</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D22" s="5" t="n">
         <v>0.714</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N22" s="6"/>
-    </row>
-    <row r="23" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="n">
-        <v>19</v>
-      </c>
-      <c r="C23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M22" s="6"/>
+      <c r="AMJ22" s="0"/>
+    </row>
+    <row r="23" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="n">
+        <v>19</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="14" t="n">
+      <c r="D23" s="15" t="n">
         <v>1.43</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="J23" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
         <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>1.3</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N24" s="6"/>
-    </row>
-    <row r="25" s="16" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" s="6"/>
+      <c r="AMJ24" s="0"/>
+    </row>
+    <row r="25" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="n">
         <v>20.1</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="16" t="n">
+      <c r="C25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="17" t="n">
         <v>0.395</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="M25" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="N25" s="18"/>
+      <c r="F25" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D26" s="5" t="n">
         <v>1.37</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N26" s="6"/>
+      <c r="L26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="6"/>
+      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0.913</v>
@@ -1403,19 +1563,22 @@
       <c r="G27" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="M27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="n">
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>3.63</v>
@@ -1426,11 +1589,17 @@
       <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M28" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N28" s="7" t="s">
-        <v>59</v>
+      <c r="J28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,31 +1607,35 @@
         <v>24</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D29" s="5" t="n">
         <v>0.0511</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N29" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M29" s="6"/>
+      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D30" s="5" t="n">
         <v>3.31</v>
@@ -1473,20 +1646,24 @@
       <c r="G30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="N30" s="6"/>
+      <c r="J30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M30" s="6"/>
+      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
         <v>25.1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D31" s="5" t="n">
         <v>3.14</v>
@@ -1497,35 +1674,42 @@
       <c r="G31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N31" s="6"/>
+      <c r="J31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M31" s="6"/>
+      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>6.6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N32" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,7 +1717,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>1.95</v>
@@ -1544,114 +1728,133 @@
       <c r="G33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L33" s="5" t="s">
-        <v>50</v>
+      <c r="J33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
         <v>28</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D34" s="5" t="n">
         <v>1.45</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="n">
+        <v>16</v>
+      </c>
+      <c r="AMJ34" s="0"/>
+    </row>
+    <row r="35" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="21" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="19" t="n">
+      <c r="C35" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="21" t="n">
         <v>0.98</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="21" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L35" s="19" t="s">
+      <c r="J35" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L35" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="M35" s="6"/>
+      <c r="AMJ35" s="0"/>
+    </row>
+    <row r="36" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="17" t="n">
         <v>30</v>
       </c>
-      <c r="M35" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="N35" s="6"/>
-    </row>
-    <row r="36" s="16" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="n">
-        <v>30</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="16" t="n">
+      <c r="C36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="17" t="n">
         <v>0.182</v>
       </c>
-      <c r="F36" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="L36" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M36" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="N36" s="18"/>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="M36" s="19"/>
+      <c r="AMJ36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="n">
         <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>3.35</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M37" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="N37" s="7" t="s">
-        <v>69</v>
+        <v>24</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,7 +1862,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>0.588</v>
@@ -1670,59 +1873,70 @@
       <c r="G38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L38" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M38" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N38" s="6"/>
+      <c r="J38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M38" s="6"/>
+      <c r="AMJ38" s="0"/>
     </row>
     <row r="39" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="n">
         <v>33</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>0.193</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="N39" s="6"/>
-    </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M39" s="6"/>
+      <c r="AMJ39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>2.86</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>73</v>
+        <v>24</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M40" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,24 +1944,28 @@
         <v>35</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>0.935</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L41" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N41" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M41" s="6"/>
+      <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="n">
@@ -1760,18 +1978,23 @@
         <v>1.15</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>75</v>
+        <v>24</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="N42" s="7"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="43" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
@@ -1784,46 +2007,52 @@
         <v>1.69</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="n">
+        <v>24</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M43" s="6"/>
+      <c r="AMJ43" s="0"/>
+    </row>
+    <row r="44" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="23" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="19" t="n">
+      <c r="C44" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="21" t="n">
         <v>97</v>
       </c>
-      <c r="F44" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L44" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="M44" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="N44" s="20" t="s">
-        <v>80</v>
-      </c>
+      <c r="F44" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J44" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="M44" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AMJ44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -1841,40 +2070,49 @@
       <c r="G45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M45" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="N45" s="7"/>
-    </row>
-    <row r="46" s="11" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="11" t="n">
+      <c r="J45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M45" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" s="12" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="12" t="n">
         <v>40</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="11" t="n">
+      <c r="D46" s="12" t="n">
         <v>2.95</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="M46" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="N46" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="F46" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMJ46" s="0"/>
     </row>
     <row r="47" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
         <v>41</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D47" s="5" t="n">
         <v>7.22</v>
@@ -1885,13 +2123,17 @@
       <c r="G47" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="N47" s="6"/>
+      <c r="J47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="M47" s="6"/>
+      <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -1904,24 +2146,27 @@
         <v>2.48</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="N48" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="25" t="n">
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>0.294</v>
@@ -1932,10 +2177,15 @@
       <c r="G49" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="M49" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="N49" s="7"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="n">
@@ -1948,73 +2198,84 @@
         <v>0.102</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L50" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="N50" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="24" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="26" t="n">
         <v>45</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>21</v>
+      <c r="C51" s="14" t="s">
+        <v>23</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>37.2</v>
       </c>
-      <c r="F51" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>12</v>
+      <c r="F51" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J51" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="N51" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="n">
+        <v>94</v>
+      </c>
+      <c r="AMJ51" s="0"/>
+    </row>
+    <row r="52" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="15" t="n">
         <v>46</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="14" t="n">
+      <c r="D52" s="15" t="n">
         <v>2.93</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M52" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N52" s="15" t="s">
-        <v>17</v>
-      </c>
+      <c r="J52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L52" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="M52" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMJ52" s="0"/>
     </row>
     <row r="53" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="n">
         <v>47</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>0.504</v>
@@ -2025,89 +2286,105 @@
       <c r="G53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M53" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="N53" s="6"/>
-    </row>
-    <row r="54" s="13" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24" t="n">
+      <c r="J53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L53" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M53" s="6"/>
+      <c r="AMJ53" s="0"/>
+    </row>
+    <row r="54" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="26" t="n">
         <v>48</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>42</v>
+      <c r="C54" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>23.8</v>
       </c>
-      <c r="F54" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L54" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="M54" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N54" s="6"/>
-    </row>
-    <row r="55" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="n">
+      <c r="F54" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M54" s="6"/>
+      <c r="AMJ54" s="0"/>
+    </row>
+    <row r="55" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="15" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="14" t="n">
+      <c r="D55" s="15" t="n">
         <v>16.1</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="M55" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="N55" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="n">
+      <c r="F55" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="M55" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AMJ55" s="0"/>
+    </row>
+    <row r="56" s="12" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D56" s="11" t="n">
+      <c r="C56" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="12" t="n">
         <v>0.649</v>
       </c>
-      <c r="F56" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L56" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M56" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="N56" s="25" t="s">
-        <v>37</v>
-      </c>
+      <c r="F56" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="M56" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AMJ56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24" t="n">
+      <c r="A57" s="26" t="n">
         <v>51</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2122,79 +2399,97 @@
       <c r="G57" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="M57" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="N57" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="24" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="26" t="n">
         <v>52</v>
       </c>
-      <c r="C58" s="13" t="s">
-        <v>28</v>
+      <c r="C58" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>16.8</v>
       </c>
-      <c r="F58" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L58" s="13" t="s">
-        <v>100</v>
-      </c>
+      <c r="F58" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L58" s="6"/>
       <c r="M58" s="6"/>
-      <c r="N58" s="6"/>
-    </row>
-    <row r="59" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24" t="n">
+      <c r="AMJ58" s="0"/>
+    </row>
+    <row r="59" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="26" t="n">
         <v>52.1</v>
       </c>
-      <c r="C59" s="13" t="s">
-        <v>28</v>
+      <c r="C59" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="D59" s="5" t="n">
         <v>17.3</v>
       </c>
-      <c r="F59" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>12</v>
-      </c>
+      <c r="F59" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L59" s="6"/>
       <c r="M59" s="6"/>
-      <c r="N59" s="6"/>
-    </row>
-    <row r="60" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="24" t="n">
+      <c r="AMJ59" s="0"/>
+    </row>
+    <row r="60" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="26" t="n">
         <v>52.2</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>28</v>
+      <c r="C60" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="F60" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>12</v>
-      </c>
+      <c r="F60" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L60" s="6"/>
       <c r="M60" s="6"/>
-      <c r="N60" s="6"/>
+      <c r="AMJ60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="n">
+      <c r="A61" s="26" t="n">
         <v>53</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>9.76</v>
@@ -2205,43 +2500,53 @@
       <c r="G61" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L61" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="M61" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="N61" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="62" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="19" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="21" t="n">
         <v>54</v>
       </c>
-      <c r="C62" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="19" t="n">
+      <c r="C62" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="21" t="n">
         <v>2.43</v>
       </c>
-      <c r="F62" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G62" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L62" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="M62" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="N62" s="20"/>
+      <c r="F62" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J62" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L62" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="M62" s="22"/>
+      <c r="AMJ62" s="0"/>
     </row>
     <row r="63" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="n">
         <v>55</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D63" s="5" t="n">
         <v>28.4</v>
@@ -2252,22 +2557,26 @@
       <c r="G63" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L63" s="5" t="s">
-        <v>104</v>
+      <c r="J63" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L63" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="M63" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="N63" s="6" t="s">
-        <v>106</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="AMJ63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
         <v>56</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>3.09</v>
@@ -2278,17 +2587,22 @@
       <c r="G64" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="M64" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="N64" s="7"/>
+        <v>114</v>
+      </c>
     </row>
     <row r="65" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="n">
         <v>57</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D65" s="5" t="n">
         <v>1.42</v>
@@ -2299,20 +2613,24 @@
       <c r="G65" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L65" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M65" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="N65" s="6"/>
+      <c r="J65" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L65" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="M65" s="6"/>
+      <c r="AMJ65" s="0"/>
     </row>
     <row r="66" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="n">
         <v>57.1</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D66" s="5" t="n">
         <v>1.43</v>
@@ -2323,18 +2641,22 @@
       <c r="G66" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L66" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="J66" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L66" s="6"/>
       <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
+      <c r="AMJ66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>58</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>55.4</v>
@@ -2345,57 +2667,70 @@
       <c r="G67" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L67" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="M67" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="N67" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" s="19" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="19" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" s="21" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="21" t="n">
         <v>59</v>
       </c>
-      <c r="C68" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D68" s="19" t="n">
+      <c r="C68" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="21" t="n">
         <v>4.13</v>
       </c>
-      <c r="F68" s="19" t="s">
+      <c r="F68" s="21" t="s">
         <v>12</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L68" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="M68" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="N68" s="20"/>
-    </row>
-    <row r="69" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="11" t="n">
+      <c r="J68" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K68" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L68" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="M68" s="22"/>
+      <c r="AMJ68" s="0"/>
+    </row>
+    <row r="69" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="11" t="n">
+      <c r="D69" s="12" t="n">
         <v>3.44</v>
       </c>
-      <c r="F69" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="M69" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="N69" s="12"/>
+      <c r="F69" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J69" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L69" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="M69" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AMJ69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -2408,24 +2743,27 @@
         <v>2.76</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="M70" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="N70" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="23" t="n">
+      <c r="A71" s="25" t="n">
         <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>3.08</v>
@@ -2436,17 +2774,20 @@
       <c r="G71" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>115</v>
+      <c r="J71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="M71" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="N71" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <v>63</v>
       </c>
@@ -2457,41 +2798,51 @@
         <v>2.45</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L72" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="M72" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="N72" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" s="19" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="19" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="21" t="n">
         <v>64</v>
       </c>
-      <c r="C73" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D73" s="19" t="n">
+      <c r="C73" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" s="21" t="n">
         <v>1.32</v>
       </c>
-      <c r="F73" s="19" t="s">
+      <c r="F73" s="21" t="s">
         <v>12</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L73" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="M73" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="N73" s="20"/>
+      <c r="J73" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K73" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L73" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="M73" s="22"/>
+      <c r="AMJ73" s="0"/>
     </row>
     <row r="74" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="n">
@@ -2509,13 +2860,17 @@
       <c r="G74" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L74" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M74" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="N74" s="6"/>
+      <c r="J74" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="M74" s="6"/>
+      <c r="AMJ74" s="0"/>
     </row>
     <row r="75" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="n">
@@ -2533,39 +2888,47 @@
       <c r="G75" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L75" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M75" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="N75" s="6"/>
+      <c r="J75" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K75" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L75" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="M75" s="6"/>
+      <c r="AMJ75" s="0"/>
     </row>
     <row r="76" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="n">
         <v>67</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D76" s="5" t="n">
         <v>4.17</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L76" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M76" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="N76" s="6"/>
-    </row>
-    <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="M76" s="6"/>
+      <c r="AMJ76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <v>68</v>
       </c>
@@ -2581,14 +2944,17 @@
       <c r="G77" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>44</v>
+      <c r="J77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L77" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="M77" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="N77" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,28 +2962,33 @@
         <v>69</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>2.07</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L78" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="M78" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N78" s="7"/>
+        <v>133</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
         <v>70</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>2.55</v>
@@ -2628,18 +2999,38 @@
       <c r="G79" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>115</v>
+      <c r="J79" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L79" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="M79" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="N79" s="7" t="s">
-        <v>128</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="1" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N79"/>
+  <autoFilter ref="A1:L79"/>
   <conditionalFormatting sqref="D20:D79 D2:D18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2686,7 +3077,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="193.83"/>
   </cols>
@@ -2699,7 +3090,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2707,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,7 +3106,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,10 +3114,10 @@
         <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,7 +3125,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +3133,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,7 +3141,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,7 +3149,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reorganised for one false alert due to reflection ring.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -13,7 +13,8 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$L$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'All Source Classification'!$A$1:$L$78</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="140">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -105,7 +106,7 @@
     <t xml:space="preserve">SIMBAD association to X-ray source at 6”. No good GAIA/2MASS within 3”. Best fit spectrum is powerlaw with index 1.4. Lx at 8kpc would be 8.9e32 erg/s. No periodicity in lcs. No detection in preior XMM obs. No MUWCLASS</t>
   </si>
   <si>
-    <t xml:space="preserve">No good GAIA/2MASS sources within 4sig+. Significant variability in hard band. Best fit spectrum is for bbody with kT=0.29keV and high nH with an additional emission line at 6.7keV. Lx at 8kpc is 4.3e33 erg/s. No MUWCLASS.</t>
+    <t xml:space="preserve">No good GAIA/2MASS sources within 4sig+. Significant variability in hard band. Best fit spectrum is for bbody with kT=0.29keV and high nH with an additional emission line at 6.7keV. Lx at 8kpc is 4.3e33 erg/s. No MUWCLASS. No nearby SFRs.</t>
   </si>
   <si>
     <t xml:space="preserve">XRB?</t>
@@ -300,10 +301,10 @@
     <t xml:space="preserve">Dwarf star?</t>
   </si>
   <si>
-    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Potential small flare in lc. Best fit spectrum is for apec with kT 0.8keV. Lx at 8kpc would be 6.1e31 erg/s. No CLAXBOI. Potential det in other XMM obs as 4XMM J180226.9-232544?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check XMM det for other source?</t>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Potential small flare in lc. Best fit spectrum is for apec with kT 0.8keV. Lx at 8kpc would be 6.1e31 erg/s. No CLAXBOI. Potential det in other XMM obs as 4XMM J180226.9-232544? Other XMM det has flux of order 7e-12. Would result in Fx/Fopt of order 100.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fit both spectra simultaneously.</t>
   </si>
   <si>
     <t xml:space="preserve">Magnetar?</t>
@@ -324,47 +325,13 @@
     <t xml:space="preserve">SIMBAD/GAIA/2MASS association. High mass XRB. Best fit spectrum is for bbody with kT=1.7keV and nH close to expected value. Lx during obs 1.5e35 erg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flaring lightcurve. Difficulties comparing spectra. All spectra very hard with high Lx estimates at 8kpc. In region sparsely populated by variable stars. No CLAXBOI. No MUWCLASS. In suspect area.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Potential close GAIA/2MASS sources. Lightcurve shows significant variability. Spectrum best fit by apec model with kT = 0.5keV. At distance of GAIA source Lx 2.3e30 erg/s. No association in ARIADNE cats. No CLAXBOI. Not detected in three other XMM GP obs.</t>
   </si>
   <si>
     <t xml:space="preserve">Chaeck Gaia enhanced cats for Lum</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ariadne – Lbol 0.28Lsun, log(Lx/Lbol) -2.3. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Several other obs with non-dets. In region sparsley populated by YSOs. No CLAXBOI. No MUWCLASS</t>
-    </r>
+    <t xml:space="preserve">Potential flare at end of lightcurve. Good GAIA and 2MASS matches within 1” and 1.5sig. Best fit spectrum is powerlaw with index 1.3. Lx at distance of GAIA source is 5.3e30 erg/s. Ariadne – Lbol 0.28Lsun, log(Lx/Lbol) -2.3. Several other obs with non-dets. In region sparsley populated by YSOs. No CLAXBOI. No MUWCLASS</t>
   </si>
   <si>
     <t xml:space="preserve">Check luminosity during final section of lc. ARIADNE fit to source.</t>
@@ -373,10 +340,13 @@
     <t xml:space="preserve">RS Cvn Var</t>
   </si>
   <si>
-    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 8sig. Best fit spectrum is for apec with kT = 2.44keV. High nH above 10^23. Compare prev XMM obs. Spectral changes? CLAXBOI XRB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Examine products from other XMM obs. Pulsation search?</t>
+    <t xml:space="preserve">HMXRB?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 8sig. Best fit spectrum is for apec with kT = 2.44keV. High nH above 10^23. Compare prev XMM obs. Spectral changes? CLAXBOI XRB. Potential higher flux in other XMM GP observation. Luminosity at 8kpc of order 10e34. High nH possible HMXRB?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined XMM spectral fit. Pulsation search?</t>
   </si>
   <si>
     <t xml:space="preserve">Good Gaia/2MASS association within 1sig. Best fit spectrum is for powerlaw with index 1. Lx at distance of ~1kpc is 2.5e31 erg/s. Ariadne – Lbol 0.95Lsun, log(Lx/Lbol) -2.2</t>
@@ -391,19 +361,16 @@
     <t xml:space="preserve">SWIFT XRB association.</t>
   </si>
   <si>
-    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s. No CLAXBOI. No MUWCLASS. Look at short-term Chandra var – EQ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Examine products from other XMM obs.</t>
+    <t xml:space="preserve">CO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clear GAIA/2MASS counterpart. Best fit spectrum is powerlaw with index 2.1. No distance estiamte, but luminosity at gal centre (8kpc) would be Lx 9.2e32 erg/s. No CLAXBOI. No MUWCLASS. Look at short-term Chandra var – EQ. Other XMM GP obs shows similar flux, no features in lc and spectra best fit as powerlaw index ~0. Fx/Fopt consistently above 1.</t>
   </si>
   <si>
     <t xml:space="preserve">GAIA/2MASS/SIMBAD association with star HD 314680B. Best fit spectrum is for 2 apec model, with kT1 = 0.1keV and kT2 = 0.34 or 5.9keV across two obs. NH matches HI4PI in both cases. Lx ~1e30 roughly at 250pc. No ARIADNE association in cat. No GAIA associated luminosity estimate. No periodicity in lightcurves.</t>
   </si>
   <si>
-    <t xml:space="preserve">Strong 2MASS association but no GAIA, and no visible optical source. SIMBAD association IRAS 1747-2648 at 4”. Best fit spec (albeit poor quality) is for power law and bbody with index -1.5, kT 0.78keV and emission line at 6.7keV. Lx at 8kpc is 3.6e33 erg/s. Very variable hard energy. No periodicity detectable in lightcurves. CLAXBOI XRB. MUWCLASS – Giant Star.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check other XMM/Chandra obs.</t>
+    <t xml:space="preserve">Strong 2MASS association but no GAIA, and no visible optical source. SIMBAD association IRAS 1747-2648 at 4”. Best fit spec (albeit poor quality) is for power law and bbody with index 1.5, kT 0.78keV and emission line at 6.7keV. Lx at 8kpc is 3.6e33 erg/s. Very variable hard energy. No periodicity detectable in lightcurves. CLAXBOI XRB. MUWCLASS – Giant Star. Previous XMM obs best fit by bbody with kt 1.6keV and high nH above 10^23. Lcs show lots of short-term variability. Flux variability just with XMM obs is of order 10.</t>
   </si>
   <si>
     <t xml:space="preserve">GAIA/2MASS/AllWISE source within 1sig. SIMBAD association to SWIFt source at 6”. Poor spectra (MOS only) and best fit is for power law with index 3.6. Lx at distance to optical source is 1.8e31 erg/s. Ariadne – Lbol 11.2Lsun, log(Lx/Lbol) -3.4</t>
@@ -412,7 +379,10 @@
     <t xml:space="preserve">No GAIA/2MASS/AllWISE source within 12sig. Best fit spectrum is for bbody kT = 1.1keV. No distance estimate, but Lx 3.6e33 erg/s at 8kpc. No CLAXBOI. No MUWCLASS.</t>
   </si>
   <si>
-    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Little information in lightcurve. Spectrum is low quality and best fits are apec and power law with kT = 5.9keV, or index of 1.5. No distance estimate, but at galactic centre Lx 1.4e33 erg/s. No CLAXBOI. No MUWCLASS</t>
+    <t xml:space="preserve">No Gaia/2MASS/AllWISE sources within 5sig. Little information in lightcurve. Spectrum is low quality and best fits are apec and power law with kT = 5.9keV, or index of 1.5. No distance estimate, but at galactic centre Lx 1.4e33 erg/s. No CLAXBOI. No MUWCLASS. Previous XMM obs has too few coutns to provide good spectral fits, but still has flux of order 2e-13. Fx/Fopt of order 10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simultaneous spectral fit?</t>
   </si>
   <si>
     <t xml:space="preserve">CV?</t>
@@ -442,16 +412,16 @@
     <t xml:space="preserve">Close association to Gaia/2MASS source. Lightcurve shows some variability. Best fit spectrum is for bbody/apec/ kT 0.7 or 1.9keV. Luminosity at distance of Gaia source Lx 1.9e32 erg/s. In region populated with several long period variable stars. Ariadne – Lbol 1466Lsun, log(Lx/Lbol) -4.5. No periodicity detectable in lightcurves.</t>
   </si>
   <si>
-    <t xml:space="preserve">SIMBAD association with 2MASS for YSO. LC shows one strong flare towards end of obs, but many bad time ints before. Best fit spec is for powerlaw with index 1.4. No distance estimate, but Lx at 8kpc is 2.9e33 erg/s. Not detected in two recent XMM obs. Flux limit 0886040201 – 9.4e-15. Check flare size/duration against YSOs. Not in MYStIX. No CLAXBOI</t>
+    <t xml:space="preserve">SIMBAD association with 2MASS for YSO. LC shows one strong flare towards end of obs, but many bad time ints before. Best fit spec is for powerlaw with index 1.4. No distance estimate, but Lx at 8kpc is 2.9e33 erg/s. Not detected in two recent XMM obs. Flux limit 0886040201 – 9.4e-15. Check flare size/duration against YSOs. Not in MYStIX. No CLAXBOI.</t>
   </si>
   <si>
     <t xml:space="preserve">Check flare against YSO/star.</t>
   </si>
   <si>
-    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Gaia/2MASS source association. Best fit spectrum is bbody with kT 1.3keV and Lx at Gaia source of 2.6e32 erg/s. No distinguishing features in lc. No CLAXBOI. No MUWCLASS. Not detected 0902780101, 0902780201, 0902780701.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check products from other XMM obs.</t>
+    <t xml:space="preserve">PN source location is affected by readout lines. MOS2 detection is used instead due to higher ML for source. Gaia/2MASS source association. Best fit spectrum is bbody with kT 1.3keV and Lx at Gaia source of 2.6e32 erg/s. No distinguishing features in lc. No CLAXBOI. No MUWCLASS. Not detected 0902780101, 0902780201, 0902780701. Det during 0902780501 on M2 has flux ~5x lower. Spec best fit by powerlaw index ~2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simultaneous fit to spec?</t>
   </si>
   <si>
     <t xml:space="preserve">No GAIA/2MASS source within 6sig. Small, but fast variability in lc at higher energy. Best fit spectrum is bbody kT = 0.38keV with an iron line at 6.4keV. Lx at 8kpc would be 1.4e33 erg/s. No periodicity detectable in lcs. CLAXBOI QSO. No MUWCLASS.</t>
@@ -485,7 +455,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -506,11 +476,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -599,7 +564,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -680,10 +645,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -708,8 +669,24 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -793,12 +770,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ80"/>
+  <dimension ref="A1:AMJ79"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M50" activeCellId="0" sqref="M50"/>
+      <selection pane="bottomLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -812,7 +789,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="98.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.52"/>
@@ -969,7 +946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -1598,7 +1575,7 @@
       <c r="L28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1772,29 +1749,29 @@
       </c>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="n">
+    <row r="35" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="20" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="21" t="n">
+      <c r="D35" s="20" t="n">
         <v>0.98</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="20" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="21" t="s">
+      <c r="J35" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="21" t="s">
+      <c r="K35" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="22" t="s">
+      <c r="L35" s="21" t="s">
         <v>71</v>
       </c>
       <c r="M35" s="6"/>
@@ -1853,7 +1830,7 @@
       <c r="L37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="M37" s="20" t="s">
+      <c r="M37" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1935,7 +1912,7 @@
       <c r="L40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="M40" s="20" t="s">
+      <c r="M40" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2024,32 +2001,32 @@
       <c r="M43" s="6"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="n">
+    <row r="44" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="22" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="21" t="n">
+      <c r="D44" s="20" t="n">
         <v>97</v>
       </c>
-      <c r="F44" s="21" t="s">
+      <c r="F44" s="20" t="s">
         <v>12</v>
       </c>
       <c r="G44" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K44" s="21" t="s">
+      <c r="J44" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="L44" s="22" t="s">
+      <c r="L44" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="M44" s="22" t="s">
+      <c r="M44" s="21" t="s">
         <v>83</v>
       </c>
       <c r="AMJ44" s="0"/>
@@ -2076,7 +2053,7 @@
       <c r="L45" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="M45" s="20" t="s">
+      <c r="M45" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2093,7 +2070,7 @@
       <c r="F46" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="24" t="s">
+      <c r="G46" s="23" t="s">
         <v>12</v>
       </c>
       <c r="J46" s="12" t="s">
@@ -2162,7 +2139,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="25" t="n">
+      <c r="A49" s="24" t="n">
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -2187,7 +2164,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="n">
         <v>44</v>
       </c>
@@ -2217,7 +2194,7 @@
       </c>
     </row>
     <row r="51" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="n">
+      <c r="A51" s="25" t="n">
         <v>45</v>
       </c>
       <c r="C51" s="14" t="s">
@@ -2299,7 +2276,7 @@
       <c r="AMJ53" s="0"/>
     </row>
     <row r="54" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="26" t="n">
+      <c r="A54" s="25" t="n">
         <v>48</v>
       </c>
       <c r="C54" s="14" t="s">
@@ -2326,101 +2303,101 @@
       <c r="M54" s="6"/>
       <c r="AMJ54" s="0"/>
     </row>
-    <row r="55" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="n">
         <v>49</v>
       </c>
       <c r="C55" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" s="15" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="M55" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AMJ55" s="0"/>
+    </row>
+    <row r="56" s="12" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="26" t="n">
+        <v>50</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="15" t="n">
-        <v>16.1</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J55" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="L55" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="M55" s="16" t="s">
+      <c r="D56" s="12" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L56" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="AMJ55" s="0"/>
-    </row>
-    <row r="56" s="12" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="12" t="n">
-        <v>50</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D56" s="12" t="n">
-        <v>0.649</v>
-      </c>
-      <c r="F56" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G56" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="13" t="s">
+      <c r="M56" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="M56" s="27" t="s">
+      <c r="AMJ56" s="28"/>
+    </row>
+    <row r="57" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="25" t="n">
+        <v>51</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="5" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K57" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="AMJ56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="26" t="n">
-        <v>51</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="1" t="n">
-        <v>2.95</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L57" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="M57" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="AMJ57" s="0"/>
     </row>
     <row r="58" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26" t="n">
-        <v>52</v>
+      <c r="A58" s="25" t="n">
+        <v>51.1</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D58" s="5" t="n">
-        <v>16.8</v>
+        <v>17.3</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>12</v>
@@ -2430,23 +2407,20 @@
       </c>
       <c r="J58" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="K58" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
       <c r="AMJ58" s="0"/>
     </row>
     <row r="59" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="26" t="n">
-        <v>52.1</v>
+      <c r="A59" s="25" t="n">
+        <v>51.2</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D59" s="5" t="n">
-        <v>17.3</v>
+        <v>24</v>
       </c>
       <c r="F59" s="14" t="s">
         <v>12</v>
@@ -2461,151 +2435,159 @@
       <c r="M59" s="6"/>
       <c r="AMJ59" s="0"/>
     </row>
-    <row r="60" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="26" t="n">
-        <v>52.2</v>
-      </c>
-      <c r="C60" s="14" t="s">
+    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="25" t="n">
+        <v>52</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>9.76</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L60" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M60" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="20" t="n">
+        <v>53</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="20" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="L61" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="M61" s="21"/>
+      <c r="AMJ61" s="0"/>
+    </row>
+    <row r="62" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="n">
+        <v>54</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="5" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L62" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M62" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AMJ62" s="0"/>
+    </row>
+    <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="n">
+        <v>56</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D60" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J60" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L60" s="6"/>
-      <c r="M60" s="6"/>
-      <c r="AMJ60" s="0"/>
-    </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="26" t="n">
-        <v>53</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>9.76</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L61" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="M61" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="21" t="n">
-        <v>54</v>
-      </c>
-      <c r="C62" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D62" s="21" t="n">
-        <v>2.43</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G62" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J62" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K62" s="21" t="s">
+      <c r="D64" s="5" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K64" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L62" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="M62" s="22"/>
-      <c r="AMJ62" s="0"/>
-    </row>
-    <row r="63" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="5" t="n">
-        <v>28.4</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K63" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="L63" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="M63" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AMJ63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="1" t="n">
-        <v>3.09</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L64" s="7" t="s">
+      <c r="L64" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="M64" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="65" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M64" s="6"/>
+      <c r="AMJ64" s="0"/>
+    </row>
+    <row r="65" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="n">
-        <v>57</v>
+        <v>56.1</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D65" s="5" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>12</v>
@@ -2619,93 +2601,95 @@
       <c r="K65" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L65" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="L65" s="6"/>
       <c r="M65" s="6"/>
       <c r="AMJ65" s="0"/>
     </row>
-    <row r="66" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
-        <v>57.1</v>
-      </c>
-      <c r="C66" s="5" t="s">
+    <row r="66" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>55.4</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L66" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="M66" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" s="20" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="20" t="n">
+        <v>58</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="5" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K66" s="5" t="s">
+      <c r="D67" s="20" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J67" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K67" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
-      <c r="AMJ66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67" s="1" t="n">
-        <v>55.4</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L67" s="7" t="s">
+      <c r="L67" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="M67" s="21"/>
+      <c r="AMJ67" s="0"/>
+    </row>
+    <row r="68" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15" t="n">
+        <v>59</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="15" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L68" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="M67" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="68" s="21" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="21" t="n">
-        <v>59</v>
-      </c>
-      <c r="C68" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" s="21" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="F68" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J68" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K68" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="L68" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="M68" s="22"/>
+      <c r="M68" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="AMJ68" s="0"/>
     </row>
-    <row r="69" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="12" t="n">
         <v>60</v>
       </c>
@@ -2713,72 +2697,78 @@
         <v>11</v>
       </c>
       <c r="D69" s="12" t="n">
-        <v>3.44</v>
+        <v>2.76</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G69" s="24" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="J69" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L69" s="13" t="s">
+      <c r="K69" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="L69" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="M69" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="AMJ69" s="28"/>
+    </row>
+    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="24" t="n">
+        <v>61</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="1" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K70" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="M69" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="AMJ69" s="0"/>
-    </row>
-    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D70" s="1" t="n">
-        <v>2.76</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="L70" s="7" t="s">
         <v>120</v>
       </c>
       <c r="M70" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="25" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="n">
         <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>3.08</v>
+        <v>2.45</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="L71" s="7" t="s">
         <v>122</v>
@@ -2787,64 +2777,63 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+    <row r="72" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="20" t="n">
         <v>63</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="20" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J72" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K72" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="L72" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="M72" s="21"/>
+      <c r="AMJ72" s="0"/>
+    </row>
+    <row r="73" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="n">
+        <v>64</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="1" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J72" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K72" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L72" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="M72" s="7" t="s">
+      <c r="D73" s="5" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L73" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="73" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="21" t="n">
-        <v>64</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" s="21" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="F73" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J73" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="K73" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="L73" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="M73" s="22"/>
+      <c r="M73" s="6"/>
       <c r="AMJ73" s="0"/>
     </row>
-    <row r="74" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="n">
         <v>65</v>
       </c>
@@ -2852,7 +2841,7 @@
         <v>11</v>
       </c>
       <c r="D74" s="5" t="n">
-        <v>3.76</v>
+        <v>2</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>12</v>
@@ -2861,13 +2850,13 @@
         <v>12</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>44</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M74" s="6"/>
       <c r="AMJ74" s="0"/>
@@ -2877,78 +2866,80 @@
         <v>66</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D75" s="5" t="n">
-        <v>2</v>
+        <v>4.17</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K75" s="5" t="s">
         <v>44</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M75" s="6"/>
       <c r="AMJ75" s="0"/>
     </row>
-    <row r="76" s="5" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="n">
         <v>67</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="D76" s="5" t="n">
-        <v>4.17</v>
+        <v>8.22</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="J76" s="5" t="s">
         <v>19</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="L76" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="M76" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="M76" s="6"/>
-      <c r="AMJ76" s="0"/>
+      <c r="AMJ76" s="30"/>
     </row>
     <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
         <v>68</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>8.22</v>
+        <v>2.07</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="L77" s="7" t="s">
         <v>130</v>
@@ -2965,16 +2956,19 @@
         <v>23</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>2.07</v>
+        <v>2.55</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="L78" s="7" t="s">
         <v>132</v>
@@ -2983,55 +2977,27 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+    <row r="79" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="12" t="n">
         <v>70</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" s="1" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K79" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L79" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="M79" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="C79" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D80" s="1" t="n">
+      <c r="D79" s="12" t="n">
         <v>4.88</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="F79" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G79" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AMJ79" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L79"/>
-  <conditionalFormatting sqref="D20:D79 D2:D18">
+  <conditionalFormatting sqref="D20:D78 D2:D18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3077,7 +3043,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="193.83"/>
   </cols>
@@ -3090,7 +3056,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,7 +3064,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,7 +3072,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3114,10 +3080,10 @@
         <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,7 +3091,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3141,7 +3107,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added new plots for STONKS GalPlane paper.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -14,8 +14,8 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$L$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'All Source Classification'!$A$1:$M$78</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'All Source Classification'!$A$1:$L$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'All Source Classification'!$A$1:$M$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'All Source Classification'!$A$1:$L$78</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -685,12 +685,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ79"/>
+  <dimension ref="A1:AMJ84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I78" activeCellId="0" sqref="I78"/>
+      <selection pane="bottomLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2880,6 +2880,30 @@
         <v>24</v>
       </c>
       <c r="AMJ79" s="15"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D81" s="1" t="n">
+        <f aca="false">MEDIAN(D2:D79)</f>
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D82" s="1" t="n">
+        <f aca="false">AVERAGE(D2:D79)</f>
+        <v>5.97818076923077</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D83" s="1" t="n">
+        <f aca="false">PERCENTILE(D2:D79,0.05)</f>
+        <v>0.2627</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D84" s="1" t="n">
+        <f aca="false">PERCENTILE(D2:D79,0.95)</f>
+        <v>24.66</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M79"/>
@@ -2929,7 +2953,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="193.83"/>
   </cols>

</xml_diff>

<commit_message>
Final update for source classifications.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -12,10 +12,10 @@
     <sheet name="Sources of Interest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$L$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'All Source Classification'!$A$1:$M$78</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'All Source Classification'!$A$1:$L$78</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$N$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'All Source Classification'!$A$1:$N$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'All Source Classification'!$A$1:$M$78</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">Combine PN and M2 data. Check Chandra obs.</t>
   </si>
   <si>
-    <t xml:space="preserve">No Gaia/2mass sources within 5sig. Lightcurve shows little variability. Spectrum best fit by powerlaw with index 0.9. No distance estimate, but Lx at 8kpc is 3.0e33 erg/s. No CLAXBOI. No MUWCLASS. Pulsations?</t>
+    <t xml:space="preserve">No Gaia/2mass sources within 5sig. Lightcurve shows little variability. Spectrum best fit by powerlaw with index 0.9. No distance estimate, but Lx at 8kpc is 3.0e33 erg/s. No CLAXBOI. No MUWCLASS. No periodicity.</t>
   </si>
   <si>
     <t xml:space="preserve">Try and combine MOS2 data with PN particularly for spectrum. Check Chandra obs. Pulsation search?</t>
@@ -447,8 +447,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -535,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -553,6 +555,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,11 +602,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,12 +691,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ84"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+      <selection pane="bottomLeft" activeCell="M52" activeCellId="0" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -699,17 +705,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="98.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="14" style="1" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="5.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="98.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,31 +730,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -760,22 +766,26 @@
       <c r="D2" s="1" t="n">
         <v>2.58</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
+      <c r="E2" s="5" t="n">
+        <f aca="false">LOG(D2*10^-12)</f>
+        <v>-11.5883802940368</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -789,19 +799,23 @@
       <c r="D3" s="1" t="n">
         <v>2.46</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
+      <c r="E3" s="5" t="n">
+        <f aca="false">LOG(D3*10^-12)</f>
+        <v>-11.6090648928966</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -815,22 +829,26 @@
       <c r="D4" s="1" t="n">
         <v>0.899</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
+      <c r="E4" s="5" t="n">
+        <f aca="false">LOG(D4*10^-12)</f>
+        <v>-12.0462403082668</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -844,19 +862,23 @@
       <c r="D5" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
+      <c r="E5" s="5" t="n">
+        <f aca="false">LOG(D5*10^-12)</f>
+        <v>-11.7958800173441</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -870,22 +892,26 @@
       <c r="D6" s="1" t="n">
         <v>4.57</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
+      <c r="E6" s="5" t="n">
+        <f aca="false">LOG(D6*10^-12)</f>
+        <v>-11.3400837999302</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>19</v>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -899,22 +925,26 @@
       <c r="D7" s="1" t="n">
         <v>2.08</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
+      <c r="E7" s="5" t="n">
+        <f aca="false">LOG(D7*10^-12)</f>
+        <v>-11.6819366650372</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>19</v>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="M7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="N7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -928,19 +958,23 @@
       <c r="D8" s="1" t="n">
         <v>2.35</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
+      <c r="E8" s="5" t="n">
+        <f aca="false">LOG(D8*10^-12)</f>
+        <v>-11.6289321377283</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="5" t="s">
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="5"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -952,19 +986,23 @@
       <c r="D9" s="1" t="n">
         <v>0.275</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="5" t="n">
+        <f aca="false">LOG(D9*10^-12)</f>
+        <v>-12.5606673061697</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -976,19 +1014,23 @@
       <c r="D10" s="1" t="n">
         <v>4.12</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
+      <c r="E10" s="5" t="n">
+        <f aca="false">LOG(D10*10^-12)</f>
+        <v>-11.3851027839669</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1002,22 +1044,26 @@
       <c r="D11" s="1" t="n">
         <v>1.85</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
+      <c r="E11" s="5" t="n">
+        <f aca="false">LOG(D11*10^-12)</f>
+        <v>-11.732828271597</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>19</v>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="5"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1029,22 +1075,26 @@
       <c r="D12" s="1" t="n">
         <v>1.54</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
+      <c r="E12" s="5" t="n">
+        <f aca="false">LOG(D12*10^-12)</f>
+        <v>-11.8124792791635</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1058,46 +1108,53 @@
       <c r="D13" s="1" t="n">
         <v>5.02</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>24</v>
+      <c r="E13" s="5" t="n">
+        <f aca="false">LOG(D13*10^-12)</f>
+        <v>-11.299296282855</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
         <v>10.2</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="7" t="n">
         <v>3.03</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="E14" s="5" t="n">
+        <f aca="false">LOG(D14*10^-12)</f>
+        <v>-11.5185573714977</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="L14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="AMJ14" s="0"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1109,22 +1166,26 @@
       <c r="D15" s="1" t="n">
         <v>2.2</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
+      <c r="E15" s="5" t="n">
+        <f aca="false">LOG(D15*10^-12)</f>
+        <v>-11.6575773191778</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="8" t="s">
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="M15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M15" s="5"/>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1136,22 +1197,26 @@
       <c r="D16" s="1" t="n">
         <v>0.431</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
+      <c r="E16" s="5" t="n">
+        <f aca="false">LOG(D16*10^-12)</f>
+        <v>-12.3655227298393</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>19</v>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M16" s="5"/>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1163,22 +1228,26 @@
       <c r="D17" s="1" t="n">
         <v>2.59</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
+      <c r="E17" s="5" t="n">
+        <f aca="false">LOG(D17*10^-12)</f>
+        <v>-11.5867002359187</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>19</v>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="5"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1190,22 +1259,26 @@
       <c r="D18" s="1" t="n">
         <v>1.18</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
+      <c r="E18" s="5" t="n">
+        <f aca="false">LOG(D18*10^-12)</f>
+        <v>-11.9281179926939</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>19</v>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="M18" s="5"/>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1217,22 +1290,26 @@
       <c r="D19" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
+      <c r="E19" s="5" t="n">
+        <f aca="false">LOG(D19*10^-12)</f>
+        <v>-11.8860566476932</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>19</v>
+      <c r="H19" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="N19" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1246,22 +1323,26 @@
       <c r="D20" s="1" t="n">
         <v>1.45</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
+      <c r="E20" s="5" t="n">
+        <f aca="false">LOG(D20*10^-12)</f>
+        <v>-11.838631997765</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>19</v>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="N20" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1275,22 +1356,26 @@
       <c r="D21" s="1" t="n">
         <v>0.833</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
+      <c r="E21" s="5" t="n">
+        <f aca="false">LOG(D21*10^-12)</f>
+        <v>-12.0793549985932</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>19</v>
+      <c r="H21" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="M21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M21" s="5"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1302,49 +1387,56 @@
       <c r="D22" s="1" t="n">
         <v>0.714</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>24</v>
+      <c r="E22" s="5" t="n">
+        <f aca="false">LOG(D22*10^-12)</f>
+        <v>-12.1463017882238</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="H22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="M22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="n">
-        <v>19</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="10" t="n">
         <v>1.43</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="9" t="s">
+      <c r="E23" s="5" t="n">
+        <f aca="false">LOG(D23*10^-12)</f>
+        <v>-11.8446639625349</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L23" s="10" t="s">
+      <c r="M23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="N23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1356,50 +1448,57 @@
       <c r="D24" s="1" t="n">
         <v>1.3</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>24</v>
+      <c r="E24" s="5" t="n">
+        <f aca="false">LOG(D24*10^-12)</f>
+        <v>-11.8860566476932</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>19</v>
+      <c r="H24" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="M24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="25" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="n">
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
         <v>20.1</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="6" t="n">
+      <c r="D25" s="7" t="n">
         <v>0.395</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="11" t="s">
+      <c r="E25" s="5" t="n">
+        <f aca="false">LOG(D25*10^-12)</f>
+        <v>-12.4034029043735</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="M25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="M25" s="12"/>
-      <c r="AMJ25" s="0"/>
+      <c r="N25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1411,22 +1510,26 @@
       <c r="D26" s="1" t="n">
         <v>1.37</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>24</v>
+      <c r="E26" s="5" t="n">
+        <f aca="false">LOG(D26*10^-12)</f>
+        <v>-11.8632794328436</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>19</v>
+      <c r="H26" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M26" s="5"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -1438,19 +1541,23 @@
       <c r="D27" s="1" t="n">
         <v>0.913</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>12</v>
+      <c r="E27" s="5" t="n">
+        <f aca="false">LOG(D27*10^-12)</f>
+        <v>-12.0395292224657</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="H27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="M27" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="N27" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1464,22 +1571,26 @@
       <c r="D28" s="1" t="n">
         <v>3.63</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>12</v>
+      <c r="E28" s="5" t="n">
+        <f aca="false">LOG(D28*10^-12)</f>
+        <v>-11.4400933749639</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="H28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M28" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="N28" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1493,22 +1604,26 @@
       <c r="D29" s="1" t="n">
         <v>0.0511</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>24</v>
+      <c r="E29" s="5" t="n">
+        <f aca="false">LOG(D29*10^-12)</f>
+        <v>-13.2915790998653</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>19</v>
+      <c r="H29" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="M29" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M29" s="5"/>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1520,22 +1635,26 @@
       <c r="D30" s="1" t="n">
         <v>3.31</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>12</v>
+      <c r="E30" s="5" t="n">
+        <f aca="false">LOG(D30*10^-12)</f>
+        <v>-11.4801720062243</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>19</v>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="M30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M30" s="5"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -1547,22 +1666,26 @@
       <c r="D31" s="1" t="n">
         <v>3.14</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>12</v>
+      <c r="E31" s="5" t="n">
+        <f aca="false">LOG(D31*10^-12)</f>
+        <v>-11.5030703519268</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>19</v>
+      <c r="H31" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="M31" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M31" s="5"/>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -1574,19 +1697,23 @@
       <c r="D32" s="1" t="n">
         <v>6.6</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>24</v>
+      <c r="E32" s="5" t="n">
+        <f aca="false">LOG(D32*10^-12)</f>
+        <v>-11.1804560644581</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="5" t="s">
+      <c r="H32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="N32" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1600,22 +1727,26 @@
       <c r="D33" s="1" t="n">
         <v>1.95</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
+      <c r="E33" s="5" t="n">
+        <f aca="false">LOG(D33*10^-12)</f>
+        <v>-11.7099653886375</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>19</v>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L33" s="5" t="s">
+      <c r="M33" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="N33" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1629,80 +1760,90 @@
       <c r="D34" s="1" t="n">
         <v>1.45</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>24</v>
+      <c r="E34" s="5" t="n">
+        <f aca="false">LOG(D34*10^-12)</f>
+        <v>-11.838631997765</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>19</v>
+      <c r="H34" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="M34" s="5" t="s">
+      <c r="N34" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="n">
+    <row r="35" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="9" t="n">
+      <c r="D35" s="10" t="n">
         <v>0.98</v>
       </c>
-      <c r="F35" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="9" t="s">
+      <c r="E35" s="5" t="n">
+        <f aca="false">LOG(D35*10^-12)</f>
+        <v>-12.0087739243075</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="L35" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="10" t="s">
+      <c r="M35" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="M35" s="5"/>
-      <c r="AMJ35" s="0"/>
-    </row>
-    <row r="36" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="n">
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D36" s="7" t="n">
         <v>0.182</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="6" t="s">
+      <c r="E36" s="5" t="n">
+        <f aca="false">LOG(D36*10^-12)</f>
+        <v>-12.7399286120149</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L36" s="12" t="s">
+      <c r="M36" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M36" s="12"/>
-      <c r="AMJ36" s="0"/>
+      <c r="N36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1714,22 +1855,26 @@
       <c r="D37" s="1" t="n">
         <v>3.35</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>24</v>
+      <c r="E37" s="5" t="n">
+        <f aca="false">LOG(D37*10^-12)</f>
+        <v>-11.4749551929632</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="H37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="M37" s="5" t="s">
+      <c r="N37" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1743,22 +1888,26 @@
       <c r="D38" s="1" t="n">
         <v>0.588</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
+      <c r="E38" s="5" t="n">
+        <f aca="false">LOG(D38*10^-12)</f>
+        <v>-12.2306226739239</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>19</v>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="M38" s="5"/>
+      <c r="N38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -1770,22 +1919,26 @@
       <c r="D39" s="1" t="n">
         <v>0.193</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>24</v>
+      <c r="E39" s="5" t="n">
+        <f aca="false">LOG(D39*10^-12)</f>
+        <v>-12.7144426909922</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>19</v>
+      <c r="H39" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="M39" s="5"/>
+      <c r="N39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -1797,19 +1950,23 @@
       <c r="D40" s="1" t="n">
         <v>2.86</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>24</v>
+      <c r="E40" s="5" t="n">
+        <f aca="false">LOG(D40*10^-12)</f>
+        <v>-11.543633966871</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="H40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L40" s="5" t="s">
+      <c r="M40" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="M40" s="5" t="s">
+      <c r="N40" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1823,22 +1980,26 @@
       <c r="D41" s="1" t="n">
         <v>0.935</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>24</v>
+      <c r="E41" s="5" t="n">
+        <f aca="false">LOG(D41*10^-12)</f>
+        <v>-12.0291883891275</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>19</v>
+      <c r="H41" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L41" s="5" t="s">
+      <c r="M41" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="M41" s="5"/>
+      <c r="N41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1850,22 +2011,26 @@
       <c r="D42" s="1" t="n">
         <v>1.15</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>24</v>
+      <c r="E42" s="5" t="n">
+        <f aca="false">LOG(D42*10^-12)</f>
+        <v>-11.9393021596464</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="H42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="L42" s="5" t="s">
+      <c r="M42" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="M42" s="5" t="s">
+      <c r="N42" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1879,52 +2044,59 @@
       <c r="D43" s="1" t="n">
         <v>1.69</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>24</v>
+      <c r="E43" s="5" t="n">
+        <f aca="false">LOG(D43*10^-12)</f>
+        <v>-11.7721132953863</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="H43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L43" s="5" t="s">
+      <c r="M43" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M43" s="5"/>
-    </row>
-    <row r="44" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="n">
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="9" t="n">
+      <c r="D44" s="10" t="n">
         <v>97</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K44" s="9" t="s">
+      <c r="E44" s="5" t="n">
+        <f aca="false">LOG(D44*10^-12)</f>
+        <v>-10.0132282657338</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="L44" s="10" t="s">
+      <c r="M44" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="M44" s="10" t="s">
+      <c r="N44" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="AMJ44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -1936,48 +2108,55 @@
       <c r="D45" s="1" t="n">
         <v>2.82</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>12</v>
+      <c r="E45" s="5" t="n">
+        <f aca="false">LOG(D45*10^-12)</f>
+        <v>-11.5497508916806</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="H45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L45" s="5" t="s">
+      <c r="M45" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="M45" s="5" t="s">
+      <c r="N45" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" s="6" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="n">
+    <row r="46" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="6" t="n">
+      <c r="D46" s="7" t="n">
         <v>2.95</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J46" s="6" t="s">
+      <c r="E46" s="5" t="n">
+        <f aca="false">LOG(D46*10^-12)</f>
+        <v>-11.5301779840218</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L46" s="7" t="s">
+      <c r="M46" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="M46" s="7" t="s">
+      <c r="N46" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AMJ46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
@@ -1989,22 +2168,26 @@
       <c r="D47" s="1" t="n">
         <v>7.22</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>12</v>
+      <c r="E47" s="5" t="n">
+        <f aca="false">LOG(D47*10^-12)</f>
+        <v>-11.1414628024304</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>19</v>
+      <c r="H47" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L47" s="5" t="s">
+      <c r="M47" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="M47" s="5"/>
+      <c r="N47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -2016,24 +2199,28 @@
       <c r="D48" s="1" t="n">
         <v>2.48</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>24</v>
+      <c r="E48" s="5" t="n">
+        <f aca="false">LOG(D48*10^-12)</f>
+        <v>-11.6055483191738</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L48" s="5" t="s">
+      <c r="H48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M48" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="N48" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8" t="n">
+      <c r="A49" s="9" t="n">
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -2042,19 +2229,23 @@
       <c r="D49" s="1" t="n">
         <v>0.294</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>12</v>
+      <c r="E49" s="5" t="n">
+        <f aca="false">LOG(D49*10^-12)</f>
+        <v>-12.5316526695878</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L49" s="5" t="s">
+      <c r="H49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="M49" s="5" t="s">
+      <c r="N49" s="6" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2068,78 +2259,88 @@
       <c r="D50" s="1" t="n">
         <v>0.102</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>24</v>
+      <c r="E50" s="5" t="n">
+        <f aca="false">LOG(D50*10^-12)</f>
+        <v>-12.9913998282381</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="H50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L50" s="5" t="s">
+      <c r="M50" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="M50" s="5" t="s">
+      <c r="N50" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="n">
+    <row r="51" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="15" t="n">
         <v>45</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>37.2</v>
       </c>
-      <c r="F51" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L51" s="5" t="s">
+      <c r="E51" s="5" t="n">
+        <f aca="false">LOG(D51*10^-12)</f>
+        <v>-10.4294570601181</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="M51" s="5" t="s">
+      <c r="N51" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AMJ51" s="0"/>
-    </row>
-    <row r="52" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
+    </row>
+    <row r="52" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="9" t="n">
+      <c r="D52" s="10" t="n">
         <v>2.93</v>
       </c>
-      <c r="F52" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J52" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" s="10" t="s">
+      <c r="E52" s="5" t="n">
+        <f aca="false">LOG(D52*10^-12)</f>
+        <v>-11.5331323796459</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M52" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="M52" s="10" t="s">
+      <c r="N52" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AMJ52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -2151,185 +2352,207 @@
       <c r="D53" s="1" t="n">
         <v>0.504</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>12</v>
+      <c r="E53" s="5" t="n">
+        <f aca="false">LOG(D53*10^-12)</f>
+        <v>-12.2975694635545</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>19</v>
+      <c r="H53" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L53" s="5" t="s">
+      <c r="M53" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="M53" s="5"/>
-    </row>
-    <row r="54" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="n">
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="n">
         <v>48</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>23.8</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J54" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K54" s="8" t="s">
+      <c r="E54" s="5" t="n">
+        <f aca="false">LOG(D54*10^-12)</f>
+        <v>-10.6234230429435</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L54" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="L54" s="5" t="s">
+      <c r="M54" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="M54" s="5"/>
-      <c r="AMJ54" s="0"/>
-    </row>
-    <row r="55" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="n">
+      <c r="N54" s="6"/>
+    </row>
+    <row r="55" s="10" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D55" s="9" t="n">
+      <c r="D55" s="10" t="n">
         <v>0.649</v>
       </c>
-      <c r="F55" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K55" s="9" t="s">
+      <c r="E55" s="5" t="n">
+        <f aca="false">LOG(D55*10^-12)</f>
+        <v>-12.1877553031996</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L55" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="10" t="s">
+      <c r="M55" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="M55" s="10" t="s">
+      <c r="N55" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="AMJ55" s="0"/>
-    </row>
-    <row r="56" s="6" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="n">
+    </row>
+    <row r="56" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="12" t="n">
         <v>50</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="6" t="n">
+      <c r="D56" s="7" t="n">
         <v>2.95</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K56" s="6" t="s">
+      <c r="E56" s="5" t="n">
+        <f aca="false">LOG(D56*10^-12)</f>
+        <v>-11.5301779840218</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L56" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="L56" s="12" t="s">
+      <c r="M56" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="M56" s="12" t="s">
+      <c r="N56" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AMJ56" s="15"/>
-    </row>
-    <row r="57" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="n">
+    </row>
+    <row r="57" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="n">
         <v>51</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>16.8</v>
       </c>
-      <c r="F57" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J57" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K57" s="8" t="s">
+      <c r="E57" s="5" t="n">
+        <f aca="false">LOG(D57*10^-12)</f>
+        <v>-10.7746907182741</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="AMJ57" s="0"/>
-    </row>
-    <row r="58" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8" t="n">
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9" t="n">
         <v>51.1</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>17.3</v>
       </c>
-      <c r="F58" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="AMJ58" s="0"/>
-    </row>
-    <row r="59" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8" t="n">
+      <c r="E58" s="5" t="n">
+        <f aca="false">LOG(D58*10^-12)</f>
+        <v>-10.7619538968712</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+    </row>
+    <row r="59" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="9" t="n">
         <v>51.2</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="F59" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J59" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="AMJ59" s="0"/>
+      <c r="E59" s="5" t="n">
+        <f aca="false">LOG(D59*10^-12)</f>
+        <v>-10.6197887582884</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K59" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8" t="n">
+      <c r="A60" s="9" t="n">
         <v>52</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -2338,52 +2561,59 @@
       <c r="D60" s="1" t="n">
         <v>9.76</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
+      <c r="E60" s="5" t="n">
+        <f aca="false">LOG(D60*10^-12)</f>
+        <v>-11.0105501823333</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>19</v>
+      <c r="H60" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L60" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="L60" s="5" t="s">
+      <c r="M60" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="M60" s="5" t="s">
+      <c r="N60" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9" t="n">
+    <row r="61" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="9" t="n">
+      <c r="D61" s="10" t="n">
         <v>2.43</v>
       </c>
-      <c r="F61" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J61" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K61" s="9" t="s">
+      <c r="E61" s="5" t="n">
+        <f aca="false">LOG(D61*10^-12)</f>
+        <v>-11.6143937264017</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L61" s="10" t="s">
+      <c r="M61" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="M61" s="10"/>
-      <c r="AMJ61" s="0"/>
+      <c r="N61" s="11"/>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -2395,22 +2625,26 @@
       <c r="D62" s="1" t="n">
         <v>28.4</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>12</v>
+      <c r="E62" s="5" t="n">
+        <f aca="false">LOG(D62*10^-12)</f>
+        <v>-10.546681659953</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>19</v>
+      <c r="H62" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L62" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L62" s="5" t="s">
+      <c r="M62" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="M62" s="5" t="s">
+      <c r="N62" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2424,22 +2658,26 @@
       <c r="D63" s="1" t="n">
         <v>3.09</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>12</v>
+      <c r="E63" s="5" t="n">
+        <f aca="false">LOG(D63*10^-12)</f>
+        <v>-11.5100415205752</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>19</v>
+      <c r="H63" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="L63" s="5" t="s">
+      <c r="M63" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="M63" s="5" t="s">
+      <c r="N63" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2453,22 +2691,26 @@
       <c r="D64" s="1" t="n">
         <v>1.42</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>12</v>
+      <c r="E64" s="5" t="n">
+        <f aca="false">LOG(D64*10^-12)</f>
+        <v>-11.8477116556169</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>19</v>
+      <c r="H64" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L64" s="5" t="s">
+      <c r="M64" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="M64" s="5"/>
+      <c r="N64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
@@ -2480,20 +2722,24 @@
       <c r="D65" s="1" t="n">
         <v>1.43</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>12</v>
+      <c r="E65" s="5" t="n">
+        <f aca="false">LOG(D65*10^-12)</f>
+        <v>-11.8446639625349</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J65" s="1" t="s">
-        <v>19</v>
+      <c r="H65" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L65" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -2505,112 +2751,125 @@
       <c r="D66" s="1" t="n">
         <v>55.4</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>12</v>
+      <c r="E66" s="5" t="n">
+        <f aca="false">LOG(D66*10^-12)</f>
+        <v>-10.2564902352716</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="H66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K66" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="L66" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="L66" s="5" t="s">
+      <c r="M66" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="M66" s="5" t="s">
+      <c r="N66" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9" t="n">
+    <row r="67" s="10" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D67" s="9" t="n">
+      <c r="D67" s="10" t="n">
         <v>4.13</v>
       </c>
-      <c r="F67" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J67" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K67" s="9" t="s">
+      <c r="E67" s="5" t="n">
+        <f aca="false">LOG(D67*10^-12)</f>
+        <v>-11.3840499483436</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L67" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L67" s="10" t="s">
+      <c r="M67" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="M67" s="10"/>
-      <c r="AMJ67" s="0"/>
-    </row>
-    <row r="68" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="9" t="n">
+      <c r="N67" s="11"/>
+    </row>
+    <row r="68" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="9" t="n">
+      <c r="D68" s="10" t="n">
         <v>3.44</v>
       </c>
-      <c r="F68" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J68" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L68" s="10" t="s">
+      <c r="E68" s="5" t="n">
+        <f aca="false">LOG(D68*10^-12)</f>
+        <v>-11.4634415574285</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K68" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M68" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="M68" s="10" t="s">
+      <c r="N68" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AMJ68" s="0"/>
-    </row>
-    <row r="69" s="6" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="n">
+    </row>
+    <row r="69" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="6" t="n">
+      <c r="D69" s="7" t="n">
         <v>2.76</v>
       </c>
-      <c r="F69" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K69" s="6" t="s">
+      <c r="E69" s="5" t="n">
+        <f aca="false">LOG(D69*10^-12)</f>
+        <v>-11.5590909179348</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K69" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L69" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="L69" s="12" t="s">
+      <c r="M69" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="M69" s="12" t="s">
+      <c r="N69" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="AMJ69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="n">
+      <c r="A70" s="9" t="n">
         <v>61</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2619,22 +2878,26 @@
       <c r="D70" s="1" t="n">
         <v>3.08</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>12</v>
+      <c r="E70" s="5" t="n">
+        <f aca="false">LOG(D70*10^-12)</f>
+        <v>-11.5114492834996</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J70" s="1" t="s">
-        <v>19</v>
+      <c r="H70" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L70" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L70" s="5" t="s">
+      <c r="M70" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="M70" s="5" t="s">
+      <c r="N70" s="6" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2648,52 +2911,59 @@
       <c r="D71" s="1" t="n">
         <v>2.45</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>24</v>
+      <c r="E71" s="5" t="n">
+        <f aca="false">LOG(D71*10^-12)</f>
+        <v>-11.6108339156355</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>19</v>
+      <c r="H71" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L71" s="5" t="s">
+      <c r="M71" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="M71" s="5" t="s">
+      <c r="N71" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="72" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="9" t="n">
+    <row r="72" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="10" t="n">
         <v>63</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D72" s="9" t="n">
+      <c r="D72" s="10" t="n">
         <v>1.32</v>
       </c>
-      <c r="F72" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J72" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K72" s="9" t="s">
+      <c r="E72" s="5" t="n">
+        <f aca="false">LOG(D72*10^-12)</f>
+        <v>-11.8794260687942</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K72" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L72" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L72" s="10" t="s">
+      <c r="M72" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="M72" s="10"/>
-      <c r="AMJ72" s="0"/>
+      <c r="N72" s="11"/>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -2705,22 +2975,26 @@
       <c r="D73" s="1" t="n">
         <v>3.76</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>12</v>
+      <c r="E73" s="5" t="n">
+        <f aca="false">LOG(D73*10^-12)</f>
+        <v>-11.4248121550723</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J73" s="1" t="s">
-        <v>19</v>
+      <c r="H73" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L73" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L73" s="5" t="s">
+      <c r="M73" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="M73" s="5"/>
+      <c r="N73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
@@ -2732,22 +3006,26 @@
       <c r="D74" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>12</v>
+      <c r="E74" s="5" t="n">
+        <f aca="false">LOG(D74*10^-12)</f>
+        <v>-11.698970004336</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="H74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="L74" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L74" s="5" t="s">
+      <c r="M74" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="M74" s="5"/>
+      <c r="N74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
@@ -2759,22 +3037,26 @@
       <c r="D75" s="1" t="n">
         <v>4.17</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>24</v>
+      <c r="E75" s="5" t="n">
+        <f aca="false">LOG(D75*10^-12)</f>
+        <v>-11.3798639450262</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>19</v>
+      <c r="H75" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L75" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L75" s="5" t="s">
+      <c r="M75" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="M75" s="5"/>
+      <c r="N75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -2786,22 +3068,26 @@
       <c r="D76" s="1" t="n">
         <v>8.22</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>12</v>
+      <c r="E76" s="5" t="n">
+        <f aca="false">LOG(D76*10^-12)</f>
+        <v>-11.08512818246</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>19</v>
+      <c r="H76" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="K76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L76" s="5" t="s">
+      <c r="M76" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="M76" s="5" t="s">
+      <c r="N76" s="6" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2815,22 +3101,26 @@
       <c r="D77" s="1" t="n">
         <v>2.07</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>24</v>
+      <c r="E77" s="5" t="n">
+        <f aca="false">LOG(D77*10^-12)</f>
+        <v>-11.6840296545431</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>19</v>
+      <c r="H77" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L77" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L77" s="5" t="s">
+      <c r="M77" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="M77" s="5" t="s">
+      <c r="N77" s="6" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2844,42 +3134,49 @@
       <c r="D78" s="1" t="n">
         <v>2.55</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>12</v>
+      <c r="E78" s="5" t="n">
+        <f aca="false">LOG(D78*10^-12)</f>
+        <v>-11.593459819566</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J78" s="1" t="s">
+      <c r="H78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K78" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K78" s="1" t="s">
+      <c r="L78" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="L78" s="5" t="s">
+      <c r="M78" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="M78" s="5" t="s">
+      <c r="N78" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="79" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6" t="n">
+    <row r="79" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D79" s="6" t="n">
+      <c r="D79" s="7" t="n">
         <v>4.88</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AMJ79" s="15"/>
+      <c r="E79" s="5" t="n">
+        <f aca="false">LOG(D79*10^-12)</f>
+        <v>-11.3115801779973</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D81" s="1" t="n">
@@ -2888,9 +3185,9 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="1" t="n">
-        <f aca="false">AVERAGE(D2:D79)</f>
-        <v>5.97818076923077</v>
+      <c r="D82" s="17" t="n">
+        <f aca="false">(10^12)*10^AVERAGE(E2:E79)</f>
+        <v>2.23479814551686</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,7 +3203,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M79"/>
+  <autoFilter ref="A1:N79"/>
   <conditionalFormatting sqref="D20:D78 D2:D18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2921,6 +3218,942 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
     <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E60">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E74">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E75">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E76">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E77">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E78">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E79">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2953,7 +4186,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="193.83"/>
   </cols>

</xml_diff>

<commit_message>
Update for Vizier tables.
</commit_message>
<xml_diff>
--- a/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
+++ b/alert_docs/GalPlane/Tracking-Source_Analysis.xlsx
@@ -12,8 +12,8 @@
     <sheet name="Sources of Interest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$N$79</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$M$79</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'All Source Classification'!$A$1:$N$79</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'All Source Classification'!$A$1:$N$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'All Source Classification'!$A$1:$M$78</definedName>
   </definedNames>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="140">
   <si>
     <t xml:space="preserve">Src No.</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t xml:space="preserve">Future actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance Est?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log(F)</t>
   </si>
   <si>
     <t xml:space="preserve">FD</t>
@@ -537,7 +543,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,6 +570,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -691,12 +701,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N84"/>
+  <dimension ref="A1:AA84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M52" activeCellId="0" sqref="M52"/>
+      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -715,7 +727,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="98.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.96"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,13 +769,19 @@
       <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>2.58</v>
@@ -771,22 +791,49 @@
         <v>-11.5883802940368</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="7" t="n">
+        <f aca="false">LOG10(D2)-13</f>
+        <v>-12.5883802940368</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <f aca="false">AVERAGE(Q2:Q8,Q10,Q19:Q20,Q22:Q23,Q26:Q28,Q32:Q34,Q37,Q40,Q42:Q43,Q45,Q50:Q51,Q54,Q60,Q62:Q63,Q66,Q68:Q71,Q76,Q78)</f>
+        <v>-12.5370675969184</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <f aca="false">STDEV(Q2:Q8,Q10,Q19:Q20,Q22:Q23,Q26:Q28,Q32:Q34,Q37,Q40,Q42:Q43,Q45,Q50:Q51,Q54,Q60,Q62:Q63,Q66,Q68:Q71,Q76,Q78)</f>
+        <v>0.513699338790906</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <f aca="false">MEDIAN(Q2:Q8,Q10,Q19:Q20,Q22:Q23,Q26:Q28,Q32:Q34,Q37,Q40,Q42:Q43,Q45,Q50:Q51,Q54,Q60,Q62:Q63,Q66,Q68:Q71,Q76,Q78)</f>
+        <v>-12.5909200568014</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <f aca="false">10^S2</f>
+        <v>2.90357068531842E-013</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <f aca="false">10^V2</f>
+        <v>2.56495613997589E-013</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2.46</v>
@@ -804,19 +851,46 @@
         <v>-11.6090648928966</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <f aca="false">LOG10(D3)-13</f>
+        <v>-12.6090648928966</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <f aca="false">AVERAGE(Q9,Q11:Q18,Q21,Q24:Q25,Q29:Q31,Q35:Q36,Q38:Q39,Q41,Q44,Q46:Q49,Q52:Q53,Q55:Q59,Q61,Q64:Q65,Q67,Q72:Q75,Q77,Q79)</f>
+        <v>-12.7482137840815</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <f aca="false">STDEV(Q9,Q11:Q18,Q21,Q24:Q25,Q29:Q31,Q35:Q36,Q38:Q39,Q41,Q44,Q46:Q49,Q52:Q53,Q55:Q59,Q61,Q64:Q65,Q67,Q72:Q75,Q77,Q79)</f>
+        <v>0.608916211683277</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <f aca="false">MEDIAN(Q9,Q11:Q18,Q21,Q24:Q25,Q29:Q31,Q35:Q36,Q38:Q39,Q41,Q44,Q46:Q49,Q52:Q53,Q55:Q59,Q61,Q64:Q65,Q67,Q72:Q75,Q77,Q79)</f>
+        <v>-12.6914998294396</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <f aca="false">10^S3</f>
+        <v>1.78560838196605E-013</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <f aca="false">10^V3</f>
+        <v>2.03469899493758E-013</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,7 +898,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.899</v>
@@ -834,22 +908,29 @@
         <v>-12.0462403082668</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <f aca="false">LOG10(D4)-13</f>
+        <v>-13.0462403082668</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,7 +938,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1.6</v>
@@ -867,19 +948,38 @@
         <v>-11.7958800173441</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="7" t="n">
+        <f aca="false">LOG10(D5)-13</f>
+        <v>-12.7958800173441</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <f aca="false">AVERAGE(Q2:Q79)</f>
+        <v>-12.6507616976985</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <f aca="false">STDEV(Q2:Q79)</f>
+        <v>0.573236439197705</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <f aca="false">MEDIAN(Q2:Q79)</f>
+        <v>-12.6126138210186</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>4.57</v>
@@ -897,22 +997,29 @@
         <v>-11.3400837999302</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <f aca="false">LOG10(D6)-13</f>
+        <v>-12.3400837999302</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,7 +1027,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2.08</v>
@@ -930,22 +1037,29 @@
         <v>-11.6819366650372</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <f aca="false">LOG10(D7)-13</f>
+        <v>-12.6819366650372</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +1067,7 @@
         <v>6.1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>2.35</v>
@@ -963,25 +1077,32 @@
         <v>-11.6289321377283</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N8" s="6"/>
+      <c r="P8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="7" t="n">
+        <f aca="false">LOG10(D8)-13</f>
+        <v>-12.6289321377283</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0.275</v>
@@ -991,25 +1112,32 @@
         <v>-12.5606673061697</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N9" s="6"/>
+      <c r="P9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <f aca="false">LOG10(D9)-13</f>
+        <v>-13.5606673061697</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>4.12</v>
@@ -1019,19 +1147,26 @@
         <v>-11.3851027839669</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <f aca="false">LOG10(D10)-13</f>
+        <v>-12.3851027839669</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1174,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1.85</v>
@@ -1049,28 +1184,35 @@
         <v>-11.732828271597</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N11" s="6"/>
+      <c r="P11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="7" t="n">
+        <f aca="false">LOG10(D11)-13</f>
+        <v>-12.732828271597</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1.54</v>
@@ -1080,22 +1222,29 @@
         <v>-11.8124792791635</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="7" t="n">
+        <f aca="false">LOG10(D12)-13</f>
+        <v>-12.8124792791635</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1252,7 @@
         <v>10.1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>5.02</v>
@@ -1113,28 +1262,35 @@
         <v>-11.299296282855</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
+      <c r="P13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q13" s="7" t="n">
+        <f aca="false">LOG10(D13)-13</f>
+        <v>-12.299296282855</v>
+      </c>
     </row>
     <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="n">
         <v>10.2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="n">
         <v>3.03</v>
       </c>
       <c r="E14" s="5" t="n">
@@ -1142,26 +1298,33 @@
         <v>-11.5185573714977</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="P14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="7" t="n">
+        <f aca="false">LOG10(D14)-13</f>
+        <v>-12.5185573714977</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>2.2</v>
@@ -1171,28 +1334,35 @@
         <v>-11.6575773191778</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>42</v>
+        <v>21</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N15" s="6"/>
+      <c r="P15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="7" t="n">
+        <f aca="false">LOG10(D15)-13</f>
+        <v>-12.6575773191778</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0.431</v>
@@ -1202,28 +1372,35 @@
         <v>-12.3655227298393</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N16" s="6"/>
+      <c r="P16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="7" t="n">
+        <f aca="false">LOG10(D16)-13</f>
+        <v>-13.3655227298393</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>2.59</v>
@@ -1233,28 +1410,35 @@
         <v>-11.5867002359187</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N17" s="6"/>
+      <c r="P17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="7" t="n">
+        <f aca="false">LOG10(D17)-13</f>
+        <v>-12.5867002359187</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1.18</v>
@@ -1264,28 +1448,35 @@
         <v>-11.9281179926939</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N18" s="6"/>
+      <c r="P18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="7" t="n">
+        <f aca="false">LOG10(D18)-13</f>
+        <v>-12.9281179926939</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>1.3</v>
@@ -1295,22 +1486,29 @@
         <v>-11.8860566476932</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="7" t="n">
+        <f aca="false">LOG10(D19)-13</f>
+        <v>-12.8860566476932</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,7 +1516,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1.45</v>
@@ -1328,22 +1526,29 @@
         <v>-11.838631997765</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="7" t="n">
+        <f aca="false">LOG10(D20)-13</f>
+        <v>-12.838631997765</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,7 +1556,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0.833</v>
@@ -1361,28 +1566,35 @@
         <v>-12.0793549985932</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N21" s="6"/>
+      <c r="P21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="7" t="n">
+        <f aca="false">LOG10(D21)-13</f>
+        <v>-13.0793549985932</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0.714</v>
@@ -1392,50 +1604,64 @@
         <v>-12.1463017882238</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N22" s="6"/>
-    </row>
-    <row r="23" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="n">
+      <c r="P22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="7" t="n">
+        <f aca="false">LOG10(D22)-13</f>
+        <v>-13.1463017882238</v>
+      </c>
+    </row>
+    <row r="23" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="10" t="n">
+      <c r="C23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="11" t="n">
         <v>1.43</v>
       </c>
       <c r="E23" s="5" t="n">
         <f aca="false">LOG(D23*10^-12)</f>
         <v>-11.8446639625349</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>12</v>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="M23" s="11" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="7" t="n">
+        <f aca="false">LOG10(D23)-13</f>
+        <v>-12.8446639625349</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,7 +1669,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1.3</v>
@@ -1453,30 +1679,37 @@
         <v>-11.8860566476932</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N24" s="6"/>
+      <c r="P24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="7" t="n">
+        <f aca="false">LOG10(D24)-13</f>
+        <v>-12.8860566476932</v>
+      </c>
     </row>
     <row r="25" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="n">
         <v>20.1</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="7" t="n">
+        <v>33</v>
+      </c>
+      <c r="D25" s="8" t="n">
         <v>0.395</v>
       </c>
       <c r="E25" s="5" t="n">
@@ -1484,28 +1717,35 @@
         <v>-12.4034029043735</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="M25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="N25" s="13"/>
+      <c r="M25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" s="14"/>
+      <c r="P25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="7" t="n">
+        <f aca="false">LOG10(D25)-13</f>
+        <v>-13.4034029043735</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1.37</v>
@@ -1515,28 +1755,35 @@
         <v>-11.8632794328436</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N26" s="6"/>
+      <c r="P26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="7" t="n">
+        <f aca="false">LOG10(D26)-13</f>
+        <v>-12.8632794328436</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0.913</v>
@@ -1546,19 +1793,26 @@
         <v>-12.0395292224657</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q27" s="7" t="n">
+        <f aca="false">LOG10(D27)-13</f>
+        <v>-13.0395292224657</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,7 +1820,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>3.63</v>
@@ -1576,22 +1830,29 @@
         <v>-11.4400933749639</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q28" s="7" t="n">
+        <f aca="false">LOG10(D28)-13</f>
+        <v>-12.4400933749639</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,7 +1860,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>0.0511</v>
@@ -1609,28 +1870,35 @@
         <v>-13.2915790998653</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N29" s="6"/>
+      <c r="P29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="7" t="n">
+        <f aca="false">LOG10(D29)-13</f>
+        <v>-14.2915790998653</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>25</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>3.31</v>
@@ -1640,28 +1908,35 @@
         <v>-11.4801720062243</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N30" s="6"/>
+      <c r="P30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="7" t="n">
+        <f aca="false">LOG10(D30)-13</f>
+        <v>-12.4801720062243</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>25.1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>3.14</v>
@@ -1671,28 +1946,35 @@
         <v>-11.5030703519268</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N31" s="6"/>
+      <c r="P31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q31" s="7" t="n">
+        <f aca="false">LOG10(D31)-13</f>
+        <v>-12.5030703519268</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>6.6</v>
@@ -1702,19 +1984,26 @@
         <v>-11.1804560644581</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q32" s="7" t="n">
+        <f aca="false">LOG10(D32)-13</f>
+        <v>-12.1804560644581</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,7 +2011,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>1.95</v>
@@ -1732,22 +2021,29 @@
         <v>-11.7099653886375</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q33" s="7" t="n">
+        <f aca="false">LOG10(D33)-13</f>
+        <v>-12.7099653886375</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,7 +2051,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>1.45</v>
@@ -1765,63 +2061,77 @@
         <v>-11.838631997765</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="7" t="n">
+        <f aca="false">LOG10(D34)-13</f>
+        <v>-12.838631997765</v>
+      </c>
+    </row>
+    <row r="35" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11" t="n">
         <v>29</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="10" t="n">
+      <c r="C35" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="11" t="n">
         <v>0.98</v>
       </c>
       <c r="E35" s="5" t="n">
         <f aca="false">LOG(D35*10^-12)</f>
         <v>-12.0087739243075</v>
       </c>
-      <c r="G35" s="10" t="s">
-        <v>12</v>
+      <c r="G35" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L35" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M35" s="11" t="s">
-        <v>69</v>
+        <v>14</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="N35" s="6"/>
+      <c r="P35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q35" s="7" t="n">
+        <f aca="false">LOG10(D35)-13</f>
+        <v>-13.0087739243075</v>
+      </c>
     </row>
     <row r="36" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="n">
         <v>30</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="7" t="n">
+        <v>33</v>
+      </c>
+      <c r="D36" s="8" t="n">
         <v>0.182</v>
       </c>
       <c r="E36" s="5" t="n">
@@ -1829,28 +2139,35 @@
         <v>-12.7399286120149</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M36" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="N36" s="13"/>
+        <v>44</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N36" s="14"/>
+      <c r="P36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="7" t="n">
+        <f aca="false">LOG10(D36)-13</f>
+        <v>-13.7399286120149</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
         <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>3.35</v>
@@ -1860,22 +2177,29 @@
         <v>-11.4749551929632</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q37" s="7" t="n">
+        <f aca="false">LOG10(D37)-13</f>
+        <v>-12.4749551929632</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,7 +2207,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>0.588</v>
@@ -1893,28 +2217,35 @@
         <v>-12.2306226739239</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N38" s="6"/>
+      <c r="P38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q38" s="7" t="n">
+        <f aca="false">LOG10(D38)-13</f>
+        <v>-13.2306226739239</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>0.193</v>
@@ -1924,28 +2255,35 @@
         <v>-12.7144426909922</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N39" s="6"/>
+      <c r="P39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q39" s="7" t="n">
+        <f aca="false">LOG10(D39)-13</f>
+        <v>-13.7144426909922</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>34</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>2.86</v>
@@ -1955,19 +2293,26 @@
         <v>-11.543633966871</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q40" s="7" t="n">
+        <f aca="false">LOG10(D40)-13</f>
+        <v>-12.543633966871</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1975,7 +2320,7 @@
         <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>0.935</v>
@@ -1985,28 +2330,35 @@
         <v>-12.0291883891275</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N41" s="6"/>
+      <c r="P41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q41" s="7" t="n">
+        <f aca="false">LOG10(D41)-13</f>
+        <v>-13.0291883891275</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>36</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>1.15</v>
@@ -2016,22 +2368,29 @@
         <v>-11.9393021596464</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q42" s="7" t="n">
+        <f aca="false">LOG10(D42)-13</f>
+        <v>-12.9393021596464</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,7 +2398,7 @@
         <v>37</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>1.69</v>
@@ -2049,53 +2408,67 @@
         <v>-11.7721132953863</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N43" s="6"/>
-    </row>
-    <row r="44" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="n">
+      <c r="P43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q43" s="7" t="n">
+        <f aca="false">LOG10(D43)-13</f>
+        <v>-12.7721132953863</v>
+      </c>
+    </row>
+    <row r="44" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="15" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="10" t="n">
+      <c r="C44" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="11" t="n">
         <v>97</v>
       </c>
       <c r="E44" s="5" t="n">
         <f aca="false">LOG(D44*10^-12)</f>
         <v>-10.0132282657338</v>
       </c>
-      <c r="G44" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L44" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="M44" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="N44" s="11" t="s">
+      <c r="G44" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="11" t="s">
         <v>81</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="P44" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q44" s="7" t="n">
+        <f aca="false">LOG10(D44)-13</f>
+        <v>-11.0132282657338</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,7 +2476,7 @@
         <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>2.82</v>
@@ -2113,19 +2486,26 @@
         <v>-11.5497508916806</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q45" s="7" t="n">
+        <f aca="false">LOG10(D45)-13</f>
+        <v>-12.5497508916806</v>
       </c>
     </row>
     <row r="46" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,9 +2513,9 @@
         <v>40</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D46" s="8" t="n">
         <v>2.95</v>
       </c>
       <c r="E46" s="5" t="n">
@@ -2143,19 +2523,26 @@
         <v>-11.5301779840218</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="M46" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="N46" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="7" t="n">
+        <f aca="false">LOG10(D46)-13</f>
+        <v>-12.5301779840218</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,7 +2550,7 @@
         <v>41</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>7.22</v>
@@ -2173,28 +2560,35 @@
         <v>-11.1414628024304</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="N47" s="6"/>
+      <c r="P47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q47" s="7" t="n">
+        <f aca="false">LOG10(D47)-13</f>
+        <v>-12.1414628024304</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>42</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>2.48</v>
@@ -2204,27 +2598,34 @@
         <v>-11.6055483191738</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q48" s="7" t="n">
+        <f aca="false">LOG10(D48)-13</f>
+        <v>-12.6055483191738</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="n">
+      <c r="A49" s="10" t="n">
         <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>0.294</v>
@@ -2234,19 +2635,26 @@
         <v>-12.5316526695878</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q49" s="7" t="n">
+        <f aca="false">LOG10(D49)-13</f>
+        <v>-13.5316526695878</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,7 +2662,7 @@
         <v>44</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>0.102</v>
@@ -2264,30 +2672,37 @@
         <v>-12.9913998282381</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15" t="n">
+        <v>92</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q50" s="7" t="n">
+        <f aca="false">LOG10(D50)-13</f>
+        <v>-13.9913998282381</v>
+      </c>
+    </row>
+    <row r="51" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>23</v>
+      <c r="C51" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>37.2</v>
@@ -2296,50 +2711,64 @@
         <f aca="false">LOG(D51*10^-12)</f>
         <v>-10.4294570601181</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K51" s="9" t="s">
-        <v>19</v>
+      <c r="G51" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K51" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="n">
+        <v>94</v>
+      </c>
+      <c r="P51" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q51" s="7" t="n">
+        <f aca="false">LOG10(D51)-13</f>
+        <v>-11.4294570601181</v>
+      </c>
+    </row>
+    <row r="52" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="11" t="n">
         <v>46</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="10" t="n">
+      <c r="C52" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="11" t="n">
         <v>2.93</v>
       </c>
       <c r="E52" s="5" t="n">
         <f aca="false">LOG(D52*10^-12)</f>
         <v>-11.5331323796459</v>
       </c>
-      <c r="G52" s="10" t="s">
-        <v>12</v>
+      <c r="G52" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K52" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M52" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="N52" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q52" s="7" t="n">
+        <f aca="false">LOG10(D52)-13</f>
+        <v>-12.5331323796459</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,7 +2776,7 @@
         <v>47</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>0.504</v>
@@ -2357,28 +2786,35 @@
         <v>-12.2975694635545</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="N53" s="6"/>
-    </row>
-    <row r="54" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="n">
+      <c r="P53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q53" s="7" t="n">
+        <f aca="false">LOG10(D53)-13</f>
+        <v>-13.2975694635545</v>
+      </c>
+    </row>
+    <row r="54" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>46</v>
+      <c r="C54" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>23.8</v>
@@ -2387,64 +2823,78 @@
         <f aca="false">LOG(D54*10^-12)</f>
         <v>-10.6234230429435</v>
       </c>
-      <c r="G54" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L54" s="9" t="s">
-        <v>95</v>
+      <c r="G54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L54" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="N54" s="6"/>
-    </row>
-    <row r="55" s="10" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="n">
+      <c r="P54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q54" s="7" t="n">
+        <f aca="false">LOG10(D54)-13</f>
+        <v>-11.6234230429435</v>
+      </c>
+    </row>
+    <row r="55" s="11" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="11" t="n">
         <v>49</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D55" s="10" t="n">
+      <c r="C55" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="11" t="n">
         <v>0.649</v>
       </c>
       <c r="E55" s="5" t="n">
         <f aca="false">LOG(D55*10^-12)</f>
         <v>-12.1877553031996</v>
       </c>
-      <c r="G55" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K55" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L55" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M55" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="N55" s="11" t="s">
-        <v>98</v>
+      <c r="G55" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M55" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="N55" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="P55" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q55" s="7" t="n">
+        <f aca="false">LOG10(D55)-13</f>
+        <v>-13.1877553031996</v>
       </c>
     </row>
     <row r="56" s="7" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="12" t="n">
+      <c r="A56" s="13" t="n">
         <v>50</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D56" s="8" t="n">
         <v>2.95</v>
       </c>
       <c r="E56" s="5" t="n">
@@ -2452,30 +2902,37 @@
         <v>-11.5301779840218</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M56" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="N56" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="n">
+        <v>78</v>
+      </c>
+      <c r="M56" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N56" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="P56" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q56" s="7" t="n">
+        <f aca="false">LOG10(D56)-13</f>
+        <v>-12.5301779840218</v>
+      </c>
+    </row>
+    <row r="57" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="10" t="n">
         <v>51</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>31</v>
+      <c r="C57" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>16.8</v>
@@ -2484,27 +2941,34 @@
         <f aca="false">LOG(D57*10^-12)</f>
         <v>-10.7746907182741</v>
       </c>
-      <c r="G57" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K57" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L57" s="9" t="s">
-        <v>101</v>
+      <c r="G57" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
-    </row>
-    <row r="58" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="n">
+      <c r="P57" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q57" s="7" t="n">
+        <f aca="false">LOG10(D57)-13</f>
+        <v>-11.7746907182741</v>
+      </c>
+    </row>
+    <row r="58" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10" t="n">
         <v>51.1</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>31</v>
+      <c r="C58" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>17.3</v>
@@ -2513,24 +2977,31 @@
         <f aca="false">LOG(D58*10^-12)</f>
         <v>-10.7619538968712</v>
       </c>
-      <c r="G58" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K58" s="9" t="s">
-        <v>19</v>
+      <c r="G58" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K58" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="M58" s="6"/>
       <c r="N58" s="6"/>
-    </row>
-    <row r="59" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="n">
+      <c r="P58" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q58" s="7" t="n">
+        <f aca="false">LOG10(D58)-13</f>
+        <v>-11.7619538968712</v>
+      </c>
+    </row>
+    <row r="59" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="n">
         <v>51.2</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>31</v>
+      <c r="C59" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>24</v>
@@ -2539,24 +3010,31 @@
         <f aca="false">LOG(D59*10^-12)</f>
         <v>-10.6197887582884</v>
       </c>
-      <c r="G59" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K59" s="9" t="s">
-        <v>19</v>
+      <c r="G59" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K59" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
+      <c r="P59" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q59" s="7" t="n">
+        <f aca="false">LOG10(D59)-13</f>
+        <v>-11.6197887582884</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="n">
+      <c r="A60" s="10" t="n">
         <v>52</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>9.76</v>
@@ -2566,61 +3044,75 @@
         <v>-11.0105501823333</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q60" s="7" t="n">
+        <f aca="false">LOG10(D60)-13</f>
+        <v>-12.0105501823333</v>
+      </c>
+    </row>
+    <row r="61" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11" t="n">
         <v>53</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="10" t="n">
+      <c r="C61" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="11" t="n">
         <v>2.43</v>
       </c>
       <c r="E61" s="5" t="n">
         <f aca="false">LOG(D61*10^-12)</f>
         <v>-11.6143937264017</v>
       </c>
-      <c r="G61" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H61" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K61" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L61" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M61" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="N61" s="11"/>
+      <c r="G61" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K61" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M61" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="N61" s="12"/>
+      <c r="P61" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q61" s="7" t="n">
+        <f aca="false">LOG10(D61)-13</f>
+        <v>-12.6143937264017</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>54</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>28.4</v>
@@ -2630,22 +3122,29 @@
         <v>-10.546681659953</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q62" s="7" t="n">
+        <f aca="false">LOG10(D62)-13</f>
+        <v>-11.546681659953</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,7 +3152,7 @@
         <v>55</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>3.09</v>
@@ -2663,22 +3162,29 @@
         <v>-11.5100415205752</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M63" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q63" s="7" t="n">
+        <f aca="false">LOG10(D63)-13</f>
+        <v>-12.5100415205752</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,7 +3192,7 @@
         <v>56</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>1.42</v>
@@ -2696,28 +3202,35 @@
         <v>-11.8477116556169</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N64" s="6"/>
+      <c r="P64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q64" s="7" t="n">
+        <f aca="false">LOG10(D64)-13</f>
+        <v>-12.8477116556169</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <v>56.1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>1.43</v>
@@ -2727,26 +3240,33 @@
         <v>-11.8446639625349</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M65" s="6"/>
       <c r="N65" s="6"/>
+      <c r="P65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q65" s="7" t="n">
+        <f aca="false">LOG10(D65)-13</f>
+        <v>-12.8446639625349</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <v>57</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>55.4</v>
@@ -2756,83 +3276,104 @@
         <v>-10.2564902352716</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="M66" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" s="10" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q66" s="7" t="n">
+        <f aca="false">LOG10(D66)-13</f>
+        <v>-11.2564902352716</v>
+      </c>
+    </row>
+    <row r="67" s="11" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="11" t="n">
         <v>58</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" s="10" t="n">
+      <c r="C67" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" s="11" t="n">
         <v>4.13</v>
       </c>
       <c r="E67" s="5" t="n">
         <f aca="false">LOG(D67*10^-12)</f>
         <v>-11.3840499483436</v>
       </c>
-      <c r="G67" s="10" t="s">
-        <v>12</v>
+      <c r="G67" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K67" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L67" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M67" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="N67" s="11"/>
-    </row>
-    <row r="68" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="K67" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L67" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M67" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="N67" s="12"/>
+      <c r="P67" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q67" s="7" t="n">
+        <f aca="false">LOG10(D67)-13</f>
+        <v>-12.3840499483436</v>
+      </c>
+    </row>
+    <row r="68" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="11" t="n">
         <v>59</v>
       </c>
-      <c r="C68" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="10" t="n">
+      <c r="C68" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="11" t="n">
         <v>3.44</v>
       </c>
       <c r="E68" s="5" t="n">
         <f aca="false">LOG(D68*10^-12)</f>
         <v>-11.4634415574285</v>
       </c>
-      <c r="G68" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K68" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M68" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="N68" s="11" t="s">
-        <v>18</v>
+      <c r="G68" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K68" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M68" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="N68" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P68" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q68" s="7" t="n">
+        <f aca="false">LOG10(D68)-13</f>
+        <v>-12.4634415574285</v>
       </c>
     </row>
     <row r="69" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,9 +3381,9 @@
         <v>60</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D69" s="8" t="n">
         <v>2.76</v>
       </c>
       <c r="E69" s="5" t="n">
@@ -2850,30 +3391,37 @@
         <v>-11.5590909179348</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="M69" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="N69" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="M69" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="N69" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="P69" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q69" s="7" t="n">
+        <f aca="false">LOG10(D69)-13</f>
+        <v>-12.5590909179348</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="9" t="n">
+      <c r="A70" s="10" t="n">
         <v>61</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>3.08</v>
@@ -2883,22 +3431,29 @@
         <v>-11.5114492834996</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
+      </c>
+      <c r="P70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q70" s="7" t="n">
+        <f aca="false">LOG10(D70)-13</f>
+        <v>-12.5114492834996</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,7 +3461,7 @@
         <v>62</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>2.45</v>
@@ -2916,61 +3471,75 @@
         <v>-11.6108339156355</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="72" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10" t="n">
+        <v>123</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q71" s="7" t="n">
+        <f aca="false">LOG10(D71)-13</f>
+        <v>-12.6108339156355</v>
+      </c>
+    </row>
+    <row r="72" s="11" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="11" t="n">
         <v>63</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" s="10" t="n">
+      <c r="C72" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="11" t="n">
         <v>1.32</v>
       </c>
       <c r="E72" s="5" t="n">
         <f aca="false">LOG(D72*10^-12)</f>
         <v>-11.8794260687942</v>
       </c>
-      <c r="G72" s="10" t="s">
-        <v>12</v>
+      <c r="G72" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K72" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L72" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M72" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="N72" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="K72" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L72" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M72" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N72" s="12"/>
+      <c r="P72" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q72" s="7" t="n">
+        <f aca="false">LOG10(D72)-13</f>
+        <v>-12.8794260687941</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
         <v>64</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>3.76</v>
@@ -2980,28 +3549,35 @@
         <v>-11.4248121550723</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M73" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N73" s="6"/>
+      <c r="P73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q73" s="7" t="n">
+        <f aca="false">LOG10(D73)-13</f>
+        <v>-12.4248121550723</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
         <v>65</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>2</v>
@@ -3011,28 +3587,35 @@
         <v>-11.698970004336</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M74" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="N74" s="6"/>
+      <c r="P74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q74" s="7" t="n">
+        <f aca="false">LOG10(D74)-13</f>
+        <v>-12.698970004336</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
         <v>66</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>4.17</v>
@@ -3042,28 +3625,35 @@
         <v>-11.3798639450262</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M75" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="N75" s="6"/>
+      <c r="P75" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q75" s="7" t="n">
+        <f aca="false">LOG10(D75)-13</f>
+        <v>-12.3798639450262</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
         <v>67</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>8.22</v>
@@ -3073,22 +3663,29 @@
         <v>-11.08512818246</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M76" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q76" s="7" t="n">
+        <f aca="false">LOG10(D76)-13</f>
+        <v>-12.08512818246</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,7 +3693,7 @@
         <v>68</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>2.07</v>
@@ -3106,22 +3703,29 @@
         <v>-11.6840296545431</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M77" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q77" s="7" t="n">
+        <f aca="false">LOG10(D77)-13</f>
+        <v>-12.6840296545431</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3129,7 +3733,7 @@
         <v>69</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>2.55</v>
@@ -3139,22 +3743,29 @@
         <v>-11.593459819566</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M78" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="P78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q78" s="7" t="n">
+        <f aca="false">LOG10(D78)-13</f>
+        <v>-12.593459819566</v>
       </c>
     </row>
     <row r="79" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3162,7 +3773,7 @@
         <v>70</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D79" s="7" t="n">
         <v>4.88</v>
@@ -3172,10 +3783,17 @@
         <v>-11.3115801779973</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="P79" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q79" s="7" t="n">
+        <f aca="false">LOG10(D79)-13</f>
+        <v>-12.3115801779973</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,7 +3803,7 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="17" t="n">
+      <c r="D82" s="18" t="n">
         <f aca="false">(10^12)*10^AVERAGE(E2:E79)</f>
         <v>2.23479814551686</v>
       </c>
@@ -3203,7 +3821,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N79"/>
+  <autoFilter ref="A1:M79"/>
   <conditionalFormatting sqref="D20:D78 D2:D18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -4186,7 +4804,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="193.83"/>
   </cols>
@@ -4199,7 +4817,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4207,7 +4825,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4215,7 +4833,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4223,10 +4841,10 @@
         <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,7 +4852,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4242,7 +4860,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4250,7 +4868,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,7 +4876,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>